<commit_message>
General changes in infra and xls readaing - adding function to read addresses - modify the function that read the data from sheet - add function to read products
Change-Id: I2cbb4ed533504e4da926507a1c1f35cc81f17c1c
Signed-off-by: Ibatta <Ibatta@Ibatta-Lap>
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="0" windowWidth="16980" windowHeight="6390" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="16980" windowHeight="6390" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Registration" sheetId="5" r:id="rId2"/>
     <sheet name="CheckOut" sheetId="7" r:id="rId3"/>
-    <sheet name="Products" sheetId="8" r:id="rId4"/>
+    <sheet name="products" sheetId="8" r:id="rId4"/>
     <sheet name="cards" sheetId="9" r:id="rId5"/>
-    <sheet name="Addresses" sheetId="10" r:id="rId6"/>
+    <sheet name="addresses" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -323,9 +323,6 @@
     <t>firstName</t>
   </si>
   <si>
-    <t>adddress</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -393,6 +390,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>adddressLine</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1088,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="9" customFormat="1" ht="90">
+    <row r="2" spans="1:18" s="9" customFormat="1" ht="165">
       <c r="A2" s="13" t="s">
         <v>40</v>
       </c>
@@ -1204,7 +1204,7 @@
       </c>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" s="9" customFormat="1" ht="75">
+    <row r="5" spans="1:18" s="9" customFormat="1" ht="30">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -1341,10 +1341,10 @@
         <v>60</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>106</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>107</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>61</v>
@@ -1353,19 +1353,19 @@
         <v>65</v>
       </c>
       <c r="J1" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="K1" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>112</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>113</v>
       </c>
       <c r="O1" s="21"/>
       <c r="P1" s="21"/>
@@ -1392,14 +1392,14 @@
         <v>68</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="17"/>
@@ -1431,14 +1431,14 @@
         <v>69</v>
       </c>
       <c r="F3" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>104</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>105</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J3" s="16"/>
       <c r="K3" s="17"/>
@@ -1463,16 +1463,16 @@
         <v>70</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>73</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J4" s="16"/>
       <c r="K4" s="17"/>
@@ -1491,20 +1491,20 @@
         <v>56</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>71</v>
       </c>
       <c r="F5" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>104</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>105</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J5" s="16"/>
       <c r="K5" s="17"/>
@@ -1523,20 +1523,20 @@
         <v>56</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>72</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="17"/>
@@ -1557,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1598,7 +1598,7 @@
         <v>52</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45">
@@ -1615,7 +1615,7 @@
         <v>57</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1627,7 +1627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -1670,13 +1670,13 @@
         <v>85</v>
       </c>
       <c r="D2" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="F2" s="29" t="s">
         <v>116</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1690,13 +1690,13 @@
         <v>85</v>
       </c>
       <c r="D3" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="29" t="s">
-        <v>116</v>
-      </c>
       <c r="F3" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1710,13 +1710,13 @@
         <v>85</v>
       </c>
       <c r="D4" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>116</v>
-      </c>
       <c r="F4" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1730,13 +1730,13 @@
         <v>85</v>
       </c>
       <c r="D5" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>116</v>
-      </c>
       <c r="F5" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1750,13 +1750,13 @@
         <v>85</v>
       </c>
       <c r="D6" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="29" t="s">
-        <v>116</v>
-      </c>
       <c r="F6" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1770,7 +1770,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1786,7 +1786,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>98</v>
@@ -1795,21 +1795,21 @@
         <v>97</v>
       </c>
       <c r="D1" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>101</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>16</v>
@@ -1832,7 +1832,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Added get all payments cards function
Change-Id: I502687478831f0b7bb6a017fb78e5dcd71aa994a
Signed-off-by: Ibatta <Ibatta@Ibatta-Lap>
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="0" windowWidth="16980" windowHeight="6390" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="16980" windowHeight="6390" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,13 @@
     <sheet name="addresses" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:M7"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="125">
   <si>
     <t>TCID</t>
   </si>
@@ -393,6 +394,12 @@
   </si>
   <si>
     <t>adddressLine</t>
+  </si>
+  <si>
+    <t>run_test</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -531,7 +538,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -615,6 +622,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1293,261 +1303,277 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="12" customFormat="1">
+    <row r="1" spans="1:22" s="12" customFormat="1">
       <c r="A1" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="L1" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="21"/>
       <c r="P1" s="21"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
       <c r="S1" s="21"/>
       <c r="T1" s="21"/>
       <c r="U1" s="21"/>
-    </row>
-    <row r="2" spans="1:21" s="9" customFormat="1" ht="60">
-      <c r="A2" s="13" t="s">
+      <c r="V1" s="21"/>
+    </row>
+    <row r="2" spans="1:22" s="9" customFormat="1" ht="60">
+      <c r="A2" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="13" t="s">
+      <c r="H2" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="17"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="17"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="18"/>
-      <c r="O2"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="18"/>
       <c r="P2"/>
       <c r="Q2"/>
       <c r="R2"/>
       <c r="S2"/>
       <c r="T2"/>
       <c r="U2"/>
-    </row>
-    <row r="3" spans="1:21" ht="60">
-      <c r="A3" s="13" t="s">
+      <c r="V2"/>
+    </row>
+    <row r="3" spans="1:22" ht="60">
+      <c r="A3" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="F3" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="17"/>
+      <c r="K3" s="16"/>
       <c r="L3" s="17"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="18"/>
-    </row>
-    <row r="4" spans="1:21" ht="60">
-      <c r="A4" s="13" t="s">
+      <c r="M3" s="17"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="1:22" ht="60">
+      <c r="A4" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="D4" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="F4" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>103</v>
       </c>
       <c r="H4" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="J4" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
+      <c r="K4" s="16"/>
       <c r="L4" s="17"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="18"/>
-    </row>
-    <row r="5" spans="1:21" ht="60">
-      <c r="A5" s="13" t="s">
+      <c r="M4" s="17"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:22" ht="60">
+      <c r="A5" s="32"/>
+      <c r="B5" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="D5" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="G5" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="H5" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="16"/>
+      <c r="J5" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="17"/>
+      <c r="K5" s="16"/>
       <c r="L5" s="17"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="18"/>
-    </row>
-    <row r="6" spans="1:21" ht="60">
-      <c r="A6" s="13" t="s">
+      <c r="M5" s="17"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="18"/>
+    </row>
+    <row r="6" spans="1:22" ht="60">
+      <c r="A6" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="D6" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="F6" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="13" t="s">
+      <c r="H6" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17"/>
+      <c r="K6" s="16"/>
       <c r="L6" s="17"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="18"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3:I6" r:id="rId2" display="ibatta@dbi.com"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3:J6" r:id="rId2" display="ibatta@dbi.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1557,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1627,7 +1653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -1769,7 +1795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding ignore test status
Change-Id: I4954bb6bd220716dca793ed94c3cc26f898b6080
Signed-off-by: Ibatta <Ibatta@Ibatta-Lap>
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="16980" windowHeight="6390" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="16980" windowHeight="6390" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,6 @@
     <sheet name="addresses" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M7"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -200,9 +199,6 @@
     <t>qty</t>
   </si>
   <si>
-    <t>shipping</t>
-  </si>
-  <si>
     <t xml:space="preserve">payment </t>
   </si>
   <si>
@@ -396,10 +392,13 @@
     <t>adddressLine</t>
   </si>
   <si>
-    <t>run_test</t>
-  </si>
-  <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>runTest</t>
+  </si>
+  <si>
+    <t>shippingMethod</t>
   </si>
 </sst>
 </file>
@@ -1303,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1325,139 +1324,118 @@
     <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="12" customFormat="1">
+    <row r="1" spans="1:15" s="12" customFormat="1">
       <c r="A1" s="20" t="s">
         <v>123</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>53</v>
       </c>
       <c r="E1" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="60">
+      <c r="A2" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-    </row>
-    <row r="2" spans="1:22" s="9" customFormat="1" ht="60">
-      <c r="A2" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="E2" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>64</v>
-      </c>
       <c r="F2" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I2" s="16"/>
       <c r="J2" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
       <c r="N2" s="16"/>
       <c r="O2" s="18"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
-    </row>
-    <row r="3" spans="1:22" ht="60">
+    </row>
+    <row r="3" spans="1:15" ht="60">
       <c r="A3" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>45</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>103</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>104</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K3" s="16"/>
       <c r="L3" s="17"/>
@@ -1465,36 +1443,36 @@
       <c r="N3" s="16"/>
       <c r="O3" s="18"/>
     </row>
-    <row r="4" spans="1:22" ht="60">
+    <row r="4" spans="1:15" ht="60">
       <c r="A4" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>56</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K4" s="16"/>
       <c r="L4" s="17"/>
@@ -1502,32 +1480,32 @@
       <c r="N4" s="16"/>
       <c r="O4" s="18"/>
     </row>
-    <row r="5" spans="1:22" ht="60">
+    <row r="5" spans="1:15" ht="60">
       <c r="A5" s="32"/>
       <c r="B5" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>56</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G5" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>103</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>104</v>
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K5" s="16"/>
       <c r="L5" s="17"/>
@@ -1535,34 +1513,34 @@
       <c r="N5" s="16"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:22" ht="60">
+    <row r="6" spans="1:15" ht="60">
       <c r="A6" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>56</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="17"/>
@@ -1624,7 +1602,7 @@
         <v>52</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45">
@@ -1641,7 +1619,7 @@
         <v>57</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1667,122 +1645,122 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="F2" s="29" t="s">
         <v>115</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="29" t="s">
-        <v>115</v>
-      </c>
       <c r="F3" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>115</v>
-      </c>
       <c r="F4" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>115</v>
-      </c>
       <c r="F5" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="29" t="s">
-        <v>115</v>
-      </c>
       <c r="F6" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1812,30 +1790,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>100</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>16</v>
@@ -1844,21 +1822,21 @@
         <v>17</v>
       </c>
       <c r="D2" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="F2" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="G2" s="30" t="s">
         <v>93</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>16</v>
@@ -1867,16 +1845,16 @@
         <v>17</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaking SelTestCase after annotation to handle the addTestCase feature
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="16980" windowHeight="6390" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="16980" windowHeight="6390" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,6 @@
     <sheet name="addresses" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M7"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -1016,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1305,7 +1304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test pull changes from fork
Change-Id: Ia75fcdeb88e81f69b334019ae898a986051ef3c4
Signed-off-by: Ibrahem Batta <18301319+ibatta@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="16980" windowHeight="6390" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="16980" windowHeight="6390" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="addresses" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -202,203 +203,203 @@
     <t xml:space="preserve">payment </t>
   </si>
   <si>
-    <t>giftcard</t>
+    <t>P1
+P2</t>
+  </si>
+  <si>
+    <t>PREMIUM DELIVERY</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>proprties</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>visa</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>amex</t>
+  </si>
+  <si>
+    <t>maistro</t>
+  </si>
+  <si>
+    <t>diner</t>
+  </si>
+  <si>
+    <t>test_gc</t>
+  </si>
+  <si>
+    <t>logged in user with saved visa payment and shipping address</t>
+  </si>
+  <si>
+    <t>logged in user with saved master payment and shipping address</t>
+  </si>
+  <si>
+    <t>logged in user with saved amex payment and shipping address</t>
+  </si>
+  <si>
+    <t>logged in user with saved maistro payment and shipping address</t>
+  </si>
+  <si>
+    <t>logged in user with saved diner payment and shipping address</t>
+  </si>
+  <si>
+    <t>card</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>expire year</t>
+  </si>
+  <si>
+    <t>expire month</t>
+  </si>
+  <si>
+    <t>CVCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name </t>
+  </si>
+  <si>
+    <t>Accept Tester</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>378282246310005</t>
+  </si>
+  <si>
+    <t>38520000023237</t>
+  </si>
+  <si>
+    <t>5555555555554444</t>
+  </si>
+  <si>
+    <t>6759649826438453</t>
+  </si>
+  <si>
+    <t>49 Featherstone Street</t>
+  </si>
+  <si>
+    <t>LONDON</t>
+  </si>
+  <si>
+    <t>EC1Y 8SY</t>
+  </si>
+  <si>
+    <t>UNITED KINGDOM</t>
+  </si>
+  <si>
+    <t>HP19 3EQ</t>
+  </si>
+  <si>
+    <t>Ardenham Court</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>postal</t>
+  </si>
+  <si>
+    <t>countery</t>
+  </si>
+  <si>
+    <t>addressCode</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>shippingAddress</t>
+  </si>
+  <si>
+    <t>billingAddress</t>
+  </si>
+  <si>
+    <t>STANDARD DELIVERY</t>
+  </si>
+  <si>
+    <t>orderTotal</t>
+  </si>
+  <si>
+    <t>orderId</t>
+  </si>
+  <si>
+    <t>orderSubtotal</t>
+  </si>
+  <si>
+    <t>orderTax</t>
+  </si>
+  <si>
+    <t>orderShipping</t>
+  </si>
+  <si>
+    <t>ibatta@dbi.com</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>334</t>
+  </si>
+  <si>
+    <t>335</t>
+  </si>
+  <si>
+    <t>336</t>
+  </si>
+  <si>
+    <t>337</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>adddressLine</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>runTest</t>
+  </si>
+  <si>
+    <t>shippingMethod</t>
+  </si>
+  <si>
+    <t>coupon</t>
   </si>
   <si>
     <t>loggedin
 old-user
 saved-shipping
-save-payment</t>
-  </si>
-  <si>
-    <t>P1
-P2</t>
-  </si>
-  <si>
-    <t>PREMIUM DELIVERY</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>proprties</t>
-  </si>
-  <si>
-    <t>desc</t>
-  </si>
-  <si>
-    <t>visa</t>
-  </si>
-  <si>
-    <t>master</t>
-  </si>
-  <si>
-    <t>amex</t>
-  </si>
-  <si>
-    <t>maistro</t>
-  </si>
-  <si>
-    <t>diner</t>
-  </si>
-  <si>
-    <t>test_gc</t>
-  </si>
-  <si>
-    <t>logged in user with saved visa payment and shipping address</t>
-  </si>
-  <si>
-    <t>logged in user with saved master payment and shipping address</t>
-  </si>
-  <si>
-    <t>logged in user with saved amex payment and shipping address</t>
-  </si>
-  <si>
-    <t>logged in user with saved maistro payment and shipping address</t>
-  </si>
-  <si>
-    <t>logged in user with saved diner payment and shipping address</t>
-  </si>
-  <si>
-    <t>card</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>expire year</t>
-  </si>
-  <si>
-    <t>expire month</t>
-  </si>
-  <si>
-    <t>CVCC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name </t>
-  </si>
-  <si>
-    <t>Accept Tester</t>
-  </si>
-  <si>
-    <t>4111111111111111</t>
-  </si>
-  <si>
-    <t>378282246310005</t>
-  </si>
-  <si>
-    <t>38520000023237</t>
-  </si>
-  <si>
-    <t>5555555555554444</t>
-  </si>
-  <si>
-    <t>6759649826438453</t>
-  </si>
-  <si>
-    <t>49 Featherstone Street</t>
-  </si>
-  <si>
-    <t>LONDON</t>
-  </si>
-  <si>
-    <t>EC1Y 8SY</t>
-  </si>
-  <si>
-    <t>UNITED KINGDOM</t>
-  </si>
-  <si>
-    <t>HP19 3EQ</t>
-  </si>
-  <si>
-    <t>Ardenham Court</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>postal</t>
-  </si>
-  <si>
-    <t>countery</t>
-  </si>
-  <si>
-    <t>addressCode</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>shippingAddress</t>
-  </si>
-  <si>
-    <t>billingAddress</t>
-  </si>
-  <si>
-    <t>STANDARD DELIVERY</t>
-  </si>
-  <si>
-    <t>orderTotal</t>
-  </si>
-  <si>
-    <t>orderId</t>
-  </si>
-  <si>
-    <t>orderSubtotal</t>
-  </si>
-  <si>
-    <t>orderTax</t>
-  </si>
-  <si>
-    <t>orderShipping</t>
-  </si>
-  <si>
-    <t>ibatta@dbi.com</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>333</t>
-  </si>
-  <si>
-    <t>334</t>
-  </si>
-  <si>
-    <t>335</t>
-  </si>
-  <si>
-    <t>336</t>
-  </si>
-  <si>
-    <t>337</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>adddressLine</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>runTest</t>
-  </si>
-  <si>
-    <t>shippingMethod</t>
+saved-payment</t>
   </si>
 </sst>
 </file>
@@ -1304,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1328,79 +1329,79 @@
   <sheetData>
     <row r="1" spans="1:15" s="12" customFormat="1">
       <c r="A1" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>53</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>59</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H1" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="21" t="s">
+      <c r="M1" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="M1" s="22" t="s">
+      <c r="O1" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="9" customFormat="1" ht="60">
       <c r="A2" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>63</v>
-      </c>
       <c r="F2" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I2" s="16"/>
       <c r="J2" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
@@ -1410,32 +1411,32 @@
     </row>
     <row r="3" spans="1:15" ht="60">
       <c r="A3" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>45</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K3" s="16"/>
       <c r="L3" s="17"/>
@@ -1445,34 +1446,34 @@
     </row>
     <row r="4" spans="1:15" ht="60">
       <c r="A4" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>56</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K4" s="16"/>
       <c r="L4" s="17"/>
@@ -1483,29 +1484,29 @@
     <row r="5" spans="1:15" ht="60">
       <c r="A5" s="32"/>
       <c r="B5" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>56</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K5" s="16"/>
       <c r="L5" s="17"/>
@@ -1515,32 +1516,32 @@
     </row>
     <row r="6" spans="1:15" ht="60">
       <c r="A6" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>56</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="17"/>
@@ -1602,7 +1603,7 @@
         <v>52</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45">
@@ -1619,7 +1620,7 @@
         <v>57</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1645,122 +1646,122 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>80</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>113</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E3" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="29" t="s">
         <v>114</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1790,30 +1791,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>98</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>16</v>
@@ -1822,21 +1823,21 @@
         <v>17</v>
       </c>
       <c r="D2" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="G2" s="30" t="s">
         <v>91</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>16</v>
@@ -1845,16 +1846,16 @@
         <v>17</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E3" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>91</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
demo Joe: added correct exception
Change-Id: Ic07bc93aff533a05c0974751182e665f5c5b293d
Signed-off-by: Ibrahem Batta <18301319+ibatta@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -15,13 +15,13 @@
     <sheet name="addresses" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:N6"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="134">
   <si>
     <t>TCID</t>
   </si>
@@ -173,40 +173,21 @@
     <t>name</t>
   </si>
   <si>
-    <t>/yacceleratorstorefront/en/Categories/Bags%2BBoardbags/Bags/Seizure-Satchel/p/300613490</t>
-  </si>
-  <si>
     <t>black</t>
   </si>
   <si>
-    <t>Size Uni, £34.79  21</t>
-  </si>
-  <si>
     <t xml:space="preserve">products </t>
   </si>
   <si>
-    <t>/yacceleratorstorefront/en/Categories/Bags%2BBoardbags/Bags/Seizure-Bag/p/300441924</t>
-  </si>
-  <si>
-    <t>clay court</t>
-  </si>
-  <si>
     <t>P2</t>
   </si>
   <si>
-    <t>Size Uni, £24.26  4</t>
-  </si>
-  <si>
     <t>qty</t>
   </si>
   <si>
     <t xml:space="preserve">payment </t>
   </si>
   <si>
-    <t>P1
-P2</t>
-  </si>
-  <si>
     <t>PREMIUM DELIVERY</t>
   </si>
   <si>
@@ -376,9 +357,6 @@
   </si>
   <si>
     <t>337</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>adddressLine</t>
@@ -399,6 +377,59 @@
     <t>loggedin
 old-user
 saved-shipping
+saved-payment</t>
+  </si>
+  <si>
+    <t>UNITED STATES</t>
+  </si>
+  <si>
+    <t>NEW YORK</t>
+  </si>
+  <si>
+    <t>254 park Ave</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>https://hybrisdemo.conexus.co.uk:9002/yacceleratorstorefront/en/Categories/Bags%2BBoardbags/Bags/Seizure-Satchel/p/300613491</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Size Uni, £34.79  21</t>
+  </si>
+  <si>
+    <t>https://hybrisdemo.conexus.co.uk:9002/yacceleratorstorefront/en/Brands/Toko/Snowboard-Ski-Tool-Toko-Waxremover-HC3-500ml/p/45572</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>P1
+P2
+P3</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>https://hybrisdemo.conexus.co.uk:9002/yacceleratorstorefront/en/Brands/Playboard/T-Shirt-Men-Playboard-Raster-SS/p/300046037</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Size XL, £26.68  99</t>
+  </si>
+  <si>
+    <t>loggedin
+old-user
+new-shipping
 saved-payment</t>
   </si>
 </sst>
@@ -1303,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1329,79 +1360,79 @@
   <sheetData>
     <row r="1" spans="1:15" s="12" customFormat="1">
       <c r="A1" s="20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G1" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="N1" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>103</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="9" customFormat="1" ht="60">
       <c r="A2" s="32" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I2" s="16"/>
       <c r="J2" s="13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
@@ -1409,34 +1440,34 @@
       <c r="N2" s="16"/>
       <c r="O2" s="18"/>
     </row>
-    <row r="3" spans="1:15" ht="60">
+    <row r="3" spans="1:15" s="9" customFormat="1" ht="60">
       <c r="A3" s="32" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>45</v>
+        <v>128</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="K3" s="16"/>
       <c r="L3" s="17"/>
@@ -1444,36 +1475,32 @@
       <c r="N3" s="16"/>
       <c r="O3" s="18"/>
     </row>
-    <row r="4" spans="1:15" ht="60">
-      <c r="A4" s="32" t="s">
-        <v>120</v>
-      </c>
+    <row r="4" spans="1:15" customFormat="1" ht="60">
+      <c r="A4" s="32"/>
       <c r="B4" s="13" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>70</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="I4" s="16"/>
       <c r="J4" s="13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="K4" s="16"/>
       <c r="L4" s="17"/>
@@ -1481,32 +1508,34 @@
       <c r="N4" s="16"/>
       <c r="O4" s="18"/>
     </row>
-    <row r="5" spans="1:15" ht="60">
+    <row r="5" spans="1:15" customFormat="1" ht="60">
       <c r="A5" s="32"/>
       <c r="B5" s="13" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E5" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>104</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="13" t="s">
-        <v>110</v>
       </c>
       <c r="K5" s="16"/>
       <c r="L5" s="17"/>
@@ -1514,34 +1543,32 @@
       <c r="N5" s="16"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" ht="60">
-      <c r="A6" s="32" t="s">
-        <v>120</v>
-      </c>
+    <row r="6" spans="1:15" customFormat="1" ht="60">
+      <c r="A6" s="32"/>
       <c r="B6" s="13" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="17"/>
@@ -1549,26 +1576,96 @@
       <c r="N6" s="16"/>
       <c r="O6" s="18"/>
     </row>
+    <row r="7" spans="1:15" customFormat="1" ht="60">
+      <c r="A7" s="32"/>
+      <c r="B7" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="18"/>
+    </row>
+    <row r="8" spans="1:15" customFormat="1" ht="60">
+      <c r="A8" s="32"/>
+      <c r="B8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="16"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="18"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3:J6" r:id="rId2" display="ibatta@dbi.com"/>
+    <hyperlink ref="J4:J7" r:id="rId2" display="ibatta@dbi.com"/>
+    <hyperlink ref="J8" r:id="rId3"/>
+    <hyperlink ref="J3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1586,41 +1683,54 @@
         <v>47</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60">
       <c r="A2" s="24" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>51</v>
-      </c>
       <c r="D2" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60">
+      <c r="A3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45">
-      <c r="A3" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="B3" s="27" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>118</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60">
+      <c r="A4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="31" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1633,7 +1743,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1646,122 +1756,122 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="23" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="28" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="28" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="28" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="28" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="28" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D6" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="29" t="s">
         <v>111</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1772,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1791,30 +1901,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="23" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>16</v>
@@ -1823,21 +1933,21 @@
         <v>17</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="28" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>16</v>
@@ -1846,16 +1956,39 @@
         <v>17</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>91</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="28">
+        <v>10167</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
General fixes/ progress in checkout flows
- cart: added keys class to habdle the keys from hash map input format
- PDP: added keys 
- basecheckout: added keys/enhancements -progress in checkouts tests 
- selectorUtils: added enhancements 
- checkout: added enhancements, key class 
- common: added phone and title
- datasheet: added phone and title to address 

Change-Id: I176b5a0a48a2a84040f84216e313f97c2bf185e2
Signed-off-by: Ibrahem Batta <18301319+ibatta@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="1890" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,12 @@
     <sheet name="addresses" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N6"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="139">
   <si>
     <t>TCID</t>
   </si>
@@ -239,16 +238,7 @@
     <t>number</t>
   </si>
   <si>
-    <t>expire year</t>
-  </si>
-  <si>
-    <t>expire month</t>
-  </si>
-  <si>
     <t>CVCC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name </t>
   </si>
   <si>
     <t>Accept Tester</t>
@@ -427,13 +417,37 @@
     <t>Size XL, £26.68  99</t>
   </si>
   <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>MR.</t>
+  </si>
+  <si>
+    <t>14725836952</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>expireYear</t>
+  </si>
+  <si>
+    <t>expireMonth</t>
+  </si>
+  <si>
     <t>loggedin
 old-user
 new-shipping
 saved-payment</t>
   </si>
   <si>
-    <t>invalid</t>
+    <t>loggedin
+old-user
+saved-shipping
+new-payment</t>
   </si>
 </sst>
 </file>
@@ -500,7 +514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -564,6 +578,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -572,7 +597,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -659,6 +684,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1339,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1363,7 +1391,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="12" customFormat="1">
       <c r="A1" s="20" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>58</v>
@@ -1375,51 +1403,51 @@
         <v>51</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>54</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>56</v>
       </c>
       <c r="K1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="21" t="s">
         <v>100</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="9" customFormat="1" ht="60">
       <c r="A2" s="32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>55</v>
@@ -1428,16 +1456,16 @@
         <v>59</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
@@ -1446,17 +1474,15 @@
       <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="60">
-      <c r="A3" s="32" t="s">
-        <v>113</v>
-      </c>
+      <c r="A3" s="32"/>
       <c r="B3" s="13" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>55</v>
@@ -1465,14 +1491,14 @@
         <v>59</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K3" s="16"/>
       <c r="L3" s="17"/>
@@ -1480,13 +1506,13 @@
       <c r="N3" s="16"/>
       <c r="O3" s="18"/>
     </row>
-    <row r="4" spans="1:15" customFormat="1" ht="60">
+    <row r="4" spans="1:15" ht="60">
       <c r="A4" s="32"/>
       <c r="B4" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>45</v>
@@ -1498,14 +1524,14 @@
         <v>60</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I4" s="16"/>
       <c r="J4" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K4" s="16"/>
       <c r="L4" s="17"/>
@@ -1513,13 +1539,13 @@
       <c r="N4" s="16"/>
       <c r="O4" s="18"/>
     </row>
-    <row r="5" spans="1:15" customFormat="1" ht="60">
+    <row r="5" spans="1:15" ht="60">
       <c r="A5" s="32"/>
       <c r="B5" s="13" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>52</v>
@@ -1531,16 +1557,16 @@
         <v>61</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>64</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K5" s="16"/>
       <c r="L5" s="17"/>
@@ -1548,32 +1574,32 @@
       <c r="N5" s="16"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" customFormat="1" ht="60">
+    <row r="6" spans="1:15" ht="60">
       <c r="A6" s="32"/>
       <c r="B6" s="13" t="s">
         <v>68</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>52</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>62</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="17"/>
@@ -1581,32 +1607,32 @@
       <c r="N6" s="16"/>
       <c r="O6" s="18"/>
     </row>
-    <row r="7" spans="1:15" customFormat="1" ht="60">
+    <row r="7" spans="1:15" ht="60">
       <c r="A7" s="32"/>
       <c r="B7" s="13" t="s">
         <v>69</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>52</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>63</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I7" s="16"/>
       <c r="J7" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K7" s="16"/>
       <c r="L7" s="17"/>
@@ -1614,32 +1640,32 @@
       <c r="N7" s="16"/>
       <c r="O7" s="18"/>
     </row>
-    <row r="8" spans="1:15" customFormat="1" ht="60">
+    <row r="8" spans="1:15" ht="60">
       <c r="A8" s="32"/>
       <c r="B8" s="13" t="s">
         <v>68</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>52</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I8" s="16"/>
       <c r="J8" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K8" s="16"/>
       <c r="L8" s="17"/>
@@ -1696,16 +1722,16 @@
         <v>45</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>50</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60">
@@ -1713,29 +1739,29 @@
         <v>52</v>
       </c>
       <c r="B3" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="E3" s="31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60">
       <c r="A4" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="31" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1747,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1767,16 +1793,16 @@
         <v>71</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="D1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>72</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1784,19 +1810,19 @@
         <v>59</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1804,19 +1830,19 @@
         <v>60</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D3" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="29" t="s">
         <v>105</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1824,19 +1850,19 @@
         <v>62</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E4" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="29" t="s">
         <v>106</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1844,19 +1870,19 @@
         <v>61</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1864,19 +1890,19 @@
         <v>63</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1887,49 +1913,56 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="23" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" s="23" t="s">
+      <c r="I1" s="33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="28" t="s">
         <v>91</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="28" t="s">
-        <v>94</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>16</v>
@@ -1937,22 +1970,28 @@
       <c r="C2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>16</v>
@@ -1960,22 +1999,28 @@
       <c r="C3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="30" t="s">
-        <v>87</v>
+      <c r="D3" s="28" t="s">
+        <v>132</v>
       </c>
       <c r="E3" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>16</v>
@@ -1984,16 +2029,22 @@
         <v>17</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="F4" s="28">
+        <v>117</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="28">
         <v>10167</v>
       </c>
-      <c r="G4" s="28" t="s">
-        <v>118</v>
+      <c r="H4" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix implicit modifier and use explicit one for pages
Change-Id: Idc837e58b497a74c5fea65d2856fc132733f6869
Signed-off-by: Ibrahem Batta <18301319+ibatta@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="products" sheetId="8" r:id="rId4"/>
     <sheet name="cards" sheetId="9" r:id="rId5"/>
     <sheet name="addresses" sheetId="10" r:id="rId6"/>
+    <sheet name="CheckOut.bak" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="139">
   <si>
     <t>TCID</t>
   </si>
@@ -1365,10 +1366,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1673,15 +1674,49 @@
       <c r="N8" s="16"/>
       <c r="O8" s="18"/>
     </row>
+    <row r="9" spans="1:15" ht="60">
+      <c r="A9" s="32"/>
+      <c r="B9" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K9" s="16"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="18"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J4:J7" r:id="rId2" display="ibatta@dbi.com"/>
-    <hyperlink ref="J8" r:id="rId3"/>
-    <hyperlink ref="J3" r:id="rId4"/>
+    <hyperlink ref="J9" r:id="rId2"/>
+    <hyperlink ref="J3" r:id="rId3"/>
+    <hyperlink ref="J8" r:id="rId4"/>
+    <hyperlink ref="J4:J7" r:id="rId5" display="ibatta@dbi.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1773,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2051,4 +2086,360 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="12" customFormat="1">
+      <c r="A1" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="60">
+      <c r="A2" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K2" s="16"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:15" s="9" customFormat="1" ht="60">
+      <c r="A3" s="32"/>
+      <c r="B3" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" s="16"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="1:15" ht="60">
+      <c r="A4" s="32"/>
+      <c r="B4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K4" s="16"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:15" ht="60">
+      <c r="A5" s="32"/>
+      <c r="B5" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="18"/>
+    </row>
+    <row r="6" spans="1:15" ht="60">
+      <c r="A6" s="32"/>
+      <c r="B6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" s="16"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="18"/>
+    </row>
+    <row r="7" spans="1:15" ht="60">
+      <c r="A7" s="32"/>
+      <c r="B7" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="18"/>
+    </row>
+    <row r="8" spans="1:15" ht="60">
+      <c r="A8" s="32"/>
+      <c r="B8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8" s="16"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="18"/>
+    </row>
+    <row r="9" spans="1:15" ht="60">
+      <c r="A9" s="32"/>
+      <c r="B9" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K9" s="16"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="18"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J4:J7" r:id="rId2" display="ibatta@dbi.com"/>
+    <hyperlink ref="J8" r:id="rId3"/>
+    <hyperlink ref="J3" r:id="rId4"/>
+    <hyperlink ref="J9" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId6"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merge message factory and added enhancements and flows to chekcout base
- added functions to cart 
- added functions to checkout pages 
- added subtotal verification to checkout base
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="5670" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Registration" sheetId="5" r:id="rId2"/>
     <sheet name="CheckOut" sheetId="7" r:id="rId3"/>
-    <sheet name="products" sheetId="8" r:id="rId4"/>
-    <sheet name="cards" sheetId="9" r:id="rId5"/>
-    <sheet name="addresses" sheetId="10" r:id="rId6"/>
-    <sheet name="CheckOut.bak" sheetId="12" r:id="rId7"/>
+    <sheet name="users" sheetId="13" r:id="rId4"/>
+    <sheet name="products" sheetId="8" r:id="rId5"/>
+    <sheet name="cards" sheetId="9" r:id="rId6"/>
+    <sheet name="addresses" sheetId="10" r:id="rId7"/>
+    <sheet name="CheckOut.bak" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="145">
   <si>
     <t>TCID</t>
   </si>
@@ -448,6 +449,27 @@
     <t>loggedin
 old-user
 saved-shipping
+new-payment</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>ibatta</t>
+  </si>
+  <si>
+    <t>loggedin
+old-user
+new-shipping
 new-payment</t>
   </si>
 </sst>
@@ -598,7 +620,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -688,6 +710,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1369,7 +1394,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1445,7 +1470,7 @@
         <v>65</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>125</v>
@@ -1460,10 +1485,7 @@
         <v>91</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="J2" s="13" t="s">
         <v>101</v>
@@ -1631,7 +1653,9 @@
       <c r="H7" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="J7" s="13" t="s">
         <v>101</v>
       </c>
@@ -1722,10 +1746,60 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="24">
+        <v>1234567</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1804,7 +1878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -1946,7 +2020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -2088,7 +2162,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O9"/>
   <sheetViews>

</xml_diff>

<commit_message>
added sign in error message getter
Signed-off-by: Ibrahem Batta <18301319+ibatta@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="16065" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="17010" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="5" r:id="rId1"/>
@@ -490,33 +490,33 @@
     <t>2226</t>
   </si>
   <si>
+    <t>£10.99</t>
+  </si>
+  <si>
+    <t>£53.36</t>
+  </si>
+  <si>
+    <t>Your order includes £8.89 tax.</t>
+  </si>
+  <si>
+    <t>£64.35</t>
+  </si>
+  <si>
     <t>ORDER NUMBER
-00001255</t>
-  </si>
-  <si>
-    <t>£38.58</t>
-  </si>
-  <si>
-    <t>£10.99</t>
-  </si>
-  <si>
-    <t>Your order includes £6.43 tax.</t>
-  </si>
-  <si>
-    <t>£49.57</t>
+00001269</t>
+  </si>
+  <si>
+    <t>£77.16</t>
+  </si>
+  <si>
+    <t>Your order includes £12.86 tax.</t>
+  </si>
+  <si>
+    <t>£88.15</t>
   </si>
   <si>
     <t>ORDER NUMBER
-00001257</t>
-  </si>
-  <si>
-    <t>£53.36</t>
-  </si>
-  <si>
-    <t>Your order includes £8.89 tax.</t>
-  </si>
-  <si>
-    <t>£64.35</t>
+00001271</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1418,7 @@
     <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1505,19 +1505,19 @@
         <v>96</v>
       </c>
       <c r="L2" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="P2" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="6" customFormat="1" ht="60">
@@ -1647,19 +1647,19 @@
         <v>96</v>
       </c>
       <c r="L5" s="34" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="60">

</xml_diff>

<commit_message>
Added a set of tests for cart / tmp to be converted to excel sheet merge Abeer changes for PLP / profile validation
Signed-off-by: Ibrahem Batta <18301319+ibatta@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="28350" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="33030" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="255">
   <si>
     <t>aa@gg.cc</t>
   </si>
@@ -739,14 +739,6 @@
   </si>
   <si>
     <t>ORDER NUMBER
-00001390</t>
-  </si>
-  <si>
-    <t>ORDER NUMBER
-00001392</t>
-  </si>
-  <si>
-    <t>ORDER NUMBER
 00001394</t>
   </si>
   <si>
@@ -826,12 +818,37 @@
   <si>
     <t>ORDER NUMBER
 00001427</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER
+00001478</t>
+  </si>
+  <si>
+    <t>T38</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER
+00001534</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER
+00001572</t>
+  </si>
+  <si>
+    <t>£115.74</t>
+  </si>
+  <si>
+    <t>Your order includes £19.29 tax.</t>
+  </si>
+  <si>
+    <t>£126.73</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -1421,23 +1438,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="3" width="15.7109375" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="13.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="13.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="9" customFormat="1">
@@ -1692,7 +1709,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="cc@dd.cc"/>
+    <hyperlink ref="B3" r:id="rId32" display="cc@dd.cc"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1704,28 +1721,28 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B38"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.87890625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="10.671875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.74609375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="28.88671875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.8984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="9" customFormat="1">
@@ -1811,16 +1828,16 @@
         <v>92</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>202</v>
+        <v>254</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>198</v>
+        <v>252</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>200</v>
+        <v>253</v>
       </c>
       <c r="P2" s="14" t="s">
         <v>195</v>
@@ -1830,7 +1847,9 @@
       <c r="A3" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="C3" s="10" t="s">
         <v>149</v>
       </c>
@@ -1857,19 +1876,19 @@
         <v>92</v>
       </c>
       <c r="L3" s="33" t="s">
-        <v>227</v>
+        <v>141</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>198</v>
+        <v>141</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>200</v>
+        <v>141</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>195</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="6" customFormat="1" ht="60">
@@ -1903,7 +1922,7 @@
         <v>92</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M4" s="14" t="s">
         <v>201</v>
@@ -1949,7 +1968,7 @@
         <v>92</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M5" s="14" t="s">
         <v>202</v>
@@ -1995,7 +2014,7 @@
         <v>92</v>
       </c>
       <c r="L6" s="33" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M6" s="14" t="s">
         <v>202</v>
@@ -2041,7 +2060,7 @@
         <v>92</v>
       </c>
       <c r="L7" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="M7" s="14" t="s">
         <v>201</v>
@@ -2133,7 +2152,7 @@
         <v>92</v>
       </c>
       <c r="L9" s="33" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M9" s="14" t="s">
         <v>197</v>
@@ -2179,7 +2198,7 @@
         <v>92</v>
       </c>
       <c r="L10" s="33" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M10" s="14" t="s">
         <v>201</v>
@@ -2225,7 +2244,7 @@
         <v>92</v>
       </c>
       <c r="L11" s="33" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M11" s="14" t="s">
         <v>202</v>
@@ -2271,7 +2290,7 @@
         <v>92</v>
       </c>
       <c r="L12" s="33" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M12" s="14" t="s">
         <v>202</v>
@@ -2360,10 +2379,10 @@
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L14" s="33" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M14" s="14" t="s">
         <v>202</v>
@@ -2406,10 +2425,10 @@
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L15" s="33" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M15" s="14" t="s">
         <v>202</v>
@@ -2452,10 +2471,10 @@
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M16" s="14" t="s">
         <v>201</v>
@@ -2498,10 +2517,10 @@
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L17" s="33" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M17" s="14" t="s">
         <v>202</v>
@@ -2544,10 +2563,10 @@
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="10" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="L18" s="33" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="M18" s="14" t="s">
         <v>202</v>
@@ -2590,10 +2609,10 @@
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L19" s="33" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M19" s="14" t="s">
         <v>201</v>
@@ -2685,7 +2704,7 @@
         <v>92</v>
       </c>
       <c r="L21" s="33" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="M21" s="14" t="s">
         <v>197</v>
@@ -2731,7 +2750,7 @@
         <v>92</v>
       </c>
       <c r="L22" s="33" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="M22" s="14" t="s">
         <v>201</v>
@@ -3480,32 +3499,76 @@
         <v>199</v>
       </c>
     </row>
+    <row r="39" spans="1:16" ht="60">
+      <c r="A39" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="B39" s="29"/>
+      <c r="C39" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J39" s="5"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="M39" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="N39" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="O39" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="P39" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K3" r:id="rId2"/>
-    <hyperlink ref="K4" r:id="rId3"/>
-    <hyperlink ref="K5" r:id="rId4"/>
-    <hyperlink ref="K6" r:id="rId5"/>
-    <hyperlink ref="K7" r:id="rId6"/>
-    <hyperlink ref="K8" r:id="rId7"/>
-    <hyperlink ref="K9" r:id="rId8"/>
-    <hyperlink ref="K10" r:id="rId9"/>
-    <hyperlink ref="K11" r:id="rId10"/>
-    <hyperlink ref="K12" r:id="rId11"/>
-    <hyperlink ref="K13" r:id="rId12"/>
-    <hyperlink ref="K20" r:id="rId13"/>
-    <hyperlink ref="K21" r:id="rId14"/>
-    <hyperlink ref="K22" r:id="rId15"/>
-    <hyperlink ref="K23" r:id="rId16"/>
-    <hyperlink ref="K24" r:id="rId17"/>
-    <hyperlink ref="K25" r:id="rId18"/>
-    <hyperlink ref="K26" r:id="rId19"/>
-    <hyperlink ref="K27" r:id="rId20"/>
-    <hyperlink ref="K28" r:id="rId21"/>
-    <hyperlink ref="K29" r:id="rId22"/>
-    <hyperlink ref="K30" r:id="rId23"/>
-    <hyperlink ref="K31" r:id="rId24"/>
+    <hyperlink ref="K2" r:id="rId722"/>
+    <hyperlink ref="K3" r:id="rId723"/>
+    <hyperlink ref="K4" r:id="rId724"/>
+    <hyperlink ref="K5" r:id="rId725"/>
+    <hyperlink ref="K6" r:id="rId726"/>
+    <hyperlink ref="K7" r:id="rId727"/>
+    <hyperlink ref="K8" r:id="rId728"/>
+    <hyperlink ref="K9" r:id="rId729"/>
+    <hyperlink ref="K10" r:id="rId730"/>
+    <hyperlink ref="K11" r:id="rId731"/>
+    <hyperlink ref="K12" r:id="rId732"/>
+    <hyperlink ref="K13" r:id="rId733"/>
+    <hyperlink ref="K20" r:id="rId734"/>
+    <hyperlink ref="K21" r:id="rId735"/>
+    <hyperlink ref="K22" r:id="rId736"/>
+    <hyperlink ref="K23" r:id="rId737"/>
+    <hyperlink ref="K24" r:id="rId738"/>
+    <hyperlink ref="K25" r:id="rId739"/>
+    <hyperlink ref="K26" r:id="rId740"/>
+    <hyperlink ref="K27" r:id="rId741"/>
+    <hyperlink ref="K28" r:id="rId742"/>
+    <hyperlink ref="K29" r:id="rId743"/>
+    <hyperlink ref="K30" r:id="rId744"/>
+    <hyperlink ref="K31" r:id="rId745"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId25"/>
@@ -3525,10 +3588,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1">
@@ -3579,7 +3642,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
@@ -3594,14 +3657,14 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3681,15 +3744,15 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3831,14 +3894,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="12" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3970,26 +4033,26 @@
   </sheetPr>
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" workbookViewId="0">
-      <selection sqref="A1:P38"/>
+    <sheetView topLeftCell="A31" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="9" customFormat="1">
@@ -4046,7 +4109,9 @@
       <c r="A2" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="29"/>
+      <c r="B2" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="C2" s="10" t="s">
         <v>148</v>
       </c>
@@ -4092,7 +4157,9 @@
       <c r="A3" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="C3" s="10" t="s">
         <v>149</v>
       </c>
@@ -5720,30 +5787,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K3" r:id="rId2"/>
-    <hyperlink ref="K4" r:id="rId3"/>
-    <hyperlink ref="K5" r:id="rId4"/>
-    <hyperlink ref="K6" r:id="rId5"/>
-    <hyperlink ref="K7" r:id="rId6"/>
-    <hyperlink ref="K8" r:id="rId7"/>
-    <hyperlink ref="K9" r:id="rId8"/>
-    <hyperlink ref="K10" r:id="rId9"/>
-    <hyperlink ref="K11" r:id="rId10"/>
-    <hyperlink ref="K12" r:id="rId11"/>
-    <hyperlink ref="K13" r:id="rId12"/>
-    <hyperlink ref="K20" r:id="rId13"/>
-    <hyperlink ref="K21" r:id="rId14"/>
-    <hyperlink ref="K22" r:id="rId15"/>
-    <hyperlink ref="K23" r:id="rId16"/>
-    <hyperlink ref="K24" r:id="rId17"/>
-    <hyperlink ref="K25" r:id="rId18"/>
-    <hyperlink ref="K26" r:id="rId19"/>
-    <hyperlink ref="K27" r:id="rId20"/>
-    <hyperlink ref="K28" r:id="rId21"/>
-    <hyperlink ref="K29" r:id="rId22"/>
-    <hyperlink ref="K30" r:id="rId23"/>
-    <hyperlink ref="K31" r:id="rId24"/>
+    <hyperlink ref="K2" r:id="rId722"/>
+    <hyperlink ref="K3" r:id="rId723"/>
+    <hyperlink ref="K4" r:id="rId724"/>
+    <hyperlink ref="K5" r:id="rId725"/>
+    <hyperlink ref="K6" r:id="rId726"/>
+    <hyperlink ref="K7" r:id="rId727"/>
+    <hyperlink ref="K8" r:id="rId728"/>
+    <hyperlink ref="K9" r:id="rId729"/>
+    <hyperlink ref="K10" r:id="rId730"/>
+    <hyperlink ref="K11" r:id="rId731"/>
+    <hyperlink ref="K12" r:id="rId732"/>
+    <hyperlink ref="K13" r:id="rId733"/>
+    <hyperlink ref="K20" r:id="rId734"/>
+    <hyperlink ref="K21" r:id="rId735"/>
+    <hyperlink ref="K22" r:id="rId736"/>
+    <hyperlink ref="K23" r:id="rId737"/>
+    <hyperlink ref="K24" r:id="rId738"/>
+    <hyperlink ref="K25" r:id="rId739"/>
+    <hyperlink ref="K26" r:id="rId740"/>
+    <hyperlink ref="K27" r:id="rId741"/>
+    <hyperlink ref="K28" r:id="rId742"/>
+    <hyperlink ref="K29" r:id="rId743"/>
+    <hyperlink ref="K30" r:id="rId744"/>
+    <hyperlink ref="K31" r:id="rId745"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId25"/>

</xml_diff>

<commit_message>
Added fixed to emad tests, upgrade xlxs reader
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="133665" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="134595" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="5" r:id="rId1"/>
@@ -4461,8 +4461,8 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36:P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4494,13 +4494,13 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="21" t="s">
         <v>64</v>
       </c>
       <c r="D2" s="21" t="s">
@@ -4514,13 +4514,13 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>55</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -4534,13 +4534,13 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="21" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="21" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -4554,13 +4554,13 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="21" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="21" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -4574,13 +4574,13 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="21" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="21" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="21" t="s">
@@ -12617,7 +12617,7 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
personal details fixes :@
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="134595" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="154125" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2675" uniqueCount="740">
   <si>
     <t>aa@gg.cc</t>
   </si>
@@ -2125,15 +2125,6 @@
     <t xml:space="preserve">firstName </t>
   </si>
   <si>
-    <t>doVerifyCurrent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doClickCancelBtn </t>
-  </si>
-  <si>
-    <t>doClickUpdateBtn</t>
-  </si>
-  <si>
     <t>global-alerts</t>
   </si>
   <si>
@@ -2149,42 +2140,10 @@
     <t>https://hybrisdemo.conexus.co.uk:9002/yacceleratorstorefront/en/my-account/update-profile</t>
   </si>
   <si>
-    <t>MISS</t>
-  </si>
-  <si>
-    <t>Abeer</t>
-  </si>
-  <si>
-    <t>Alia</t>
-  </si>
-  <si>
     <t>Personal Details Cancel</t>
   </si>
   <si>
-    <t>Abeer1</t>
-  </si>
-  <si>
-    <t>Alia2</t>
-  </si>
-  <si>
-    <t>MS.</t>
-  </si>
-  <si>
-    <t>Abeer2</t>
-  </si>
-  <si>
-    <t>Alia3</t>
-  </si>
-  <si>
-    <t>×
-Your profile has been updated</t>
-  </si>
-  <si>
     <t>Personal Details Without firstName</t>
-  </si>
-  <si>
-    <t>×
-Please correct the errors below.</t>
   </si>
   <si>
     <t>Personal Details Without lastName</t>
@@ -2342,6 +2301,35 @@
   </si>
   <si>
     <t>Add a new payment throuth checkout then delete it from payment page</t>
+  </si>
+  <si>
+    <t>Accept2</t>
+  </si>
+  <si>
+    <t>Your profile has been updated</t>
+  </si>
+  <si>
+    <t>Please correct the errors below.</t>
+  </si>
+  <si>
+    <t>Verify current user</t>
+  </si>
+  <si>
+    <t>click cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click update </t>
+  </si>
+  <si>
+    <t>click update
+revert changes</t>
+  </si>
+  <si>
+    <t>Tester2</t>
+  </si>
+  <si>
+    <t>click update 
+revert changes</t>
   </si>
 </sst>
 </file>
@@ -2551,7 +2539,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2722,9 +2710,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2733,12 +2718,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2784,6 +2763,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3426,7 +3408,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G7" sqref="G7:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4461,7 +4443,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="P36" sqref="P36:P37"/>
     </sheetView>
   </sheetViews>
@@ -4740,7 +4722,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="21" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>11</v>
@@ -4752,13 +4734,13 @@
         <v>118</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
       <c r="F5" s="26" t="s">
         <v>71</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>73</v>
@@ -8899,8 +8881,8 @@
   </sheetPr>
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="A28" zoomScale="85" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11770,29 +11752,28 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:11">
       <c r="A1" s="16" t="s">
         <v>128</v>
       </c>
@@ -11803,340 +11784,253 @@
         <v>53</v>
       </c>
       <c r="D1" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>143</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>125</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>117</v>
+      <c r="G1" s="17" t="s">
+        <v>673</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>673</v>
-      </c>
-      <c r="I1" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="I1" s="53" t="s">
         <v>674</v>
       </c>
-      <c r="K1" s="62" t="s">
+      <c r="J1" s="53" t="s">
         <v>675</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="K1" s="53" t="s">
         <v>676</v>
       </c>
-      <c r="M1" s="53" t="s">
-        <v>677</v>
-      </c>
-      <c r="N1" s="53" t="s">
-        <v>678</v>
-      </c>
-      <c r="O1" s="53" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="45">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="55" t="s">
         <v>129</v>
       </c>
       <c r="B2" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="63" t="s">
-        <v>680</v>
-      </c>
-      <c r="D2" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
+      <c r="C2" s="62" t="s">
+        <v>677</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>734</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>327</v>
       </c>
       <c r="F2" s="48" t="s">
-        <v>681</v>
-      </c>
-      <c r="G2" s="65" t="s">
-        <v>682</v>
+        <v>678</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>683</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>684</v>
-      </c>
-      <c r="J2" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" s="56" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="56" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-    </row>
-    <row r="3" spans="1:15" ht="45">
+        <v>12</v>
+      </c>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="55" t="s">
         <v>130</v>
       </c>
       <c r="B3" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="63" t="s">
-        <v>685</v>
-      </c>
-      <c r="D3" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
+      <c r="C3" s="62" t="s">
+        <v>679</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>735</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>328</v>
       </c>
       <c r="F3" s="48" t="s">
-        <v>681</v>
-      </c>
-      <c r="G3" s="65" t="s">
-        <v>682</v>
+        <v>678</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>731</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>686</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>687</v>
-      </c>
-      <c r="J3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" s="56" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-    </row>
-    <row r="4" spans="1:15" ht="45">
+        <v>738</v>
+      </c>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="55" t="s">
         <v>131</v>
       </c>
       <c r="B4" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="63" t="s">
-        <v>685</v>
-      </c>
-      <c r="D4" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
+      <c r="C4" s="62" t="s">
+        <v>679</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>737</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>329</v>
       </c>
       <c r="F4" s="48" t="s">
-        <v>681</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>688</v>
+        <v>678</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>731</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>689</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>690</v>
-      </c>
-      <c r="J4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="66" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" s="67" t="s">
-        <v>691</v>
-      </c>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-    </row>
-    <row r="5" spans="1:15" ht="60">
+        <v>738</v>
+      </c>
+      <c r="I4" s="80" t="s">
+        <v>732</v>
+      </c>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="55" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B5" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="63" t="s">
-        <v>692</v>
-      </c>
-      <c r="D5" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
+      <c r="C5" s="62" t="s">
+        <v>680</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>736</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>330</v>
       </c>
       <c r="F5" s="48" t="s">
-        <v>681</v>
-      </c>
-      <c r="G5" s="65" t="s">
-        <v>682</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9" t="s">
-        <v>684</v>
-      </c>
-      <c r="J5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="56" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" s="67" t="s">
-        <v>693</v>
-      </c>
-      <c r="N5" s="56" t="s">
+        <v>678</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>738</v>
+      </c>
+      <c r="I5" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="J5" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="56"/>
-    </row>
-    <row r="6" spans="1:15" ht="60">
+      <c r="K5" s="56"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="55" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B6" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="63" t="s">
-        <v>694</v>
-      </c>
-      <c r="D6" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
+      <c r="C6" s="62" t="s">
+        <v>681</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>736</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>331</v>
       </c>
       <c r="F6" s="48" t="s">
-        <v>681</v>
-      </c>
-      <c r="G6" s="65" t="s">
-        <v>682</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>683</v>
-      </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" s="56" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" s="67" t="s">
-        <v>693</v>
-      </c>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56" t="s">
+        <v>678</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>731</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="90">
+    <row r="7" spans="1:11">
       <c r="A7" s="55" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B7" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="63" t="s">
-        <v>695</v>
-      </c>
-      <c r="D7" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
+      <c r="C7" s="62" t="s">
+        <v>682</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>736</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>332</v>
       </c>
       <c r="F7" s="48" t="s">
-        <v>681</v>
-      </c>
-      <c r="G7" s="65" t="s">
-        <v>682</v>
-      </c>
+        <v>678</v>
+      </c>
+      <c r="G7" s="9"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="56" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" s="67" t="s">
-        <v>693</v>
-      </c>
-      <c r="N7" s="56" t="s">
+      <c r="I7" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="J7" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="56" t="s">
+      <c r="K7" s="56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="45">
+    <row r="8" spans="1:11" ht="30">
       <c r="A8" s="55" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B8" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="63" t="s">
-        <v>696</v>
-      </c>
-      <c r="D8" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
+      <c r="C8" s="62" t="s">
+        <v>683</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>739</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>333</v>
       </c>
       <c r="F8" s="48" t="s">
-        <v>681</v>
-      </c>
-      <c r="G8" s="65" t="s">
-        <v>682</v>
+        <v>678</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>731</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>683</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>684</v>
-      </c>
-      <c r="J8" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="56" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="M8" s="67" t="s">
-        <v>691</v>
-      </c>
-      <c r="N8" s="56"/>
-      <c r="O8" s="56"/>
+        <v>738</v>
+      </c>
+      <c r="I8" s="80" t="s">
+        <v>732</v>
+      </c>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="tester29@qatesting.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="tester30@qatesting.com"/>
+    <hyperlink ref="E4" r:id="rId3" display="tester31@qatesting.com"/>
+    <hyperlink ref="E5" r:id="rId4" display="tester32@qatesting.com"/>
+    <hyperlink ref="E6" r:id="rId5" display="tester33@qatesting.com"/>
+    <hyperlink ref="E7" r:id="rId6" display="tester34@qatesting.com"/>
+    <hyperlink ref="E8" r:id="rId7" display="tester35@qatesting.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12188,25 +12082,25 @@
         <v>43</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>697</v>
+        <v>684</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>698</v>
+        <v>685</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>700</v>
+        <v>687</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>703</v>
+        <v>690</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -12216,37 +12110,37 @@
       <c r="B2" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="63" t="s">
-        <v>704</v>
-      </c>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="62" t="s">
+        <v>691</v>
+      </c>
+      <c r="D2" s="63" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="48" t="s">
-        <v>705</v>
-      </c>
-      <c r="G2" s="65" t="s">
-        <v>706</v>
-      </c>
-      <c r="H2" s="68" t="s">
-        <v>707</v>
-      </c>
-      <c r="I2" s="65" t="s">
-        <v>708</v>
-      </c>
-      <c r="J2" s="69" t="s">
-        <v>709</v>
-      </c>
-      <c r="K2" s="65" t="s">
-        <v>710</v>
-      </c>
-      <c r="L2" s="65" t="s">
-        <v>711</v>
-      </c>
-      <c r="M2" s="65">
+        <v>692</v>
+      </c>
+      <c r="G2" s="64" t="s">
+        <v>693</v>
+      </c>
+      <c r="H2" s="65" t="s">
+        <v>694</v>
+      </c>
+      <c r="I2" s="64" t="s">
+        <v>695</v>
+      </c>
+      <c r="J2" s="66" t="s">
+        <v>696</v>
+      </c>
+      <c r="K2" s="64" t="s">
+        <v>697</v>
+      </c>
+      <c r="L2" s="64" t="s">
+        <v>698</v>
+      </c>
+      <c r="M2" s="64">
         <v>0</v>
       </c>
     </row>
@@ -12257,37 +12151,37 @@
       <c r="B3" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="63" t="s">
-        <v>712</v>
-      </c>
-      <c r="D3" s="64" t="s">
+      <c r="C3" s="62" t="s">
+        <v>699</v>
+      </c>
+      <c r="D3" s="63" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="48" t="s">
-        <v>705</v>
-      </c>
-      <c r="G3" s="65" t="s">
-        <v>713</v>
-      </c>
-      <c r="H3" s="65" t="s">
-        <v>714</v>
-      </c>
-      <c r="I3" s="65" t="s">
-        <v>708</v>
-      </c>
-      <c r="J3" s="69" t="s">
-        <v>715</v>
-      </c>
-      <c r="K3" s="65" t="s">
-        <v>716</v>
-      </c>
-      <c r="L3" s="65" t="s">
-        <v>711</v>
-      </c>
-      <c r="M3" s="65">
+        <v>692</v>
+      </c>
+      <c r="G3" s="64" t="s">
+        <v>700</v>
+      </c>
+      <c r="H3" s="64" t="s">
+        <v>701</v>
+      </c>
+      <c r="I3" s="64" t="s">
+        <v>695</v>
+      </c>
+      <c r="J3" s="66" t="s">
+        <v>702</v>
+      </c>
+      <c r="K3" s="64" t="s">
+        <v>703</v>
+      </c>
+      <c r="L3" s="64" t="s">
+        <v>698</v>
+      </c>
+      <c r="M3" s="64">
         <v>1</v>
       </c>
     </row>
@@ -12310,129 +12204,129 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="70"/>
+    <col min="1" max="2" width="9.140625" style="67"/>
     <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="70" customFormat="1">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:5" s="67" customFormat="1">
+      <c r="A1" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="76" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>710</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="105">
+      <c r="A4" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>716</v>
+      </c>
+      <c r="E4" s="78" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="77" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>718</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="77" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="80" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="80" t="s">
+      <c r="D6" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" s="77" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>722</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>723</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="80" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="E7" s="78" t="s">
         <v>725</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>726</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="105">
-      <c r="A4" s="80" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>728</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>729</v>
-      </c>
-      <c r="E4" s="81" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="80" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>731</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>732</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="80" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>734</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>735</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="80" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>736</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>737</v>
-      </c>
-      <c r="E7" s="81" t="s">
-        <v>738</v>
       </c>
     </row>
   </sheetData>
@@ -12485,7 +12379,7 @@
       <c r="D1" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="68" t="s">
         <v>51</v>
       </c>
       <c r="F1" s="36" t="s">
@@ -12493,102 +12387,102 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="45">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="72" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="69" t="s">
         <v>546</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="D2" s="73" t="s">
         <v>550</v>
       </c>
-      <c r="E2" s="74" t="s">
+      <c r="E2" s="71" t="s">
         <v>323</v>
       </c>
-      <c r="F2" s="75" t="s">
+      <c r="F2" s="72" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="69" t="s">
         <v>546</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="73" t="s">
         <v>549</v>
       </c>
-      <c r="E3" s="74" t="s">
+      <c r="E3" s="71" t="s">
         <v>324</v>
       </c>
-      <c r="F3" s="75" t="s">
-        <v>717</v>
+      <c r="F3" s="72" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="72" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="69" t="s">
         <v>546</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="73" t="s">
         <v>548</v>
       </c>
-      <c r="E4" s="74" t="s">
+      <c r="E4" s="71" t="s">
         <v>325</v>
       </c>
-      <c r="F4" s="75" t="s">
-        <v>717</v>
+      <c r="F4" s="72" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="72" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="69" t="s">
         <v>546</v>
       </c>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="73" t="s">
         <v>547</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="E5" s="71" t="s">
         <v>326</v>
       </c>
-      <c r="F5" s="75" t="s">
-        <v>717</v>
+      <c r="F5" s="72" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="69" t="s">
         <v>546</v>
       </c>
-      <c r="D6" s="76" t="s">
+      <c r="D6" s="73" t="s">
         <v>545</v>
       </c>
-      <c r="E6" s="74" t="s">
+      <c r="E6" s="71" t="s">
         <v>327</v>
       </c>
-      <c r="F6" s="75" t="s">
+      <c r="F6" s="72" t="s">
         <v>83</v>
       </c>
     </row>
@@ -12641,7 +12535,7 @@
       <c r="C1" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="70" t="s">
         <v>52</v>
       </c>
       <c r="E1" s="30" t="s">
@@ -12674,13 +12568,13 @@
         <v>101</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>742</v>
+        <v>729</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>718</v>
-      </c>
-      <c r="E2" s="82" t="s">
-        <v>719</v>
+        <v>705</v>
+      </c>
+      <c r="E2" s="79" t="s">
+        <v>706</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>237</v>
@@ -12688,16 +12582,16 @@
       <c r="G2" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="77" t="s">
+      <c r="H2" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="77" t="s">
+      <c r="I2" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="77" t="s">
-        <v>717</v>
-      </c>
-      <c r="K2" s="74" t="s">
+      <c r="J2" s="74" t="s">
+        <v>704</v>
+      </c>
+      <c r="K2" s="71" t="s">
         <v>324</v>
       </c>
     </row>
@@ -12709,13 +12603,13 @@
         <v>101</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>743</v>
+        <v>730</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>720</v>
-      </c>
-      <c r="E3" s="82" t="s">
-        <v>719</v>
+        <v>707</v>
+      </c>
+      <c r="E3" s="79" t="s">
+        <v>706</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>237</v>
@@ -12723,16 +12617,16 @@
       <c r="G3" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="77" t="s">
+      <c r="I3" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="77" t="s">
-        <v>717</v>
-      </c>
-      <c r="K3" s="74" t="s">
+      <c r="J3" s="74" t="s">
+        <v>704</v>
+      </c>
+      <c r="K3" s="71" t="s">
         <v>323</v>
       </c>
     </row>

</xml_diff>

<commit_message>
emad_shawahni changes  order details order history email and password validation  + PLP Abeer
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="157845" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="158775" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="5" r:id="rId1"/>
@@ -17,11 +17,13 @@
     <sheet name="AddressBookRegression" sheetId="19" r:id="rId8"/>
     <sheet name="PaymentDetailsRegression" sheetId="25" r:id="rId9"/>
     <sheet name="StoreLocatorRegression" sheetId="26" r:id="rId10"/>
-    <sheet name="users" sheetId="13" r:id="rId11"/>
-    <sheet name="products" sheetId="8" r:id="rId12"/>
-    <sheet name="cards" sheetId="9" r:id="rId13"/>
-    <sheet name="addresses" sheetId="10" r:id="rId14"/>
-    <sheet name="users_alternatives" sheetId="20" r:id="rId15"/>
+    <sheet name="EmailAddressRegression" sheetId="27" r:id="rId11"/>
+    <sheet name="PasswordRegression" sheetId="28" r:id="rId12"/>
+    <sheet name="users" sheetId="13" r:id="rId13"/>
+    <sheet name="products" sheetId="8" r:id="rId14"/>
+    <sheet name="cards" sheetId="9" r:id="rId15"/>
+    <sheet name="addresses" sheetId="10" r:id="rId16"/>
+    <sheet name="users_alternatives" sheetId="20" r:id="rId17"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="793">
   <si>
     <t>aa@gg.cc</t>
   </si>
@@ -2159,18 +2161,6 @@
     <t>sortByText</t>
   </si>
   <si>
-    <t>orders Number</t>
-  </si>
-  <si>
-    <t>orders status</t>
-  </si>
-  <si>
-    <t>orders date</t>
-  </si>
-  <si>
-    <t>orders total</t>
-  </si>
-  <si>
     <t>orders nthChildren</t>
   </si>
   <si>
@@ -2186,18 +2176,6 @@
     <t>Order Number</t>
   </si>
   <si>
-    <t>00001785;00001787</t>
-  </si>
-  <si>
-    <t>Completed;Completed</t>
-  </si>
-  <si>
-    <t>Dec 11, 2017 7:58 AM;Dec 11, 2017 8:03 AM</t>
-  </si>
-  <si>
-    <t>£46.45;£111.25</t>
-  </si>
-  <si>
     <t>1;3;5;7</t>
   </si>
   <si>
@@ -2205,15 +2183,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>00001787;00001785</t>
-  </si>
-  <si>
-    <t>Dec 11, 2017 8:03 AM;Dec 11, 2017 7:58 AM</t>
-  </si>
-  <si>
-    <t>£111.25;£46.45</t>
   </si>
   <si>
     <t>A4</t>
@@ -2298,12 +2267,6 @@
     <t>W1T 1JY</t>
   </si>
   <si>
-    <t>Add a new payment throuth checkout and update the default payment</t>
-  </si>
-  <si>
-    <t>Add a new payment throuth checkout then delete it from payment page</t>
-  </si>
-  <si>
     <t>Accept2</t>
   </si>
   <si>
@@ -2352,6 +2315,183 @@
   </si>
   <si>
     <t>-Negative:Check that you entered a valid postcode or place name.</t>
+  </si>
+  <si>
+    <t>currentEmail</t>
+  </si>
+  <si>
+    <t>confirmNewEmail</t>
+  </si>
+  <si>
+    <t>emailErrors</t>
+  </si>
+  <si>
+    <t>confirmEmailEerrors</t>
+  </si>
+  <si>
+    <t>passwordErrors</t>
+  </si>
+  <si>
+    <t>Email Address Check</t>
+  </si>
+  <si>
+    <t>https://hybrisdemo.conexus.co.uk:9002/yacceleratorstorefront/en/my-account/update-email</t>
+  </si>
+  <si>
+    <t>Email Address Cancel</t>
+  </si>
+  <si>
+    <t>tester@qatesting.com</t>
+  </si>
+  <si>
+    <t>Email Address Update</t>
+  </si>
+  <si>
+    <t>etabib@qatesting.com</t>
+  </si>
+  <si>
+    <t>Email Address Update Without  NewEmail</t>
+  </si>
+  <si>
+    <t>utester2@qatesting.com</t>
+  </si>
+  <si>
+    <t>Email Address Update Without ConfirmEmail</t>
+  </si>
+  <si>
+    <t>utester3@qatesting.com</t>
+  </si>
+  <si>
+    <t>Please confirm your email address</t>
+  </si>
+  <si>
+    <t>Email Address Update Without password</t>
+  </si>
+  <si>
+    <t>utester4@qatesting.com</t>
+  </si>
+  <si>
+    <t>Please enter your password</t>
+  </si>
+  <si>
+    <t>Email Address Update With Invalid email</t>
+  </si>
+  <si>
+    <t>tester1</t>
+  </si>
+  <si>
+    <t>utester5@qatesting.com</t>
+  </si>
+  <si>
+    <t>Email Address Update With Invalid confirm email</t>
+  </si>
+  <si>
+    <t>utester6@qatesting.com</t>
+  </si>
+  <si>
+    <t>tester2</t>
+  </si>
+  <si>
+    <t>Email and Re-enter email address does not match</t>
+  </si>
+  <si>
+    <t>Email Address Update With differnt confirm email</t>
+  </si>
+  <si>
+    <t>utester7@qatesting.com</t>
+  </si>
+  <si>
+    <t>utester8@qatesting.com</t>
+  </si>
+  <si>
+    <t>Email Address Update With Invalid password</t>
+  </si>
+  <si>
+    <t>utester9@qatesting.com</t>
+  </si>
+  <si>
+    <t>Please enter your current password</t>
+  </si>
+  <si>
+    <t>Email Address Update With already existing account</t>
+  </si>
+  <si>
+    <t>click update</t>
+  </si>
+  <si>
+    <t>The email you entered is not available</t>
+  </si>
+  <si>
+    <t>currentPassword</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>confirmNewPassword</t>
+  </si>
+  <si>
+    <t>currentPasswordErrors</t>
+  </si>
+  <si>
+    <t>newPasswordEerrors</t>
+  </si>
+  <si>
+    <t>confirmNewPasswordErrors</t>
+  </si>
+  <si>
+    <t>Password Cancel</t>
+  </si>
+  <si>
+    <t>https://hybrisdemo.conexus.co.uk:9002/yacceleratorstorefront/en/my-account/update-password</t>
+  </si>
+  <si>
+    <t>Password Update</t>
+  </si>
+  <si>
+    <t>Your password has been changed</t>
+  </si>
+  <si>
+    <t>Password Update: Without  current password</t>
+  </si>
+  <si>
+    <t>Password Update: Incorrect current password</t>
+  </si>
+  <si>
+    <t>Password Update: Without new password</t>
+  </si>
+  <si>
+    <t>Password does not meet minimum requirements.</t>
+  </si>
+  <si>
+    <t>Password Update: Invalid new password</t>
+  </si>
+  <si>
+    <t>Password Update: Without confirm new password</t>
+  </si>
+  <si>
+    <t>Password Update: Incorrect confirm new password</t>
+  </si>
+  <si>
+    <t>Password Update: Pasword not match password rules.</t>
+  </si>
+  <si>
+    <t>Password Update: Confirm password not matching.</t>
+  </si>
+  <si>
+    <t>Password and password confirmation do not match</t>
+  </si>
+  <si>
+    <t>Order History with No Orders</t>
+  </si>
+  <si>
+    <t>tester1@ordershistory.com</t>
+  </si>
+  <si>
+    <t>Add a new payment through checkout and update the default payment</t>
+  </si>
+  <si>
+    <t>Add a new payment through checkout then delete it from payment page</t>
   </si>
 </sst>
 </file>
@@ -2561,7 +2701,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2735,16 +2875,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2790,6 +2921,32 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3430,8 +3587,8 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3451,11 +3608,11 @@
       <c r="C1" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="67" t="s">
         <v>52</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3466,11 +3623,11 @@
         <v>101</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
       <c r="D2" s="33"/>
-      <c r="E2" s="81" t="s">
-        <v>745</v>
+      <c r="E2" s="78" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3481,11 +3638,11 @@
         <v>101</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>742</v>
+        <v>729</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21" t="s">
-        <v>744</v>
+        <v>731</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3496,10 +3653,10 @@
         <v>101</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>743</v>
+        <v>730</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>746</v>
+        <v>733</v>
       </c>
       <c r="E4" s="21"/>
     </row>
@@ -3510,6 +3667,938 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>734</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>735</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="84" t="s">
+        <v>674</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="L1" s="84" t="s">
+        <v>737</v>
+      </c>
+      <c r="M1" s="84" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="60">
+      <c r="A2" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2" s="79" t="s">
+        <v>721</v>
+      </c>
+      <c r="E2" s="85" t="s">
+        <v>324</v>
+      </c>
+      <c r="F2" s="85" t="s">
+        <v>740</v>
+      </c>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+    </row>
+    <row r="3" spans="1:13" ht="60">
+      <c r="A3" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>741</v>
+      </c>
+      <c r="D3" s="79" t="s">
+        <v>722</v>
+      </c>
+      <c r="E3" s="85" t="s">
+        <v>325</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>740</v>
+      </c>
+      <c r="G3" s="85" t="s">
+        <v>742</v>
+      </c>
+      <c r="H3" s="68" t="s">
+        <v>742</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+    </row>
+    <row r="4" spans="1:13" ht="60">
+      <c r="A4" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>743</v>
+      </c>
+      <c r="D4" s="79" t="s">
+        <v>724</v>
+      </c>
+      <c r="E4" s="85" t="s">
+        <v>326</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>740</v>
+      </c>
+      <c r="G4" s="85" t="s">
+        <v>744</v>
+      </c>
+      <c r="H4" s="85" t="s">
+        <v>744</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="J4" s="77" t="s">
+        <v>719</v>
+      </c>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+    </row>
+    <row r="5" spans="1:13" ht="60">
+      <c r="A5" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>745</v>
+      </c>
+      <c r="D5" s="79" t="s">
+        <v>723</v>
+      </c>
+      <c r="E5" s="85" t="s">
+        <v>324</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>740</v>
+      </c>
+      <c r="G5" s="31"/>
+      <c r="H5" s="85" t="s">
+        <v>746</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="J5" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K5" s="77" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+    </row>
+    <row r="6" spans="1:13" ht="60">
+      <c r="A6" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>747</v>
+      </c>
+      <c r="D6" s="79" t="s">
+        <v>723</v>
+      </c>
+      <c r="E6" s="85" t="s">
+        <v>325</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>740</v>
+      </c>
+      <c r="G6" s="85" t="s">
+        <v>748</v>
+      </c>
+      <c r="H6" s="31"/>
+      <c r="I6" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="J6" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77" t="s">
+        <v>749</v>
+      </c>
+      <c r="M6" s="77"/>
+    </row>
+    <row r="7" spans="1:13" ht="60">
+      <c r="A7" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>750</v>
+      </c>
+      <c r="D7" s="79" t="s">
+        <v>723</v>
+      </c>
+      <c r="E7" s="85" t="s">
+        <v>326</v>
+      </c>
+      <c r="F7" s="52" t="s">
+        <v>740</v>
+      </c>
+      <c r="G7" s="85" t="s">
+        <v>751</v>
+      </c>
+      <c r="H7" s="85" t="s">
+        <v>751</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="60">
+      <c r="A8" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>753</v>
+      </c>
+      <c r="D8" s="79" t="s">
+        <v>723</v>
+      </c>
+      <c r="E8" s="85" t="s">
+        <v>324</v>
+      </c>
+      <c r="F8" s="52" t="s">
+        <v>740</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>754</v>
+      </c>
+      <c r="H8" s="68" t="s">
+        <v>755</v>
+      </c>
+      <c r="I8" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="J8" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K8" s="77" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+    </row>
+    <row r="9" spans="1:13" ht="60">
+      <c r="A9" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>756</v>
+      </c>
+      <c r="D9" s="79" t="s">
+        <v>723</v>
+      </c>
+      <c r="E9" s="85" t="s">
+        <v>325</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>740</v>
+      </c>
+      <c r="G9" s="68" t="s">
+        <v>757</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>758</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="J9" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77" t="s">
+        <v>759</v>
+      </c>
+      <c r="M9" s="77"/>
+    </row>
+    <row r="10" spans="1:13" ht="60">
+      <c r="A10" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="62" t="s">
+        <v>760</v>
+      </c>
+      <c r="D10" s="79" t="s">
+        <v>723</v>
+      </c>
+      <c r="E10" s="85" t="s">
+        <v>326</v>
+      </c>
+      <c r="F10" s="52" t="s">
+        <v>740</v>
+      </c>
+      <c r="G10" s="68" t="s">
+        <v>761</v>
+      </c>
+      <c r="H10" s="68" t="s">
+        <v>762</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="J10" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K10" s="77"/>
+      <c r="L10" s="77" t="s">
+        <v>759</v>
+      </c>
+      <c r="M10" s="77"/>
+    </row>
+    <row r="11" spans="1:13" ht="60">
+      <c r="A11" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="62" t="s">
+        <v>763</v>
+      </c>
+      <c r="D11" s="79" t="s">
+        <v>723</v>
+      </c>
+      <c r="E11" s="85" t="s">
+        <v>324</v>
+      </c>
+      <c r="F11" s="52" t="s">
+        <v>740</v>
+      </c>
+      <c r="G11" s="68" t="s">
+        <v>764</v>
+      </c>
+      <c r="H11" s="68" t="s">
+        <v>764</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K11" s="77"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="77" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="60">
+      <c r="A12" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>766</v>
+      </c>
+      <c r="D12" s="79" t="s">
+        <v>767</v>
+      </c>
+      <c r="E12" s="85" t="s">
+        <v>325</v>
+      </c>
+      <c r="F12" s="52" t="s">
+        <v>740</v>
+      </c>
+      <c r="G12" s="85" t="s">
+        <v>344</v>
+      </c>
+      <c r="H12" s="85" t="s">
+        <v>344</v>
+      </c>
+      <c r="I12" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="J12" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K12" s="77" t="s">
+        <v>768</v>
+      </c>
+      <c r="L12" s="77"/>
+      <c r="M12" s="77"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="G12" r:id="rId3"/>
+    <hyperlink ref="H3" r:id="rId4"/>
+    <hyperlink ref="H8" r:id="rId5"/>
+    <hyperlink ref="H4" r:id="rId6"/>
+    <hyperlink ref="H5" r:id="rId7"/>
+    <hyperlink ref="G6" r:id="rId8"/>
+    <hyperlink ref="G7" r:id="rId9"/>
+    <hyperlink ref="H7" r:id="rId10"/>
+    <hyperlink ref="G9" r:id="rId11"/>
+    <hyperlink ref="G10" r:id="rId12"/>
+    <hyperlink ref="H10" r:id="rId13"/>
+    <hyperlink ref="G11" r:id="rId14"/>
+    <hyperlink ref="H11" r:id="rId15"/>
+    <hyperlink ref="H12" r:id="rId16"/>
+    <hyperlink ref="E4" r:id="rId17"/>
+    <hyperlink ref="E2" r:id="rId18"/>
+    <hyperlink ref="E3" r:id="rId19"/>
+    <hyperlink ref="E7" r:id="rId20"/>
+    <hyperlink ref="E5" r:id="rId21"/>
+    <hyperlink ref="E6" r:id="rId22"/>
+    <hyperlink ref="E10" r:id="rId23"/>
+    <hyperlink ref="E8" r:id="rId24"/>
+    <hyperlink ref="E9" r:id="rId25"/>
+    <hyperlink ref="E11" r:id="rId26"/>
+    <hyperlink ref="E12" r:id="rId27"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId28"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>769</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>770</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>771</v>
+      </c>
+      <c r="J1" s="53" t="s">
+        <v>674</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>772</v>
+      </c>
+      <c r="L1" s="53" t="s">
+        <v>773</v>
+      </c>
+      <c r="M1" s="53" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="60">
+      <c r="A2" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>775</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>722</v>
+      </c>
+      <c r="E2" s="80" t="s">
+        <v>324</v>
+      </c>
+      <c r="F2" s="82" t="s">
+        <v>776</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="H2" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="I2" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+    </row>
+    <row r="3" spans="1:13" ht="60">
+      <c r="A3" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>777</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>724</v>
+      </c>
+      <c r="E3" s="80" t="s">
+        <v>325</v>
+      </c>
+      <c r="F3" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="H3" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="I3" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="J3" s="77" t="s">
+        <v>778</v>
+      </c>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="56"/>
+    </row>
+    <row r="4" spans="1:13" ht="60">
+      <c r="A4" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>779</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>723</v>
+      </c>
+      <c r="E4" s="80" t="s">
+        <v>326</v>
+      </c>
+      <c r="F4" s="82" t="s">
+        <v>776</v>
+      </c>
+      <c r="G4" s="81"/>
+      <c r="H4" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="I4" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="J4" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K4" s="77" t="s">
+        <v>765</v>
+      </c>
+      <c r="L4" s="77"/>
+      <c r="M4" s="56"/>
+    </row>
+    <row r="5" spans="1:13" ht="60">
+      <c r="A5" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>780</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>723</v>
+      </c>
+      <c r="E5" s="80" t="s">
+        <v>324</v>
+      </c>
+      <c r="F5" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="G5" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="H5" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="I5" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="J5" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K5" s="77" t="s">
+        <v>765</v>
+      </c>
+      <c r="L5" s="77"/>
+      <c r="M5" s="56"/>
+    </row>
+    <row r="6" spans="1:13" ht="60">
+      <c r="A6" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>781</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>723</v>
+      </c>
+      <c r="E6" s="80" t="s">
+        <v>325</v>
+      </c>
+      <c r="F6" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="J6" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77" t="s">
+        <v>782</v>
+      </c>
+      <c r="M6" s="56"/>
+    </row>
+    <row r="7" spans="1:13" ht="60">
+      <c r="A7" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>783</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>723</v>
+      </c>
+      <c r="E7" s="80" t="s">
+        <v>326</v>
+      </c>
+      <c r="F7" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="H7" s="9">
+        <v>123</v>
+      </c>
+      <c r="I7" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="J7" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77" t="s">
+        <v>782</v>
+      </c>
+      <c r="M7" s="56"/>
+    </row>
+    <row r="8" spans="1:13" ht="60">
+      <c r="A8" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>784</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>723</v>
+      </c>
+      <c r="E8" s="80" t="s">
+        <v>324</v>
+      </c>
+      <c r="F8" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="H8" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="60">
+      <c r="A9" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>785</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>723</v>
+      </c>
+      <c r="E9" s="80" t="s">
+        <v>325</v>
+      </c>
+      <c r="F9" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="H9" s="9">
+        <v>12345678</v>
+      </c>
+      <c r="I9" s="9">
+        <v>123</v>
+      </c>
+      <c r="J9" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="60">
+      <c r="A10" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="62" t="s">
+        <v>786</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>723</v>
+      </c>
+      <c r="E10" s="80" t="s">
+        <v>326</v>
+      </c>
+      <c r="F10" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="G10" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="H10" s="9">
+        <v>123</v>
+      </c>
+      <c r="I10" s="9">
+        <v>123</v>
+      </c>
+      <c r="J10" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K10" s="77"/>
+      <c r="L10" s="77" t="s">
+        <v>782</v>
+      </c>
+      <c r="M10" s="77" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="60">
+      <c r="A11" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="62" t="s">
+        <v>787</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>723</v>
+      </c>
+      <c r="E11" s="80" t="s">
+        <v>324</v>
+      </c>
+      <c r="F11" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="G11" s="9">
+        <v>1234567</v>
+      </c>
+      <c r="H11" s="9">
+        <v>123456789</v>
+      </c>
+      <c r="I11" s="9">
+        <v>123456798</v>
+      </c>
+      <c r="J11" s="77" t="s">
+        <v>720</v>
+      </c>
+      <c r="K11" s="77"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="77" t="s">
+        <v>788</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="E11" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E5" r:id="rId7"/>
+    <hyperlink ref="E6" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E8" r:id="rId10"/>
+    <hyperlink ref="E9" r:id="rId11"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId12"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -4431,7 +5520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -4545,7 +5634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -4690,7 +5779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -4831,7 +5920,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="21" t="s">
-        <v>704</v>
+        <v>693</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>11</v>
@@ -4843,13 +5932,13 @@
         <v>118</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>727</v>
+        <v>716</v>
       </c>
       <c r="F5" s="26" t="s">
         <v>71</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>728</v>
+        <v>717</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>73</v>
@@ -4864,7 +5953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -11928,7 +13017,7 @@
         <v>677</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>734</v>
+        <v>721</v>
       </c>
       <c r="E2" s="48" t="s">
         <v>327</v>
@@ -11955,7 +13044,7 @@
         <v>679</v>
       </c>
       <c r="D3" s="62" t="s">
-        <v>735</v>
+        <v>722</v>
       </c>
       <c r="E3" s="48" t="s">
         <v>328</v>
@@ -11964,10 +13053,10 @@
         <v>678</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>738</v>
+        <v>725</v>
       </c>
       <c r="I3" s="56"/>
       <c r="J3" s="56"/>
@@ -11982,7 +13071,7 @@
         <v>679</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>737</v>
+        <v>724</v>
       </c>
       <c r="E4" s="48" t="s">
         <v>329</v>
@@ -11991,13 +13080,13 @@
         <v>678</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>738</v>
-      </c>
-      <c r="I4" s="80" t="s">
-        <v>732</v>
+        <v>725</v>
+      </c>
+      <c r="I4" s="77" t="s">
+        <v>719</v>
       </c>
       <c r="J4" s="56"/>
       <c r="K4" s="56"/>
@@ -12011,7 +13100,7 @@
         <v>680</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>736</v>
+        <v>723</v>
       </c>
       <c r="E5" s="48" t="s">
         <v>330</v>
@@ -12021,10 +13110,10 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>738</v>
-      </c>
-      <c r="I5" s="80" t="s">
-        <v>733</v>
+        <v>725</v>
+      </c>
+      <c r="I5" s="77" t="s">
+        <v>720</v>
       </c>
       <c r="J5" s="56" t="s">
         <v>5</v>
@@ -12040,7 +13129,7 @@
         <v>681</v>
       </c>
       <c r="D6" s="62" t="s">
-        <v>736</v>
+        <v>723</v>
       </c>
       <c r="E6" s="48" t="s">
         <v>331</v>
@@ -12049,11 +13138,11 @@
         <v>678</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
       <c r="H6" s="9"/>
-      <c r="I6" s="80" t="s">
-        <v>733</v>
+      <c r="I6" s="77" t="s">
+        <v>720</v>
       </c>
       <c r="J6" s="56"/>
       <c r="K6" s="56" t="s">
@@ -12069,7 +13158,7 @@
         <v>682</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>736</v>
+        <v>723</v>
       </c>
       <c r="E7" s="48" t="s">
         <v>332</v>
@@ -12079,8 +13168,8 @@
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="80" t="s">
-        <v>733</v>
+      <c r="I7" s="77" t="s">
+        <v>720</v>
       </c>
       <c r="J7" s="56" t="s">
         <v>5</v>
@@ -12098,7 +13187,7 @@
         <v>683</v>
       </c>
       <c r="D8" s="62" t="s">
-        <v>739</v>
+        <v>726</v>
       </c>
       <c r="E8" s="48" t="s">
         <v>333</v>
@@ -12107,13 +13196,13 @@
         <v>678</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>738</v>
-      </c>
-      <c r="I8" s="80" t="s">
-        <v>732</v>
+        <v>725</v>
+      </c>
+      <c r="I8" s="77" t="s">
+        <v>719</v>
       </c>
       <c r="J8" s="56"/>
       <c r="K8" s="56"/>
@@ -12137,10 +13226,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12149,7 +13238,7 @@
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
     <col min="6" max="6" width="45.28515625" style="5" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
@@ -12159,7 +13248,7 @@
     <col min="12" max="13" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="16" t="s">
         <v>128</v>
       </c>
@@ -12170,37 +13259,22 @@
         <v>53</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>143</v>
+        <v>51</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="F1" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="F1" s="16" t="s">
+        <v>684</v>
+      </c>
       <c r="G1" s="16" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>685</v>
-      </c>
-      <c r="I1" s="16" t="s">
         <v>686</v>
       </c>
-      <c r="J1" s="29" t="s">
-        <v>687</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>688</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>689</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:8" ht="45">
       <c r="A2" s="55" t="s">
         <v>129</v>
       </c>
@@ -12208,40 +13282,25 @@
         <v>101</v>
       </c>
       <c r="C2" s="62" t="s">
-        <v>691</v>
-      </c>
-      <c r="D2" s="63" t="s">
+        <v>687</v>
+      </c>
+      <c r="D2" s="87" t="s">
+        <v>323</v>
+      </c>
+      <c r="E2" s="83" t="s">
+        <v>688</v>
+      </c>
+      <c r="F2" s="63" t="s">
+        <v>689</v>
+      </c>
+      <c r="G2" s="63" t="s">
+        <v>690</v>
+      </c>
+      <c r="H2" s="63">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="48" t="s">
-        <v>692</v>
-      </c>
-      <c r="G2" s="64" t="s">
-        <v>693</v>
-      </c>
-      <c r="H2" s="65" t="s">
-        <v>694</v>
-      </c>
-      <c r="I2" s="64" t="s">
-        <v>695</v>
-      </c>
-      <c r="J2" s="66" t="s">
-        <v>696</v>
-      </c>
-      <c r="K2" s="64" t="s">
-        <v>697</v>
-      </c>
-      <c r="L2" s="64" t="s">
-        <v>698</v>
-      </c>
-      <c r="M2" s="64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+    </row>
+    <row r="3" spans="1:8" ht="45">
       <c r="A3" s="55" t="s">
         <v>130</v>
       </c>
@@ -12249,42 +13308,51 @@
         <v>101</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>699</v>
-      </c>
-      <c r="D3" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="48" t="s">
+        <v>691</v>
+      </c>
+      <c r="D3" s="87" t="s">
+        <v>324</v>
+      </c>
+      <c r="E3" s="83" t="s">
+        <v>688</v>
+      </c>
+      <c r="F3" s="63" t="s">
         <v>692</v>
       </c>
-      <c r="G3" s="64" t="s">
-        <v>700</v>
-      </c>
-      <c r="H3" s="64" t="s">
-        <v>701</v>
-      </c>
-      <c r="I3" s="64" t="s">
-        <v>695</v>
-      </c>
-      <c r="J3" s="66" t="s">
-        <v>702</v>
-      </c>
-      <c r="K3" s="64" t="s">
-        <v>703</v>
-      </c>
-      <c r="L3" s="64" t="s">
-        <v>698</v>
-      </c>
-      <c r="M3" s="64">
+      <c r="G3" s="63" t="s">
+        <v>690</v>
+      </c>
+      <c r="H3" s="63">
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:8" ht="45">
+      <c r="A4" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>789</v>
+      </c>
+      <c r="D4" s="88" t="s">
+        <v>790</v>
+      </c>
+      <c r="E4" s="83" t="s">
+        <v>688</v>
+      </c>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -12301,129 +13369,129 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="67"/>
+    <col min="1" max="2" width="9.140625" style="64"/>
     <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="67" customFormat="1">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:5" s="64" customFormat="1">
+      <c r="A1" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="76" t="s">
+      <c r="E1" s="73" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>698</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>699</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="74" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="105">
+      <c r="A4" s="74" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="E4" s="75" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="77" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="77" t="s">
+      <c r="E5" s="7" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="74" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>709</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>710</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="77" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="77" t="s">
+      <c r="E6" s="7" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>712</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>713</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E7" s="75" t="s">
         <v>714</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="105">
-      <c r="A4" s="77" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>715</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>716</v>
-      </c>
-      <c r="E4" s="78" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="77" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>718</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>719</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="77" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>721</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>722</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="77" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>723</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>724</v>
-      </c>
-      <c r="E7" s="78" t="s">
-        <v>725</v>
       </c>
     </row>
   </sheetData>
@@ -12476,7 +13544,7 @@
       <c r="D1" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="65" t="s">
         <v>51</v>
       </c>
       <c r="F1" s="36" t="s">
@@ -12484,102 +13552,102 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="45">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="66" t="s">
         <v>546</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="70" t="s">
         <v>550</v>
       </c>
-      <c r="E2" s="71" t="s">
+      <c r="E2" s="68" t="s">
         <v>323</v>
       </c>
-      <c r="F2" s="72" t="s">
+      <c r="F2" s="69" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="66" t="s">
         <v>546</v>
       </c>
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="70" t="s">
         <v>549</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="E3" s="68" t="s">
         <v>324</v>
       </c>
-      <c r="F3" s="72" t="s">
-        <v>704</v>
+      <c r="F3" s="69" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="69" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="66" t="s">
         <v>546</v>
       </c>
-      <c r="D4" s="73" t="s">
+      <c r="D4" s="70" t="s">
         <v>548</v>
       </c>
-      <c r="E4" s="71" t="s">
+      <c r="E4" s="68" t="s">
         <v>325</v>
       </c>
-      <c r="F4" s="72" t="s">
-        <v>704</v>
+      <c r="F4" s="69" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="66" t="s">
         <v>546</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="70" t="s">
         <v>547</v>
       </c>
-      <c r="E5" s="71" t="s">
+      <c r="E5" s="68" t="s">
         <v>326</v>
       </c>
-      <c r="F5" s="72" t="s">
-        <v>704</v>
+      <c r="F5" s="69" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="69" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="66" t="s">
         <v>546</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="70" t="s">
         <v>545</v>
       </c>
-      <c r="E6" s="71" t="s">
+      <c r="E6" s="68" t="s">
         <v>327</v>
       </c>
-      <c r="F6" s="72" t="s">
+      <c r="F6" s="69" t="s">
         <v>83</v>
       </c>
     </row>
@@ -12608,8 +13676,8 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12632,7 +13700,7 @@
       <c r="C1" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="67" t="s">
         <v>52</v>
       </c>
       <c r="E1" s="30" t="s">
@@ -12665,13 +13733,13 @@
         <v>101</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>729</v>
+        <v>791</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>705</v>
-      </c>
-      <c r="E2" s="79" t="s">
-        <v>706</v>
+        <v>694</v>
+      </c>
+      <c r="E2" s="76" t="s">
+        <v>695</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>237</v>
@@ -12679,16 +13747,16 @@
       <c r="G2" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="74" t="s">
-        <v>704</v>
-      </c>
-      <c r="K2" s="71" t="s">
+      <c r="J2" s="71" t="s">
+        <v>693</v>
+      </c>
+      <c r="K2" s="68" t="s">
         <v>324</v>
       </c>
     </row>
@@ -12700,13 +13768,13 @@
         <v>101</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>730</v>
+        <v>792</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>707</v>
-      </c>
-      <c r="E3" s="79" t="s">
-        <v>706</v>
+        <v>696</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>695</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>237</v>
@@ -12714,16 +13782,16 @@
       <c r="G3" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="74" t="s">
+      <c r="H3" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="74" t="s">
-        <v>704</v>
-      </c>
-      <c r="K3" s="71" t="s">
+      <c r="J3" s="71" t="s">
+        <v>693</v>
+      </c>
+      <c r="K3" s="68" t="s">
         <v>323</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update classpath and driver/ lib locations
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,26 +4,27 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="158775" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="5" activeTab="8"/>
+    <workbookView minimized="1" xWindow="160635" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="5" r:id="rId1"/>
     <sheet name="CheckOutRegression" sheetId="7" r:id="rId2"/>
-    <sheet name="CartRegression" sheetId="18" r:id="rId3"/>
-    <sheet name="PLPRegression" sheetId="21" r:id="rId4"/>
-    <sheet name="PersonalDetailsRegression" sheetId="22" r:id="rId5"/>
-    <sheet name="OrderHistoryRegression" sheetId="23" r:id="rId6"/>
-    <sheet name="RegistrationRegression" sheetId="24" r:id="rId7"/>
-    <sheet name="AddressBookRegression" sheetId="19" r:id="rId8"/>
-    <sheet name="PaymentDetailsRegression" sheetId="25" r:id="rId9"/>
-    <sheet name="StoreLocatorRegression" sheetId="26" r:id="rId10"/>
-    <sheet name="EmailAddressRegression" sheetId="27" r:id="rId11"/>
-    <sheet name="PasswordRegression" sheetId="28" r:id="rId12"/>
-    <sheet name="users" sheetId="13" r:id="rId13"/>
-    <sheet name="products" sheetId="8" r:id="rId14"/>
-    <sheet name="cards" sheetId="9" r:id="rId15"/>
-    <sheet name="addresses" sheetId="10" r:id="rId16"/>
-    <sheet name="users_alternatives" sheetId="20" r:id="rId17"/>
+    <sheet name="PDPRegression" sheetId="29" r:id="rId3"/>
+    <sheet name="CartRegression" sheetId="18" r:id="rId4"/>
+    <sheet name="PLPRegression" sheetId="21" r:id="rId5"/>
+    <sheet name="PersonalDetailsRegression" sheetId="22" r:id="rId6"/>
+    <sheet name="OrderHistoryRegression" sheetId="23" r:id="rId7"/>
+    <sheet name="RegistrationRegression" sheetId="24" r:id="rId8"/>
+    <sheet name="AddressBookRegression" sheetId="19" r:id="rId9"/>
+    <sheet name="PaymentDetailsRegression" sheetId="25" r:id="rId10"/>
+    <sheet name="StoreLocatorRegression" sheetId="26" r:id="rId11"/>
+    <sheet name="EmailAddressRegression" sheetId="27" r:id="rId12"/>
+    <sheet name="PasswordRegression" sheetId="28" r:id="rId13"/>
+    <sheet name="users" sheetId="13" r:id="rId14"/>
+    <sheet name="products" sheetId="8" r:id="rId15"/>
+    <sheet name="cards" sheetId="9" r:id="rId16"/>
+    <sheet name="addresses" sheetId="10" r:id="rId17"/>
+    <sheet name="users_alternatives" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2915" uniqueCount="800">
   <si>
     <t>aa@gg.cc</t>
   </si>
@@ -2492,6 +2493,35 @@
   </si>
   <si>
     <t>Add a new payment through checkout then delete it from payment page</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>https://hybrisdemo.conexus.co.uk:9002/yacceleratorstorefront/en/Brands/Toko/Snowboard-Ski-Tool-Toko-Waxremover-HC3-500ml/p/45572?site=apparel-uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guest, verify the PDP basics </t>
+  </si>
+  <si>
+    <t>id
+name
+price
+summary
+desc
+stock level indicator add to cart button
+share link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get reviews
+</t>
+  </si>
+  <si>
+    <t>max number of prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product size 
+product color </t>
   </si>
 </sst>
 </file>
@@ -3585,6 +3615,142 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>694</v>
+      </c>
+      <c r="E2" s="76" t="s">
+        <v>695</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="71" t="s">
+        <v>693</v>
+      </c>
+      <c r="K2" s="68" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>792</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>696</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>695</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" s="71" t="s">
+        <v>693</v>
+      </c>
+      <c r="K3" s="68" t="s">
+        <v>323</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -3666,7 +3832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -4152,7 +4318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -4598,7 +4764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -5520,15 +5686,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5628,13 +5794,26 @@
         <v>268</v>
       </c>
     </row>
+    <row r="7" spans="1:5" ht="75">
+      <c r="A7" s="27" t="s">
+        <v>793</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>794</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="40" t="s">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -5779,7 +5958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -5953,7 +6132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -11872,6 +12051,183 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="120">
+      <c r="A2" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>796</v>
+      </c>
+      <c r="E2" s="80"/>
+      <c r="F2" s="56"/>
+    </row>
+    <row r="3" spans="1:6" ht="30">
+      <c r="A3" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62" t="s">
+        <v>797</v>
+      </c>
+      <c r="E3" s="80"/>
+      <c r="F3" s="77"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62" t="s">
+        <v>798</v>
+      </c>
+      <c r="E4" s="80"/>
+      <c r="F4" s="77"/>
+    </row>
+    <row r="5" spans="1:6" ht="30">
+      <c r="A5" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62" t="s">
+        <v>799</v>
+      </c>
+      <c r="E5" s="80"/>
+      <c r="F5" s="77"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="77"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="77"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="77"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="77"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="77"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="77"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -12602,7 +12958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -12945,7 +13301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -13221,7 +13577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -13356,7 +13712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -13512,7 +13868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -13667,140 +14023,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId11"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="8" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1:K3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>791</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>694</v>
-      </c>
-      <c r="E2" s="76" t="s">
-        <v>695</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>237</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="71" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="71" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" s="71" t="s">
-        <v>693</v>
-      </c>
-      <c r="K2" s="68" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>792</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>696</v>
-      </c>
-      <c r="E3" s="76" t="s">
-        <v>695</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>237</v>
-      </c>
-      <c r="G3" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="71" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="71" t="s">
-        <v>82</v>
-      </c>
-      <c r="J3" s="71" t="s">
-        <v>693</v>
-      </c>
-      <c r="K3" s="68" t="s">
-        <v>323</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added PDP tests, common fix
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="160635" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="165285" yWindow="0" windowWidth="16980" windowHeight="7020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="5" r:id="rId1"/>
@@ -22,9 +22,10 @@
     <sheet name="PasswordRegression" sheetId="28" r:id="rId13"/>
     <sheet name="users" sheetId="13" r:id="rId14"/>
     <sheet name="products" sheetId="8" r:id="rId15"/>
-    <sheet name="cards" sheetId="9" r:id="rId16"/>
-    <sheet name="addresses" sheetId="10" r:id="rId17"/>
-    <sheet name="users_alternatives" sheetId="20" r:id="rId18"/>
+    <sheet name="products_back" sheetId="31" r:id="rId16"/>
+    <sheet name="cards" sheetId="9" r:id="rId17"/>
+    <sheet name="addresses" sheetId="10" r:id="rId18"/>
+    <sheet name="users_alternatives" sheetId="20" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2915" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2958" uniqueCount="821">
   <si>
     <t>aa@gg.cc</t>
   </si>
@@ -2522,6 +2523,69 @@
   <si>
     <t xml:space="preserve">product size 
 product color </t>
+  </si>
+  <si>
+    <t>Guest, verify reviews</t>
+  </si>
+  <si>
+    <t>Guest, verify max number of products</t>
+  </si>
+  <si>
+    <t>Guest, verify product veriants</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>reviews</t>
+  </si>
+  <si>
+    <t>Summary: Snowboard Ski Tool Toko Waxremover HC3 500ml</t>
+  </si>
+  <si>
+    <t>£12.86</t>
+  </si>
+  <si>
+    <t>Description: Snowboard Ski Tool Toko Waxremover HC3 500ml</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>Snowboard Ski Tool Toko Waxremover HC3 500ml</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>300613491</t>
+  </si>
+  <si>
+    <t>300046037</t>
+  </si>
+  <si>
+    <t>300046592</t>
+  </si>
+  <si>
+    <t>Seizure Satchel brown Uni</t>
+  </si>
+  <si>
+    <t>T-Shirt Men Playboard Flower SS black M</t>
+  </si>
+  <si>
+    <t>118514</t>
+  </si>
+  <si>
+    <t>Avionics Shades Black</t>
+  </si>
+  <si>
+    <t>Shades Fox The Duncan polished black grey</t>
   </si>
 </sst>
 </file>
@@ -2587,7 +2651,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2723,6 +2787,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2731,7 +2808,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2976,6 +3053,28 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3326,8 +3425,8 @@
   </sheetPr>
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5691,10 +5790,238 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>804</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="89" t="s">
+        <v>803</v>
+      </c>
+      <c r="I1" s="89" t="s">
+        <v>667</v>
+      </c>
+      <c r="J1" s="89" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="89" t="s">
+        <v>805</v>
+      </c>
+      <c r="L1" s="89" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="60">
+      <c r="A2" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>816</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+    </row>
+    <row r="3" spans="1:12" ht="60">
+      <c r="A3" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>814</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>817</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+    </row>
+    <row r="4" spans="1:12" ht="60">
+      <c r="A4" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>818</v>
+      </c>
+      <c r="C4" s="69" t="s">
+        <v>819</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>260</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+    </row>
+    <row r="5" spans="1:12" ht="60">
+      <c r="A5" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>815</v>
+      </c>
+      <c r="C5" s="69" t="s">
+        <v>820</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>238</v>
+      </c>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+    </row>
+    <row r="6" spans="1:12" ht="60">
+      <c r="A6" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>818</v>
+      </c>
+      <c r="C6" s="69" t="s">
+        <v>819</v>
+      </c>
+      <c r="D6" s="92" t="s">
+        <v>260</v>
+      </c>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="91" t="s">
+        <v>268</v>
+      </c>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="90"/>
+    </row>
+    <row r="7" spans="1:12" ht="75">
+      <c r="A7" s="40" t="s">
+        <v>793</v>
+      </c>
+      <c r="B7" s="33">
+        <v>45572</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>810</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>794</v>
+      </c>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="40" t="s">
+        <v>268</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>806</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>807</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>808</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="L7" s="33" t="s">
+        <v>811</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF002060"/>
+  </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5813,7 +6140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -5958,7 +6285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -6132,7 +6459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -12051,10 +12378,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12063,11 +12390,12 @@
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="16" t="s">
         <v>128</v>
       </c>
@@ -12081,141 +12409,84 @@
         <v>52</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>812</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="G1" s="53" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="120">
+    <row r="2" spans="1:7" ht="120">
       <c r="A2" s="55" t="s">
         <v>129</v>
       </c>
       <c r="B2" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="93" t="s">
         <v>795</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="93" t="s">
         <v>796</v>
       </c>
-      <c r="E2" s="80"/>
-      <c r="F2" s="56"/>
-    </row>
-    <row r="3" spans="1:6" ht="30">
+      <c r="E2" s="93" t="s">
+        <v>793</v>
+      </c>
+      <c r="F2" s="94"/>
+      <c r="G2" s="95"/>
+    </row>
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="93" t="s">
+        <v>800</v>
+      </c>
+      <c r="D3" s="93" t="s">
         <v>797</v>
       </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="77"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" s="93" t="s">
+        <v>793</v>
+      </c>
+      <c r="F3" s="94"/>
+      <c r="G3" s="96"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62" t="s">
+      <c r="B4" s="55"/>
+      <c r="C4" s="93" t="s">
+        <v>801</v>
+      </c>
+      <c r="D4" s="93" t="s">
         <v>798</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="77"/>
-    </row>
-    <row r="5" spans="1:6" ht="30">
+      <c r="E4" s="93" t="s">
+        <v>793</v>
+      </c>
+      <c r="F4" s="94"/>
+      <c r="G4" s="96"/>
+    </row>
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62" t="s">
+      <c r="B5" s="55"/>
+      <c r="C5" s="93" t="s">
+        <v>802</v>
+      </c>
+      <c r="D5" s="93" t="s">
         <v>799</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="77"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="77"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="55" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="77"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="55" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="77"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="55" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="77"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="55" t="s">
-        <v>138</v>
-      </c>
-      <c r="B10" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="77"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="55" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="77"/>
+      <c r="E5" s="93" t="s">
+        <v>793</v>
+      </c>
+      <c r="F5" s="94"/>
+      <c r="G5" s="96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13585,7 +13856,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added PDP tests T1
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="165285" yWindow="0" windowWidth="16980" windowHeight="7020" activeTab="2"/>
+    <workbookView xWindow="166215" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="5" r:id="rId1"/>
@@ -2505,87 +2505,86 @@
     <t xml:space="preserve">Guest, verify the PDP basics </t>
   </si>
   <si>
+    <t xml:space="preserve">get reviews
+</t>
+  </si>
+  <si>
+    <t>max number of prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product size 
+product color </t>
+  </si>
+  <si>
+    <t>Guest, verify reviews</t>
+  </si>
+  <si>
+    <t>Guest, verify max number of products</t>
+  </si>
+  <si>
+    <t>Guest, verify product veriants</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>reviews</t>
+  </si>
+  <si>
+    <t>Summary: Snowboard Ski Tool Toko Waxremover HC3 500ml</t>
+  </si>
+  <si>
+    <t>£12.86</t>
+  </si>
+  <si>
+    <t>Description: Snowboard Ski Tool Toko Waxremover HC3 500ml</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>Snowboard Ski Tool Toko Waxremover HC3 500ml</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>300613491</t>
+  </si>
+  <si>
+    <t>300046037</t>
+  </si>
+  <si>
+    <t>300046592</t>
+  </si>
+  <si>
+    <t>Seizure Satchel brown Uni</t>
+  </si>
+  <si>
+    <t>T-Shirt Men Playboard Flower SS black M</t>
+  </si>
+  <si>
+    <t>118514</t>
+  </si>
+  <si>
+    <t>Avionics Shades Black</t>
+  </si>
+  <si>
+    <t>Shades Fox The Duncan polished black grey</t>
+  </si>
+  <si>
     <t>id
 name
 price
 summary
 desc
-stock level indicator add to cart button
-share link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">get reviews
-</t>
-  </si>
-  <si>
-    <t>max number of prod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product size 
-product color </t>
-  </si>
-  <si>
-    <t>Guest, verify reviews</t>
-  </si>
-  <si>
-    <t>Guest, verify max number of products</t>
-  </si>
-  <si>
-    <t>Guest, verify product veriants</t>
-  </si>
-  <si>
-    <t>summary</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>reviews</t>
-  </si>
-  <si>
-    <t>Summary: Snowboard Ski Tool Toko Waxremover HC3 500ml</t>
-  </si>
-  <si>
-    <t>£12.86</t>
-  </si>
-  <si>
-    <t>Description: Snowboard Ski Tool Toko Waxremover HC3 500ml</t>
-  </si>
-  <si>
-    <t>rating</t>
-  </si>
-  <si>
-    <t>Snowboard Ski Tool Toko Waxremover HC3 500ml</t>
-  </si>
-  <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>300613491</t>
-  </si>
-  <si>
-    <t>300046037</t>
-  </si>
-  <si>
-    <t>300046592</t>
-  </si>
-  <si>
-    <t>Seizure Satchel brown Uni</t>
-  </si>
-  <si>
-    <t>T-Shirt Men Playboard Flower SS black M</t>
-  </si>
-  <si>
-    <t>118514</t>
-  </si>
-  <si>
-    <t>Avionics Shades Black</t>
-  </si>
-  <si>
-    <t>Shades Fox The Duncan polished black grey</t>
+stock level indicator add to cart button</t>
   </si>
 </sst>
 </file>
@@ -5793,7 +5792,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5812,7 +5811,7 @@
         <v>44</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C1" s="36" t="s">
         <v>117</v>
@@ -5830,7 +5829,7 @@
         <v>48</v>
       </c>
       <c r="H1" s="89" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="I1" s="89" t="s">
         <v>667</v>
@@ -5839,10 +5838,10 @@
         <v>53</v>
       </c>
       <c r="K1" s="89" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="L1" s="89" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="60">
@@ -5850,10 +5849,10 @@
         <v>40</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>110</v>
@@ -5878,10 +5877,10 @@
         <v>47</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C3" s="69" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D3" s="52" t="s">
         <v>114</v>
@@ -5906,10 +5905,10 @@
         <v>113</v>
       </c>
       <c r="B4" s="27" t="s">
+        <v>817</v>
+      </c>
+      <c r="C4" s="69" t="s">
         <v>818</v>
-      </c>
-      <c r="C4" s="69" t="s">
-        <v>819</v>
       </c>
       <c r="D4" s="52" t="s">
         <v>260</v>
@@ -5930,10 +5929,10 @@
         <v>237</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C5" s="69" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D5" s="52" t="s">
         <v>238</v>
@@ -5954,10 +5953,10 @@
         <v>267</v>
       </c>
       <c r="B6" s="27" t="s">
+        <v>817</v>
+      </c>
+      <c r="C6" s="69" t="s">
         <v>818</v>
-      </c>
-      <c r="C6" s="69" t="s">
-        <v>819</v>
       </c>
       <c r="D6" s="92" t="s">
         <v>260</v>
@@ -5981,7 +5980,7 @@
         <v>45572</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D7" s="52" t="s">
         <v>794</v>
@@ -5992,19 +5991,19 @@
         <v>268</v>
       </c>
       <c r="H7" s="37" t="s">
+        <v>805</v>
+      </c>
+      <c r="I7" s="33" t="s">
         <v>806</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="J7" s="37" t="s">
         <v>807</v>
-      </c>
-      <c r="J7" s="37" t="s">
-        <v>808</v>
       </c>
       <c r="K7" s="33" t="s">
         <v>235</v>
       </c>
       <c r="L7" s="33" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
   </sheetData>
@@ -12381,7 +12380,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12409,7 +12408,7 @@
         <v>52</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>51</v>
@@ -12418,7 +12417,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120">
+    <row r="2" spans="1:7" ht="105">
       <c r="A2" s="55" t="s">
         <v>129</v>
       </c>
@@ -12429,7 +12428,7 @@
         <v>795</v>
       </c>
       <c r="D2" s="93" t="s">
-        <v>796</v>
+        <v>820</v>
       </c>
       <c r="E2" s="93" t="s">
         <v>793</v>
@@ -12443,10 +12442,10 @@
       </c>
       <c r="B3" s="55"/>
       <c r="C3" s="93" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D3" s="93" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E3" s="93" t="s">
         <v>793</v>
@@ -12460,10 +12459,10 @@
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="93" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D4" s="93" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E4" s="93" t="s">
         <v>793</v>
@@ -12477,10 +12476,10 @@
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="93" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D5" s="93" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E5" s="93" t="s">
         <v>793</v>

</xml_diff>

<commit_message>
checkout negative cases fixes
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="182985" yWindow="0" windowWidth="16980" windowHeight="7020"/>
+    <workbookView xWindow="183915" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="AccountSetupRegression" sheetId="37" r:id="rId1"/>
@@ -3756,7 +3756,7 @@
   </sheetPr>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
@@ -5779,17 +5779,22 @@
   </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="10" max="11" width="37.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="32.85546875" customWidth="1"/>
+    <col min="11" max="11" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>93</v>
       </c>
@@ -5824,7 +5829,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="90">
+    <row r="2" spans="1:11" ht="45">
       <c r="A2" s="56" t="s">
         <v>94</v>
       </c>
@@ -5859,7 +5864,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="90">
+    <row r="3" spans="1:11" ht="45">
       <c r="A3" s="56" t="s">
         <v>95</v>
       </c>
@@ -5894,7 +5899,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="105">
+    <row r="4" spans="1:11" ht="45">
       <c r="A4" s="56" t="s">
         <v>96</v>
       </c>
@@ -5929,7 +5934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="90">
+    <row r="5" spans="1:11" ht="45">
       <c r="A5" s="56" t="s">
         <v>97</v>
       </c>
@@ -5964,7 +5969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="90">
+    <row r="6" spans="1:11" ht="45">
       <c r="A6" s="56" t="s">
         <v>98</v>
       </c>
@@ -5999,7 +6004,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="90">
+    <row r="7" spans="1:11" ht="45">
       <c r="A7" s="56" t="s">
         <v>99</v>
       </c>
@@ -6034,7 +6039,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="60">
+    <row r="8" spans="1:11" ht="45">
       <c r="A8" s="56" t="s">
         <v>100</v>
       </c>
@@ -6069,7 +6074,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="90">
+    <row r="9" spans="1:11" ht="45">
       <c r="A9" s="56" t="s">
         <v>101</v>
       </c>
@@ -6104,7 +6109,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="90">
+    <row r="10" spans="1:11" ht="45">
       <c r="A10" s="56" t="s">
         <v>103</v>
       </c>
@@ -6139,7 +6144,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="90">
+    <row r="11" spans="1:11" ht="45">
       <c r="A11" s="56" t="s">
         <v>104</v>
       </c>
@@ -6174,7 +6179,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="90">
+    <row r="12" spans="1:11" ht="45">
       <c r="A12" s="56" t="s">
         <v>106</v>
       </c>
@@ -6209,7 +6214,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="90">
+    <row r="13" spans="1:11" ht="45">
       <c r="A13" s="56" t="s">
         <v>129</v>
       </c>
@@ -6244,7 +6249,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="90">
+    <row r="14" spans="1:11" ht="45">
       <c r="A14" s="56" t="s">
         <v>130</v>
       </c>
@@ -6279,7 +6284,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="90">
+    <row r="15" spans="1:11" ht="45">
       <c r="A15" s="56" t="s">
         <v>131</v>
       </c>

</xml_diff>

<commit_message>
visual testing home page
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="188580" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="189510" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="16" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="AccountSetupRegression" sheetId="37" r:id="rId1"/>
@@ -27,10 +27,11 @@
     <sheet name="PasswordRegression" sheetId="28" r:id="rId18"/>
     <sheet name="MailSignupRegression" sheetId="38" r:id="rId19"/>
     <sheet name="QuickViewRegression" sheetId="39" r:id="rId20"/>
-    <sheet name="users" sheetId="13" r:id="rId21"/>
-    <sheet name="products" sheetId="8" r:id="rId22"/>
-    <sheet name="cards" sheetId="9" r:id="rId23"/>
-    <sheet name="addresses" sheetId="10" r:id="rId24"/>
+    <sheet name="VisualTestingHPRegression" sheetId="40" r:id="rId21"/>
+    <sheet name="users" sheetId="13" r:id="rId22"/>
+    <sheet name="products" sheetId="8" r:id="rId23"/>
+    <sheet name="cards" sheetId="9" r:id="rId24"/>
+    <sheet name="addresses" sheetId="10" r:id="rId25"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2380" uniqueCount="719">
   <si>
     <t>Please enter a valid email</t>
   </si>
@@ -2237,6 +2238,57 @@
     <t xml:space="preserve">loggedin
 product size 
 product color </t>
+  </si>
+  <si>
+    <t>check header guest</t>
+  </si>
+  <si>
+    <t>check footer guest</t>
+  </si>
+  <si>
+    <t>check body guest</t>
+  </si>
+  <si>
+    <t>QV5</t>
+  </si>
+  <si>
+    <t>QV6</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>HP_Header</t>
+  </si>
+  <si>
+    <t>HP_Footer</t>
+  </si>
+  <si>
+    <t>HP_Body</t>
+  </si>
+  <si>
+    <t>update
+herader</t>
+  </si>
+  <si>
+    <t>update
+footer</t>
+  </si>
+  <si>
+    <t>update
+body</t>
+  </si>
+  <si>
+    <t>verify
+header</t>
+  </si>
+  <si>
+    <t>verify
+footer</t>
+  </si>
+  <si>
+    <t>verify
+body</t>
   </si>
 </sst>
 </file>
@@ -8244,12 +8296,151 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="89" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30">
+      <c r="A2" s="53" t="s">
+        <v>693</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>704</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>716</v>
+      </c>
+      <c r="E2" s="90" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" s="53" t="s">
+        <v>694</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>705</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>717</v>
+      </c>
+      <c r="E3" s="91" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30">
+      <c r="A4" s="53" t="s">
+        <v>695</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>706</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>718</v>
+      </c>
+      <c r="E4" s="90" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30">
+      <c r="A5" s="53" t="s">
+        <v>696</v>
+      </c>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53" t="s">
+        <v>704</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>713</v>
+      </c>
+      <c r="E5" s="90" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30">
+      <c r="A6" s="53" t="s">
+        <v>707</v>
+      </c>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53" t="s">
+        <v>705</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>714</v>
+      </c>
+      <c r="E6" s="91" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" s="53" t="s">
+        <v>708</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53" t="s">
+        <v>706</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>715</v>
+      </c>
+      <c r="E7" s="90" t="s">
+        <v>712</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet19">
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -9762,7 +9953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet20">
     <tabColor rgb="FF002060"/>
@@ -10016,7 +10207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet22">
     <tabColor rgb="FF002060"/>
@@ -10161,7 +10352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet23">
     <tabColor rgb="FF002060"/>
@@ -11916,7 +12107,7 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
missing case from checkout
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="194160" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="17" activeTab="20"/>
+    <workbookView xWindow="204390" yWindow="0" windowWidth="16980" windowHeight="7020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AccountSetupRegression" sheetId="37" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2585" uniqueCount="772">
   <si>
     <t>Please enter a valid email</t>
   </si>
@@ -2345,6 +2345,114 @@
   <si>
     <t>update
 header</t>
+  </si>
+  <si>
+    <t>COB-39</t>
+  </si>
+  <si>
+    <t>login during checkout</t>
+  </si>
+  <si>
+    <t>logging During Checkout
+old-user
+new-shipping
+new-payment</t>
+  </si>
+  <si>
+    <t>AC-38</t>
+  </si>
+  <si>
+    <t>AC-39</t>
+  </si>
+  <si>
+    <t>AC-40</t>
+  </si>
+  <si>
+    <t>AC-41</t>
+  </si>
+  <si>
+    <t>AC-42</t>
+  </si>
+  <si>
+    <t>AC-43</t>
+  </si>
+  <si>
+    <t>AC-44</t>
+  </si>
+  <si>
+    <t>AC-45</t>
+  </si>
+  <si>
+    <t>AC-46</t>
+  </si>
+  <si>
+    <t>AC-47</t>
+  </si>
+  <si>
+    <t>tester147@ACVtesting.com</t>
+  </si>
+  <si>
+    <t>tester148@ACVtesting.com</t>
+  </si>
+  <si>
+    <t>tester149@ACVtesting.com</t>
+  </si>
+  <si>
+    <t>tester151@ACVtesting.com</t>
+  </si>
+  <si>
+    <t>tester152@ACVtesting.com</t>
+  </si>
+  <si>
+    <t>tester153@ACVtesting.com</t>
+  </si>
+  <si>
+    <t>tester154@ACVtesting.com</t>
+  </si>
+  <si>
+    <t>tester155@ACVtesting.com</t>
+  </si>
+  <si>
+    <t>tester156@ACVtesting.com</t>
+  </si>
+  <si>
+    <t>tester157@ACVtesting.com</t>
+  </si>
+  <si>
+    <t>tester150@ACVtesting.com</t>
+  </si>
+  <si>
+    <t>U78</t>
+  </si>
+  <si>
+    <t>U79</t>
+  </si>
+  <si>
+    <t>U80</t>
+  </si>
+  <si>
+    <t>U81</t>
+  </si>
+  <si>
+    <t>U82</t>
+  </si>
+  <si>
+    <t>U83</t>
+  </si>
+  <si>
+    <t>U84</t>
+  </si>
+  <si>
+    <t>U85</t>
+  </si>
+  <si>
+    <t>U86</t>
+  </si>
+  <si>
+    <t>U87</t>
+  </si>
+  <si>
+    <t>U88</t>
   </si>
 </sst>
 </file>
@@ -2558,7 +2666,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2818,6 +2926,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3165,10 +3277,10 @@
   <sheetPr codeName="Sheet25">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView topLeftCell="A11" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3211,9 +3323,7 @@
       <c r="A2" s="19" t="s">
         <v>604</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B2" s="19"/>
       <c r="C2" s="23" t="s">
         <v>168</v>
       </c>
@@ -3285,9 +3395,7 @@
       <c r="A5" s="19" t="s">
         <v>607</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B5" s="19"/>
       <c r="C5" s="23" t="s">
         <v>78</v>
       </c>
@@ -3311,9 +3419,7 @@
       <c r="A6" s="19" t="s">
         <v>608</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B6" s="19"/>
       <c r="C6" s="23" t="s">
         <v>78</v>
       </c>
@@ -3337,9 +3443,7 @@
       <c r="A7" s="19" t="s">
         <v>609</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B7" s="19"/>
       <c r="C7" s="23" t="s">
         <v>78</v>
       </c>
@@ -3579,9 +3683,7 @@
       <c r="A17" s="19" t="s">
         <v>619</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B17" s="19"/>
       <c r="C17" s="23" t="s">
         <v>78</v>
       </c>
@@ -3725,9 +3827,7 @@
       <c r="A23" s="19" t="s">
         <v>625</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B23" s="19"/>
       <c r="C23" s="23" t="s">
         <v>78</v>
       </c>
@@ -3751,9 +3851,7 @@
       <c r="A24" s="19" t="s">
         <v>626</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B24" s="19"/>
       <c r="C24" s="23" t="s">
         <v>78</v>
       </c>
@@ -3777,9 +3875,7 @@
       <c r="A25" s="19" t="s">
         <v>627</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B25" s="19"/>
       <c r="C25" s="23" t="s">
         <v>78</v>
       </c>
@@ -3803,9 +3899,7 @@
       <c r="A26" s="19" t="s">
         <v>628</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B26" s="19"/>
       <c r="C26" s="23" t="s">
         <v>78</v>
       </c>
@@ -3973,9 +4067,7 @@
       <c r="A33" s="19" t="s">
         <v>635</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B33" s="19"/>
       <c r="C33" s="23" t="s">
         <v>78</v>
       </c>
@@ -4112,12 +4204,257 @@
         <v>47</v>
       </c>
       <c r="H38" s="38" t="s">
-        <v>677</v>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H39" s="37" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="19" t="s">
+        <v>741</v>
+      </c>
+      <c r="B40" s="19"/>
+      <c r="C40" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H40" s="37" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="19" t="s">
+        <v>742</v>
+      </c>
+      <c r="B41" s="19"/>
+      <c r="C41" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H41" s="94" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="19" t="s">
+        <v>743</v>
+      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H42" s="37" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="19" t="s">
+        <v>744</v>
+      </c>
+      <c r="B43" s="19"/>
+      <c r="C43" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H43" s="37" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="19" t="s">
+        <v>745</v>
+      </c>
+      <c r="B44" s="19"/>
+      <c r="C44" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H44" s="37" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="B45" s="19"/>
+      <c r="C45" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H45" s="37" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="19" t="s">
+        <v>747</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H46" s="37" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="19" t="s">
+        <v>748</v>
+      </c>
+      <c r="B47" s="19"/>
+      <c r="C47" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H47" s="37" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="19" t="s">
+        <v>749</v>
+      </c>
+      <c r="B48" s="19"/>
+      <c r="C48" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H48" s="37" t="s">
+        <v>759</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H41" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7008,16 +7345,16 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -7099,9 +7436,7 @@
       <c r="A3" s="19" t="s">
         <v>544</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B3" s="19"/>
       <c r="C3" s="22" t="s">
         <v>109</v>
       </c>
@@ -7132,9 +7467,7 @@
       <c r="A4" s="19" t="s">
         <v>545</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B4" s="19"/>
       <c r="C4" s="22" t="s">
         <v>24</v>
       </c>
@@ -7198,9 +7531,7 @@
       <c r="A6" s="19" t="s">
         <v>547</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B6" s="19"/>
       <c r="C6" s="22" t="s">
         <v>109</v>
       </c>
@@ -7564,7 +7895,9 @@
       <c r="A18" s="19" t="s">
         <v>559</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="C18" s="22" t="s">
         <v>118</v>
       </c>
@@ -8081,7 +8414,9 @@
       <c r="A35" s="19" t="s">
         <v>576</v>
       </c>
-      <c r="B35" s="19"/>
+      <c r="B35" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="C35" s="22" t="s">
         <v>125</v>
       </c>
@@ -8222,9 +8557,45 @@
       <c r="J39" s="24"/>
       <c r="K39" s="37"/>
     </row>
+    <row r="40" spans="1:11" ht="60">
+      <c r="A40" s="19" t="s">
+        <v>737</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>738</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>739</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J40" s="24"/>
+      <c r="K40" s="93" t="s">
+        <v>665</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K40" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8360,7 +8731,7 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -8734,10 +9105,10 @@
   <sheetPr codeName="Sheet19">
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="N27" sqref="M27:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8748,7 +9119,7 @@
     <col min="7" max="7" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1">
+    <row r="1" spans="1:7">
       <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
@@ -10243,9 +10614,265 @@
         <v>677</v>
       </c>
     </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="30" t="s">
+        <v>761</v>
+      </c>
+      <c r="B66" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C66" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D66" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G66" s="38" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="30" t="s">
+        <v>762</v>
+      </c>
+      <c r="B67" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C67" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G67" s="37" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="30" t="s">
+        <v>763</v>
+      </c>
+      <c r="B68" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C68" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G68" s="37" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="30" t="s">
+        <v>764</v>
+      </c>
+      <c r="B69" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D69" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F69" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G69" s="94" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="30" t="s">
+        <v>765</v>
+      </c>
+      <c r="B70" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D70" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G70" s="37" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="30" t="s">
+        <v>766</v>
+      </c>
+      <c r="B71" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F71" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G71" s="37" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="30" t="s">
+        <v>767</v>
+      </c>
+      <c r="B72" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C72" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F72" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G72" s="37" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="30" t="s">
+        <v>768</v>
+      </c>
+      <c r="B73" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D73" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G73" s="37" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="30" t="s">
+        <v>769</v>
+      </c>
+      <c r="B74" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D74" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G74" s="37" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="30" t="s">
+        <v>770</v>
+      </c>
+      <c r="B75" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C75" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E75" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F75" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G75" s="37" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="30" t="s">
+        <v>771</v>
+      </c>
+      <c r="B76" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C76" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D76" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F76" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G76" s="37" t="s">
+        <v>759</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G69" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
edge/ IE/ grid support
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="206250" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="18" activeTab="23"/>
+    <workbookView xWindow="208110" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="AccountSetupRegression" sheetId="37" r:id="rId1"/>
@@ -4587,8 +4587,8 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9107,7 +9107,7 @@
   </sheetPr>
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
round1: tweak page/ selectors
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="214620" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="216480" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="AccountSetupRegression" sheetId="37" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2580" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2575" uniqueCount="775">
   <si>
     <t>Please enter a valid email</t>
   </si>
@@ -11386,7 +11386,7 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -13012,8 +13012,8 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13062,9 +13062,7 @@
       <c r="A3" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="58" t="s">
-        <v>64</v>
-      </c>
+      <c r="B3" s="58"/>
       <c r="C3" s="5" t="s">
         <v>362</v>
       </c>
@@ -13079,9 +13077,7 @@
       <c r="A4" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="58" t="s">
-        <v>64</v>
-      </c>
+      <c r="B4" s="58"/>
       <c r="C4" s="5" t="s">
         <v>365</v>
       </c>
@@ -13096,9 +13092,7 @@
       <c r="A5" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="58" t="s">
-        <v>64</v>
-      </c>
+      <c r="B5" s="58"/>
       <c r="C5" s="5" t="s">
         <v>368</v>
       </c>
@@ -13113,9 +13107,7 @@
       <c r="A6" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="58" t="s">
-        <v>64</v>
-      </c>
+      <c r="B6" s="58"/>
       <c r="C6" s="5" t="s">
         <v>371</v>
       </c>
@@ -13130,9 +13122,7 @@
       <c r="A7" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="58" t="s">
-        <v>64</v>
-      </c>
+      <c r="B7" s="58"/>
       <c r="C7" s="5" t="s">
         <v>373</v>
       </c>

</xml_diff>

<commit_message>
round 3 tweak sheet 2
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="217410" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="218340" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="AccountSetupRegression" sheetId="37" r:id="rId1"/>
@@ -1184,9 +1184,6 @@
     <t>existingUser</t>
   </si>
   <si>
-    <t>invalidEmail:An account already exists for this email address.</t>
-  </si>
-  <si>
     <t>Try to register without filling data.</t>
   </si>
   <si>
@@ -2441,24 +2438,27 @@
     <t>Guest, verify the PDP basics add to cart button</t>
   </si>
   <si>
-    <t>firstNameError:Please enter a First Name
-lastNameError:Please enter a Last Name
-invalidEmail:Please enter an Email Address
-passwordError:Please enter a Password
-confirmPasswordError:Please enter a Password Again</t>
-  </si>
-  <si>
-    <t>invalidEmail:Please enter valid email address.</t>
-  </si>
-  <si>
-    <t>passwordMismatchError:The Password and Confirmation Password do not match</t>
-  </si>
-  <si>
-    <t>passwordError:Please enter a strong Password of at least 6 characters
-confirmPasswordError:The Password and Confirmation Password do not match</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thank you for registering. </t>
+    <t xml:space="preserve">ThankyouValidation: Thank you for registering. </t>
+  </si>
+  <si>
+    <t>EmailValidation:An account already exists for this email address.</t>
+  </si>
+  <si>
+    <t>firstNameValidation:Please enter a First Name
+lastNameValidation:Please enter a Last Name
+EmailValidation:Please enter an Email Address
+PasswordValidation:Please enter a Password
+PasswordConfValidation:Please enter a Password Again</t>
+  </si>
+  <si>
+    <t>EmailValidation:Please enter valid email address.</t>
+  </si>
+  <si>
+    <t>PasswordConfValidation:The Password and Confirmation Password do not match</t>
+  </si>
+  <si>
+    <t>PasswordValidation:Please enter a strong Password of at least 6 characters
+PasswordConfValidation:The Password and Confirmation Password do not match</t>
   </si>
 </sst>
 </file>
@@ -2672,7 +2672,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2950,6 +2950,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3342,7 +3351,7 @@
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1">
       <c r="A2" s="19" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="23" t="s">
@@ -3361,12 +3370,12 @@
         <v>45</v>
       </c>
       <c r="H2" s="86" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1">
       <c r="A3" s="19" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="23" t="s">
@@ -3385,12 +3394,12 @@
         <v>46</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1">
       <c r="A4" s="19" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="23" t="s">
@@ -3409,12 +3418,12 @@
         <v>45</v>
       </c>
       <c r="H4" s="38" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1">
       <c r="A5" s="19" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="23" t="s">
@@ -3433,12 +3442,12 @@
         <v>45</v>
       </c>
       <c r="H5" s="38" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1">
       <c r="A6" s="19" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="23" t="s">
@@ -3457,12 +3466,12 @@
         <v>46</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1">
       <c r="A7" s="19" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="23" t="s">
@@ -3481,12 +3490,12 @@
         <v>45</v>
       </c>
       <c r="H7" s="38" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1">
       <c r="A8" s="19" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="23" t="s">
@@ -3505,12 +3514,12 @@
         <v>45</v>
       </c>
       <c r="H8" s="38" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1">
       <c r="A9" s="19" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="23" t="s">
@@ -3529,12 +3538,12 @@
         <v>46</v>
       </c>
       <c r="H9" s="38" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="19" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="23" t="s">
@@ -3553,12 +3562,12 @@
         <v>45</v>
       </c>
       <c r="H10" s="38" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1">
       <c r="A11" s="19" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="23" t="s">
@@ -3577,12 +3586,12 @@
         <v>45</v>
       </c>
       <c r="H11" s="38" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="19" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="23" t="s">
@@ -3601,12 +3610,12 @@
         <v>46</v>
       </c>
       <c r="H12" s="38" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="19" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="23" t="s">
@@ -3625,12 +3634,12 @@
         <v>45</v>
       </c>
       <c r="H13" s="38" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="23" t="s">
@@ -3649,12 +3658,12 @@
         <v>45</v>
       </c>
       <c r="H14" s="38" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="23" t="s">
@@ -3673,12 +3682,12 @@
         <v>46</v>
       </c>
       <c r="H15" s="38" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="19" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="23" t="s">
@@ -3697,12 +3706,12 @@
         <v>45</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="19" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="23" t="s">
@@ -3721,12 +3730,12 @@
         <v>45</v>
       </c>
       <c r="H17" s="38" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="23" t="s">
@@ -3745,12 +3754,12 @@
         <v>46</v>
       </c>
       <c r="H18" s="38" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="23" t="s">
@@ -3769,12 +3778,12 @@
         <v>45</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="23" t="s">
@@ -3793,12 +3802,12 @@
         <v>45</v>
       </c>
       <c r="H20" s="38" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="19" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="23" t="s">
@@ -3817,12 +3826,12 @@
         <v>46</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="23" t="s">
@@ -3841,12 +3850,12 @@
         <v>45</v>
       </c>
       <c r="H22" s="38" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="19" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="23" t="s">
@@ -3865,12 +3874,12 @@
         <v>45</v>
       </c>
       <c r="H23" s="38" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="19" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="23" t="s">
@@ -3889,12 +3898,12 @@
         <v>46</v>
       </c>
       <c r="H24" s="38" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="19" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="23" t="s">
@@ -3913,12 +3922,12 @@
         <v>45</v>
       </c>
       <c r="H25" s="38" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="19" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="23" t="s">
@@ -3937,12 +3946,12 @@
         <v>45</v>
       </c>
       <c r="H26" s="38" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="23" t="s">
@@ -3961,12 +3970,12 @@
         <v>46</v>
       </c>
       <c r="H27" s="38" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="19" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="23" t="s">
@@ -3985,12 +3994,12 @@
         <v>45</v>
       </c>
       <c r="H28" s="38" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="19" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="23" t="s">
@@ -4009,12 +4018,12 @@
         <v>45</v>
       </c>
       <c r="H29" s="38" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="19" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="23" t="s">
@@ -4033,12 +4042,12 @@
         <v>46</v>
       </c>
       <c r="H30" s="38" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="19" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="23" t="s">
@@ -4057,12 +4066,12 @@
         <v>45</v>
       </c>
       <c r="H31" s="38" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="19" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="23" t="s">
@@ -4081,12 +4090,12 @@
         <v>45</v>
       </c>
       <c r="H32" s="38" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="19" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="23" t="s">
@@ -4105,12 +4114,12 @@
         <v>46</v>
       </c>
       <c r="H33" s="38" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="19" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="23" t="s">
@@ -4129,12 +4138,12 @@
         <v>45</v>
       </c>
       <c r="H34" s="38" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="23" t="s">
@@ -4153,12 +4162,12 @@
         <v>45</v>
       </c>
       <c r="H35" s="38" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="19" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B36" s="19"/>
       <c r="C36" s="23" t="s">
@@ -4177,12 +4186,12 @@
         <v>46</v>
       </c>
       <c r="H36" s="38" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="19" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="23" t="s">
@@ -4201,12 +4210,12 @@
         <v>45</v>
       </c>
       <c r="H37" s="38" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="19" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B38" s="19"/>
       <c r="C38" s="23" t="s">
@@ -4225,12 +4234,12 @@
         <v>45</v>
       </c>
       <c r="H38" s="38" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="19" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B39" s="19" t="s">
         <v>64</v>
@@ -4251,12 +4260,12 @@
         <v>45</v>
       </c>
       <c r="H39" s="37" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="19" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B40" s="19"/>
       <c r="C40" s="23" t="s">
@@ -4275,12 +4284,12 @@
         <v>45</v>
       </c>
       <c r="H40" s="37" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="19" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B41" s="19"/>
       <c r="C41" s="23" t="s">
@@ -4299,12 +4308,12 @@
         <v>45</v>
       </c>
       <c r="H41" s="93" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="19" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B42" s="19"/>
       <c r="C42" s="23" t="s">
@@ -4323,12 +4332,12 @@
         <v>45</v>
       </c>
       <c r="H42" s="37" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="19" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B43" s="19"/>
       <c r="C43" s="23" t="s">
@@ -4347,12 +4356,12 @@
         <v>45</v>
       </c>
       <c r="H43" s="37" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="19" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B44" s="19"/>
       <c r="C44" s="23" t="s">
@@ -4371,12 +4380,12 @@
         <v>45</v>
       </c>
       <c r="H44" s="37" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="19" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B45" s="19"/>
       <c r="C45" s="23" t="s">
@@ -4395,12 +4404,12 @@
         <v>45</v>
       </c>
       <c r="H45" s="37" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="19" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B46" s="19"/>
       <c r="C46" s="23" t="s">
@@ -4419,12 +4428,12 @@
         <v>45</v>
       </c>
       <c r="H46" s="37" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="19" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B47" s="19"/>
       <c r="C47" s="23" t="s">
@@ -4443,12 +4452,12 @@
         <v>45</v>
       </c>
       <c r="H47" s="37" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B48" s="19"/>
       <c r="C48" s="23" t="s">
@@ -4467,7 +4476,7 @@
         <v>45</v>
       </c>
       <c r="H48" s="37" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
   </sheetData>
@@ -4539,7 +4548,7 @@
         <v>64</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>356</v>
@@ -4571,7 +4580,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>357</v>
@@ -4633,7 +4642,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4644,11 +4653,11 @@
         <v>64</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="61" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4659,11 +4668,11 @@
         <v>64</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4674,10 +4683,10 @@
         <v>64</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E4" s="14"/>
     </row>
@@ -4730,10 +4739,10 @@
         <v>14</v>
       </c>
       <c r="F1" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>390</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>391</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>84</v>
@@ -4742,27 +4751,27 @@
         <v>337</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="K1" s="64" t="s">
         <v>392</v>
       </c>
-      <c r="K1" s="64" t="s">
+      <c r="L1" s="64" t="s">
         <v>393</v>
-      </c>
-      <c r="L1" s="64" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="43" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B2" s="43" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E2" s="85" t="s">
         <v>229</v>
@@ -4777,23 +4786,23 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="43" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E3" s="63" t="s">
         <v>219</v>
       </c>
       <c r="F3" s="63" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G3" s="63" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H3" s="2">
         <v>1234567</v>
@@ -4805,29 +4814,29 @@
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" s="43" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E4" s="85" t="s">
         <v>220</v>
       </c>
       <c r="F4" s="85" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G4" s="85" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H4" s="2">
         <v>1234567</v>
       </c>
       <c r="I4" s="84" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
@@ -4835,27 +4844,27 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="43" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E5" s="37" t="s">
         <v>221</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="37" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H5" s="2">
         <v>1234567</v>
       </c>
       <c r="I5" s="84" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J5" s="84" t="s">
         <v>0</v>
@@ -4865,89 +4874,89 @@
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" s="43" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>222</v>
       </c>
       <c r="F6" s="85" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G6" s="27"/>
       <c r="H6" s="2">
         <v>1234567</v>
       </c>
       <c r="I6" s="84" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J6" s="84"/>
       <c r="K6" s="84" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="L6" s="60"/>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" s="43" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B7" s="43"/>
       <c r="C7" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>223</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="84" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J7" s="84"/>
       <c r="K7" s="84"/>
       <c r="L7" s="60" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="43" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E8" s="37" t="s">
         <v>224</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H8" s="2">
         <v>1234567</v>
       </c>
       <c r="I8" s="84" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J8" t="s">
         <v>0</v>
@@ -4957,128 +4966,128 @@
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="43" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>225</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H9" s="2">
         <v>1234567</v>
       </c>
       <c r="I9" s="84" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J9" s="84"/>
       <c r="K9" s="84" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L9" s="60"/>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" s="43" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B10" s="43"/>
       <c r="C10" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>226</v>
       </c>
       <c r="F10" s="37" t="s">
+        <v>572</v>
+      </c>
+      <c r="G10" s="37" t="s">
         <v>573</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>574</v>
       </c>
       <c r="H10" s="2">
         <v>1234567</v>
       </c>
       <c r="I10" s="84" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J10" s="84"/>
       <c r="K10" s="84" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L10" s="60"/>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="43" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B11" s="43"/>
       <c r="C11" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>227</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="H11" s="2">
         <v>874531324</v>
       </c>
       <c r="I11" s="84" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J11" s="84"/>
       <c r="K11" s="84"/>
       <c r="L11" s="60" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="43" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B12" s="43"/>
       <c r="C12" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D12" s="27" t="s">
         <v>413</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>414</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>228</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H12" s="2">
         <v>1234567</v>
       </c>
       <c r="I12" s="84" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J12" s="84" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K12" s="84"/>
       <c r="L12" s="60"/>
@@ -5130,7 +5139,7 @@
         <v>16</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>306</v>
@@ -5174,16 +5183,16 @@
     </row>
     <row r="2" spans="4:20" ht="45">
       <c r="D2" s="43" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E2" s="43" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>322</v>
@@ -5227,16 +5236,16 @@
     </row>
     <row r="3" spans="4:20" ht="45">
       <c r="D3" s="43" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E3" s="43" t="s">
         <v>64</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>327</v>
@@ -5280,16 +5289,16 @@
     </row>
     <row r="4" spans="4:20" ht="30">
       <c r="D4" s="43" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E4" s="43" t="s">
         <v>64</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>332</v>
@@ -5333,16 +5342,16 @@
     </row>
     <row r="5" spans="4:20" ht="45">
       <c r="D5" s="43" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E5" s="43" t="s">
         <v>64</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>335</v>
@@ -5386,16 +5395,16 @@
     </row>
     <row r="6" spans="4:20" ht="30">
       <c r="D6" s="43" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E6" s="43" t="s">
         <v>64</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -5463,13 +5472,13 @@
         <v>64</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E2" s="60" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5480,10 +5489,10 @@
         <v>64</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E3" s="60">
         <v>500</v>
@@ -5560,10 +5569,10 @@
         <v>64</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D2" s="72" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E2" s="73" t="s">
         <v>5</v>
@@ -5581,10 +5590,10 @@
         <v>45</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60">
@@ -5595,10 +5604,10 @@
         <v>64</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D3" s="72" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E3" s="73" t="s">
         <v>5</v>
@@ -5616,10 +5625,10 @@
         <v>45</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K3" s="63" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60">
@@ -5630,10 +5639,10 @@
         <v>64</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D4" s="72" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E4" s="73" t="s">
         <v>5</v>
@@ -5651,7 +5660,7 @@
         <v>45</v>
       </c>
       <c r="J4" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K4" s="63" t="s">
         <v>1</v>
@@ -5665,10 +5674,10 @@
         <v>64</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D5" s="72" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E5" s="73" t="s">
         <v>5</v>
@@ -5686,7 +5695,7 @@
         <v>45</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K5" s="63" t="s">
         <v>2</v>
@@ -5700,10 +5709,10 @@
         <v>64</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D6" s="72" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E6" s="73" t="s">
         <v>5</v>
@@ -5721,10 +5730,10 @@
         <v>45</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K6" s="27" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="60">
@@ -5735,10 +5744,10 @@
         <v>64</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D7" s="72" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E7" s="73" t="s">
         <v>5</v>
@@ -5756,10 +5765,10 @@
         <v>45</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60">
@@ -5770,10 +5779,10 @@
         <v>64</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D8" s="72" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E8" s="73" t="s">
         <v>5</v>
@@ -5791,10 +5800,10 @@
         <v>45</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K8" s="27" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45">
@@ -5805,10 +5814,10 @@
         <v>64</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E9" s="73" t="s">
         <v>5</v>
@@ -5826,10 +5835,10 @@
         <v>45</v>
       </c>
       <c r="J9" s="27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K9" s="27" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="45">
@@ -5840,10 +5849,10 @@
         <v>64</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E10" s="73" t="s">
         <v>5</v>
@@ -5861,10 +5870,10 @@
         <v>45</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K10" s="27" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="45">
@@ -5875,10 +5884,10 @@
         <v>64</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E11" s="73" t="s">
         <v>5</v>
@@ -5896,10 +5905,10 @@
         <v>45</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="45">
@@ -5910,10 +5919,10 @@
         <v>64</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E12" s="73" t="s">
         <v>5</v>
@@ -5931,10 +5940,10 @@
         <v>45</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K12" s="27" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="45">
@@ -5945,10 +5954,10 @@
         <v>64</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E13" s="73" t="s">
         <v>5</v>
@@ -5966,10 +5975,10 @@
         <v>45</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K13" s="27" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45">
@@ -5980,10 +5989,10 @@
         <v>64</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E14" s="73" t="s">
         <v>5</v>
@@ -6001,10 +6010,10 @@
         <v>45</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="45">
@@ -6015,10 +6024,10 @@
         <v>64</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E15" s="73" t="s">
         <v>5</v>
@@ -6036,10 +6045,10 @@
         <v>45</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K15" s="27" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -6141,7 +6150,7 @@
         <v>68</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F2" s="22" t="s">
         <v>13</v>
@@ -6157,7 +6166,7 @@
       </c>
       <c r="J2" s="24"/>
       <c r="K2" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L2" s="15" t="s">
         <v>95</v>
@@ -6187,7 +6196,7 @@
         <v>68</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>13</v>
@@ -6203,7 +6212,7 @@
       </c>
       <c r="J3" s="24"/>
       <c r="K3" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L3" s="15" t="s">
         <v>149</v>
@@ -6233,7 +6242,7 @@
         <v>68</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>49</v>
@@ -6249,7 +6258,7 @@
       </c>
       <c r="J4" s="24"/>
       <c r="K4" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>150</v>
@@ -6279,7 +6288,7 @@
         <v>82</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>13</v>
@@ -6295,7 +6304,7 @@
       </c>
       <c r="J5" s="24"/>
       <c r="K5" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>151</v>
@@ -6325,7 +6334,7 @@
         <v>82</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>13</v>
@@ -6341,7 +6350,7 @@
       </c>
       <c r="J6" s="24"/>
       <c r="K6" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L6" s="15" t="s">
         <v>152</v>
@@ -6371,7 +6380,7 @@
         <v>82</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>49</v>
@@ -6387,7 +6396,7 @@
       </c>
       <c r="J7" s="24"/>
       <c r="K7" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L7" s="15" t="s">
         <v>153</v>
@@ -6417,7 +6426,7 @@
         <v>104</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>13</v>
@@ -6433,7 +6442,7 @@
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>95</v>
@@ -6463,7 +6472,7 @@
         <v>104</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>13</v>
@@ -6479,7 +6488,7 @@
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>154</v>
@@ -6509,7 +6518,7 @@
         <v>104</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>49</v>
@@ -6525,7 +6534,7 @@
       </c>
       <c r="J10" s="24"/>
       <c r="K10" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L10" s="15" t="s">
         <v>155</v>
@@ -6557,7 +6566,7 @@
         <v>105</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F11" s="22" t="s">
         <v>13</v>
@@ -6573,7 +6582,7 @@
       </c>
       <c r="J11" s="24"/>
       <c r="K11" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L11" s="15" t="s">
         <v>156</v>
@@ -6603,7 +6612,7 @@
         <v>105</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F12" s="22" t="s">
         <v>13</v>
@@ -6619,7 +6628,7 @@
       </c>
       <c r="J12" s="24"/>
       <c r="K12" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L12" s="15" t="s">
         <v>157</v>
@@ -6649,7 +6658,7 @@
         <v>105</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>49</v>
@@ -6665,7 +6674,7 @@
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L13" s="15" t="s">
         <v>95</v>
@@ -6691,19 +6700,19 @@
         <v>64</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>45</v>
@@ -6713,7 +6722,7 @@
       </c>
       <c r="J14" s="24"/>
       <c r="K14" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L14" s="15" t="s">
         <v>158</v>
@@ -6806,7 +6815,7 @@
         <v>64</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D2" s="82" t="s">
         <v>217</v>
@@ -6885,25 +6894,25 @@
         <v>14</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>417</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>418</v>
       </c>
       <c r="I1" s="41" t="s">
         <v>337</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="K1" s="41" t="s">
         <v>419</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="L1" s="41" t="s">
         <v>420</v>
-      </c>
-      <c r="L1" s="41" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -6914,10 +6923,10 @@
         <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E2" s="37" t="s">
         <v>218</v>
@@ -6944,10 +6953,10 @@
         <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E3" s="37" t="s">
         <v>219</v>
@@ -6962,7 +6971,7 @@
         <v>12345678</v>
       </c>
       <c r="I3" s="60" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J3" s="60"/>
       <c r="K3" s="60"/>
@@ -6976,10 +6985,10 @@
         <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>220</v>
@@ -6992,10 +7001,10 @@
         <v>12345678</v>
       </c>
       <c r="I4" s="60" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J4" s="60" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K4" s="60"/>
       <c r="L4" s="44"/>
@@ -7008,10 +7017,10 @@
         <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E5" s="37" t="s">
         <v>218</v>
@@ -7026,10 +7035,10 @@
         <v>12345678</v>
       </c>
       <c r="I5" s="60" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J5" s="60" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K5" s="60"/>
       <c r="L5" s="44"/>
@@ -7042,10 +7051,10 @@
         <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>219</v>
@@ -7058,11 +7067,11 @@
         <v>12345678</v>
       </c>
       <c r="I6" s="60" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J6" s="60"/>
       <c r="K6" s="60" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L6" s="44"/>
     </row>
@@ -7074,10 +7083,10 @@
         <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>220</v>
@@ -7092,11 +7101,11 @@
         <v>12345678</v>
       </c>
       <c r="I7" s="60" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J7" s="60"/>
       <c r="K7" s="60" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L7" s="44"/>
     </row>
@@ -7108,10 +7117,10 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E8" s="37" t="s">
         <v>218</v>
@@ -7124,12 +7133,12 @@
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="60" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J8" s="60"/>
       <c r="K8" s="60"/>
       <c r="L8" s="60" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
@@ -7140,10 +7149,10 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>219</v>
@@ -7158,12 +7167,12 @@
         <v>123</v>
       </c>
       <c r="I9" s="60" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J9" s="60"/>
       <c r="K9" s="60"/>
       <c r="L9" s="60" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
@@ -7174,10 +7183,10 @@
         <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>220</v>
@@ -7192,14 +7201,14 @@
         <v>123</v>
       </c>
       <c r="I10" s="60" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J10" s="60"/>
       <c r="K10" s="60" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L10" s="60" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45">
@@ -7210,10 +7219,10 @@
         <v>64</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>218</v>
@@ -7228,12 +7237,12 @@
         <v>123456798</v>
       </c>
       <c r="I11" s="60" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J11" s="60"/>
       <c r="K11" s="60"/>
       <c r="L11" s="60" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -7271,7 +7280,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>85</v>
@@ -7279,13 +7288,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D2" s="87"/>
       <c r="E2" s="40" t="s">
@@ -7294,19 +7303,19 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="19" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>64</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D3" s="87" t="s">
+        <v>664</v>
+      </c>
+      <c r="E3" s="40" t="s">
         <v>665</v>
-      </c>
-      <c r="E3" s="40" t="s">
-        <v>666</v>
       </c>
     </row>
   </sheetData>
@@ -7376,7 +7385,7 @@
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A2" s="19" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>64</v>
@@ -7404,12 +7413,12 @@
       </c>
       <c r="J2" s="24"/>
       <c r="K2" s="13" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A3" s="19" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="22" t="s">
@@ -7435,12 +7444,12 @@
       </c>
       <c r="J3" s="24"/>
       <c r="K3" s="38" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A4" s="19" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="22" t="s">
@@ -7466,12 +7475,12 @@
       </c>
       <c r="J4" s="24"/>
       <c r="K4" s="38" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A5" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>64</v>
@@ -7499,12 +7508,12 @@
       </c>
       <c r="J5" s="24"/>
       <c r="K5" s="38" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A6" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="22" t="s">
@@ -7530,12 +7539,12 @@
       </c>
       <c r="J6" s="24"/>
       <c r="K6" s="38" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A7" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="22" t="s">
@@ -7561,12 +7570,12 @@
       </c>
       <c r="J7" s="24"/>
       <c r="K7" s="38" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A8" s="19" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="22" t="s">
@@ -7592,12 +7601,12 @@
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="38" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A9" s="19" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="22" t="s">
@@ -7623,12 +7632,12 @@
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="38" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A10" s="19" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="22" t="s">
@@ -7654,12 +7663,12 @@
       </c>
       <c r="J10" s="24"/>
       <c r="K10" s="38" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A11" s="19" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="22" t="s">
@@ -7685,12 +7694,12 @@
       </c>
       <c r="J11" s="24"/>
       <c r="K11" s="38" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="60">
       <c r="A12" s="19" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="22" t="s">
@@ -7716,12 +7725,12 @@
       </c>
       <c r="J12" s="24"/>
       <c r="K12" s="38" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="60">
       <c r="A13" s="19" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="22" t="s">
@@ -7747,12 +7756,12 @@
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="38" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="60">
       <c r="A14" s="19" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="22" t="s">
@@ -7781,7 +7790,7 @@
     </row>
     <row r="15" spans="1:11" ht="60">
       <c r="A15" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="22" t="s">
@@ -7810,7 +7819,7 @@
     </row>
     <row r="16" spans="1:11" ht="60">
       <c r="A16" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="22" t="s">
@@ -7839,7 +7848,7 @@
     </row>
     <row r="17" spans="1:11" ht="60">
       <c r="A17" s="19" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="22" t="s">
@@ -7868,7 +7877,7 @@
     </row>
     <row r="18" spans="1:11" ht="60">
       <c r="A18" s="19" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>64</v>
@@ -7899,7 +7908,7 @@
     </row>
     <row r="19" spans="1:11" ht="60">
       <c r="A19" s="19" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="22" t="s">
@@ -7928,7 +7937,7 @@
     </row>
     <row r="20" spans="1:11" ht="60">
       <c r="A20" s="19" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="22" t="s">
@@ -7954,12 +7963,12 @@
       </c>
       <c r="J20" s="24"/>
       <c r="K20" s="38" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="60">
       <c r="A21" s="19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="22" t="s">
@@ -7985,12 +7994,12 @@
       </c>
       <c r="J21" s="24"/>
       <c r="K21" s="38" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="60">
       <c r="A22" s="19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="22" t="s">
@@ -8016,12 +8025,12 @@
       </c>
       <c r="J22" s="24"/>
       <c r="K22" s="38" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="60">
       <c r="A23" s="19" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="22" t="s">
@@ -8047,12 +8056,12 @@
       </c>
       <c r="J23" s="24"/>
       <c r="K23" s="38" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="60">
       <c r="A24" s="19" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="22" t="s">
@@ -8078,12 +8087,12 @@
       </c>
       <c r="J24" s="24"/>
       <c r="K24" s="38" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60">
       <c r="A25" s="19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="22" t="s">
@@ -8109,12 +8118,12 @@
       </c>
       <c r="J25" s="24"/>
       <c r="K25" s="38" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60">
       <c r="A26" s="19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="22" t="s">
@@ -8140,12 +8149,12 @@
       </c>
       <c r="J26" s="24"/>
       <c r="K26" s="38" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60">
       <c r="A27" s="19" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="22" t="s">
@@ -8171,12 +8180,12 @@
       </c>
       <c r="J27" s="24"/>
       <c r="K27" s="38" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60">
       <c r="A28" s="19" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="22" t="s">
@@ -8202,12 +8211,12 @@
       </c>
       <c r="J28" s="24"/>
       <c r="K28" s="38" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60">
       <c r="A29" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="22" t="s">
@@ -8233,12 +8242,12 @@
       </c>
       <c r="J29" s="24"/>
       <c r="K29" s="38" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60">
       <c r="A30" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="22" t="s">
@@ -8264,12 +8273,12 @@
       </c>
       <c r="J30" s="24"/>
       <c r="K30" s="38" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60">
       <c r="A31" s="19" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="22" t="s">
@@ -8295,12 +8304,12 @@
       </c>
       <c r="J31" s="24"/>
       <c r="K31" s="38" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="60">
       <c r="A32" s="19" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="22" t="s">
@@ -8329,7 +8338,7 @@
     </row>
     <row r="33" spans="1:11" ht="60">
       <c r="A33" s="19" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="22" t="s">
@@ -8358,7 +8367,7 @@
     </row>
     <row r="34" spans="1:11" ht="60">
       <c r="A34" s="19" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="22" t="s">
@@ -8387,7 +8396,7 @@
     </row>
     <row r="35" spans="1:11" ht="60">
       <c r="A35" s="19" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>64</v>
@@ -8418,7 +8427,7 @@
     </row>
     <row r="36" spans="1:11" ht="60">
       <c r="A36" s="19" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B36" s="19"/>
       <c r="C36" s="22" t="s">
@@ -8447,7 +8456,7 @@
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" s="19" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="22" t="s">
@@ -8476,7 +8485,7 @@
     </row>
     <row r="38" spans="1:11" ht="60">
       <c r="A38" s="19" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B38" s="19"/>
       <c r="C38" s="22" t="s">
@@ -8505,7 +8514,7 @@
     </row>
     <row r="39" spans="1:11" ht="60">
       <c r="A39" s="19" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B39" s="19"/>
       <c r="C39" s="22" t="s">
@@ -8515,7 +8524,7 @@
         <v>98</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F39" s="22" t="s">
         <v>49</v>
@@ -8534,16 +8543,16 @@
     </row>
     <row r="40" spans="1:11" ht="60">
       <c r="A40" s="19" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>64</v>
       </c>
       <c r="C40" s="22" t="s">
+        <v>711</v>
+      </c>
+      <c r="D40" s="22" t="s">
         <v>712</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>713</v>
       </c>
       <c r="E40" s="23" t="s">
         <v>5</v>
@@ -8562,7 +8571,7 @@
       </c>
       <c r="J40" s="24"/>
       <c r="K40" s="92" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
   </sheetData>
@@ -8610,7 +8619,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>14</v>
@@ -8621,53 +8630,53 @@
     </row>
     <row r="2" spans="1:7" ht="120">
       <c r="A2" s="53" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="53" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F2" s="70"/>
       <c r="G2" s="89"/>
     </row>
     <row r="3" spans="1:7" ht="45">
       <c r="A3" s="53" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="53" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E3" s="53" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F3" s="70"/>
       <c r="G3" s="90"/>
     </row>
     <row r="4" spans="1:7" ht="120">
       <c r="A4" s="53" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B4" s="53"/>
       <c r="C4" s="53" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F4" s="38" t="s">
         <v>224</v>
@@ -8676,17 +8685,17 @@
     </row>
     <row r="5" spans="1:7" ht="45">
       <c r="A5" s="53" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B5" s="53"/>
       <c r="C5" s="53" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F5" s="38" t="s">
         <v>225</v>
@@ -8733,103 +8742,103 @@
         <v>15</v>
       </c>
       <c r="E1" s="88" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="53" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="53" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E2" s="89" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="53" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B3" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E3" s="90" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
       <c r="A4" s="53" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B4" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E4" s="89" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
       <c r="A5" s="53" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="53" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E5" s="89" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="A6" s="53" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="53" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D6" s="53" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E6" s="90" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
       <c r="A7" s="53" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="53" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E7" s="89" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -8872,39 +8881,39 @@
         <v>15</v>
       </c>
       <c r="E1" s="88" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="53" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="53" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E2" s="89" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="53" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="53" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E3" s="89" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
   </sheetData>
@@ -8955,16 +8964,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="53" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="40" t="s">
+        <v>692</v>
+      </c>
+      <c r="D2" s="91" t="s">
         <v>693</v>
-      </c>
-      <c r="D2" s="91" t="s">
-        <v>694</v>
       </c>
       <c r="E2" s="40" t="s">
         <v>217</v>
@@ -8973,97 +8982,97 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="53" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B3" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C3" s="40" t="s">
+        <v>695</v>
+      </c>
+      <c r="D3" s="91" t="s">
         <v>696</v>
       </c>
-      <c r="D3" s="91" t="s">
+      <c r="E3" s="40" t="s">
         <v>697</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="F3" s="91" t="s">
         <v>698</v>
-      </c>
-      <c r="F3" s="91" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="53" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B4" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D4" s="91" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E4" s="85" t="s">
         <v>218</v>
       </c>
       <c r="F4" s="91" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="53" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B5" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C5" s="40" t="s">
+        <v>363</v>
+      </c>
+      <c r="D5" s="91" t="s">
         <v>364</v>
-      </c>
-      <c r="D5" s="91" t="s">
-        <v>365</v>
       </c>
       <c r="E5" s="91"/>
       <c r="F5" s="91" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="53" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B6" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C6" s="40" t="s">
+        <v>703</v>
+      </c>
+      <c r="D6" s="40" t="s">
         <v>704</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>705</v>
       </c>
       <c r="E6" s="40" t="s">
         <v>219</v>
       </c>
       <c r="F6" s="91" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="53" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B7" s="53" t="s">
         <v>64</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F7" s="40" t="s">
         <v>0</v>
@@ -9712,7 +9721,7 @@
         <v>100</v>
       </c>
       <c r="G27" s="37" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -9735,7 +9744,7 @@
         <v>100</v>
       </c>
       <c r="G28" s="37" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -9758,7 +9767,7 @@
         <v>100</v>
       </c>
       <c r="G29" s="86" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -9781,7 +9790,7 @@
         <v>100</v>
       </c>
       <c r="G30" s="38" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -9804,7 +9813,7 @@
         <v>100</v>
       </c>
       <c r="G31" s="38" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -9827,7 +9836,7 @@
         <v>100</v>
       </c>
       <c r="G32" s="38" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -9850,7 +9859,7 @@
         <v>100</v>
       </c>
       <c r="G33" s="38" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -9873,7 +9882,7 @@
         <v>100</v>
       </c>
       <c r="G34" s="38" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -9896,7 +9905,7 @@
         <v>100</v>
       </c>
       <c r="G35" s="38" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -9919,7 +9928,7 @@
         <v>100</v>
       </c>
       <c r="G36" s="38" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -9942,7 +9951,7 @@
         <v>100</v>
       </c>
       <c r="G37" s="38" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -9965,7 +9974,7 @@
         <v>100</v>
       </c>
       <c r="G38" s="38" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -9988,7 +9997,7 @@
         <v>100</v>
       </c>
       <c r="G39" s="38" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -10011,7 +10020,7 @@
         <v>100</v>
       </c>
       <c r="G40" s="38" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -10034,7 +10043,7 @@
         <v>100</v>
       </c>
       <c r="G41" s="38" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -10057,7 +10066,7 @@
         <v>100</v>
       </c>
       <c r="G42" s="38" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -10080,7 +10089,7 @@
         <v>100</v>
       </c>
       <c r="G43" s="38" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -10103,7 +10112,7 @@
         <v>100</v>
       </c>
       <c r="G44" s="38" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -10126,7 +10135,7 @@
         <v>100</v>
       </c>
       <c r="G45" s="38" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -10149,7 +10158,7 @@
         <v>100</v>
       </c>
       <c r="G46" s="38" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -10172,7 +10181,7 @@
         <v>100</v>
       </c>
       <c r="G47" s="38" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -10195,7 +10204,7 @@
         <v>100</v>
       </c>
       <c r="G48" s="38" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -10218,7 +10227,7 @@
         <v>100</v>
       </c>
       <c r="G49" s="38" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -10241,7 +10250,7 @@
         <v>100</v>
       </c>
       <c r="G50" s="38" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -10264,7 +10273,7 @@
         <v>100</v>
       </c>
       <c r="G51" s="38" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -10287,7 +10296,7 @@
         <v>100</v>
       </c>
       <c r="G52" s="38" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -10310,7 +10319,7 @@
         <v>100</v>
       </c>
       <c r="G53" s="38" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -10333,7 +10342,7 @@
         <v>100</v>
       </c>
       <c r="G54" s="38" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -10356,7 +10365,7 @@
         <v>100</v>
       </c>
       <c r="G55" s="38" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -10379,7 +10388,7 @@
         <v>100</v>
       </c>
       <c r="G56" s="38" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -10402,7 +10411,7 @@
         <v>100</v>
       </c>
       <c r="G57" s="38" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -10425,7 +10434,7 @@
         <v>100</v>
       </c>
       <c r="G58" s="38" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -10448,7 +10457,7 @@
         <v>100</v>
       </c>
       <c r="G59" s="38" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -10471,7 +10480,7 @@
         <v>100</v>
       </c>
       <c r="G60" s="38" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -10494,7 +10503,7 @@
         <v>100</v>
       </c>
       <c r="G61" s="38" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -10517,7 +10526,7 @@
         <v>100</v>
       </c>
       <c r="G62" s="38" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -10540,7 +10549,7 @@
         <v>100</v>
       </c>
       <c r="G63" s="38" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -10563,7 +10572,7 @@
         <v>100</v>
       </c>
       <c r="G64" s="38" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -10586,12 +10595,12 @@
         <v>100</v>
       </c>
       <c r="G65" s="38" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="30" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B66" s="31" t="s">
         <v>77</v>
@@ -10609,12 +10618,12 @@
         <v>100</v>
       </c>
       <c r="G66" s="38" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="30" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B67" s="31" t="s">
         <v>77</v>
@@ -10632,12 +10641,12 @@
         <v>100</v>
       </c>
       <c r="G67" s="37" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="30" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B68" s="31" t="s">
         <v>77</v>
@@ -10655,12 +10664,12 @@
         <v>100</v>
       </c>
       <c r="G68" s="37" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="30" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B69" s="31" t="s">
         <v>77</v>
@@ -10678,12 +10687,12 @@
         <v>100</v>
       </c>
       <c r="G69" s="93" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="30" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B70" s="31" t="s">
         <v>77</v>
@@ -10701,12 +10710,12 @@
         <v>100</v>
       </c>
       <c r="G70" s="37" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="30" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B71" s="31" t="s">
         <v>77</v>
@@ -10724,12 +10733,12 @@
         <v>100</v>
       </c>
       <c r="G71" s="37" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="30" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B72" s="31" t="s">
         <v>77</v>
@@ -10747,12 +10756,12 @@
         <v>100</v>
       </c>
       <c r="G72" s="37" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="30" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B73" s="31" t="s">
         <v>77</v>
@@ -10770,12 +10779,12 @@
         <v>100</v>
       </c>
       <c r="G73" s="37" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="30" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B74" s="31" t="s">
         <v>77</v>
@@ -10793,12 +10802,12 @@
         <v>100</v>
       </c>
       <c r="G74" s="37" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="30" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B75" s="31" t="s">
         <v>77</v>
@@ -10816,12 +10825,12 @@
         <v>100</v>
       </c>
       <c r="G75" s="37" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="30" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B76" s="31" t="s">
         <v>77</v>
@@ -10839,7 +10848,7 @@
         <v>100</v>
       </c>
       <c r="G76" s="37" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
   </sheetData>
@@ -10876,7 +10885,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C1" s="26" t="s">
         <v>76</v>
@@ -10888,13 +10897,13 @@
         <v>11</v>
       </c>
       <c r="F1" s="67" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G1" s="67" t="s">
         <v>330</v>
       </c>
       <c r="H1" s="67" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="285">
@@ -10902,25 +10911,25 @@
         <v>5</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D2" s="75" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>160</v>
       </c>
       <c r="F2" s="97" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="60">
@@ -10928,10 +10937,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D3" s="75" t="s">
         <v>75</v>
@@ -10949,10 +10958,10 @@
         <v>74</v>
       </c>
       <c r="B4" s="30" t="s">
+        <v>451</v>
+      </c>
+      <c r="C4" s="31" t="s">
         <v>452</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>453</v>
       </c>
       <c r="D4" s="75" t="s">
         <v>185</v>
@@ -10969,10 +10978,10 @@
         <v>162</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D5" s="75" t="s">
         <v>163</v>
@@ -10989,10 +10998,10 @@
         <v>191</v>
       </c>
       <c r="B6" s="30" t="s">
+        <v>451</v>
+      </c>
+      <c r="C6" s="31" t="s">
         <v>452</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>453</v>
       </c>
       <c r="D6" s="76" t="s">
         <v>185</v>
@@ -11006,49 +11015,49 @@
     </row>
     <row r="7" spans="1:16" ht="75">
       <c r="A7" s="30" t="s">
+        <v>438</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>513</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>446</v>
+      </c>
+      <c r="D7" s="75" t="s">
         <v>439</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>514</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>447</v>
-      </c>
-      <c r="D7" s="75" t="s">
-        <v>440</v>
       </c>
       <c r="E7" s="30" t="s">
         <v>192</v>
       </c>
       <c r="F7" s="27" t="s">
+        <v>443</v>
+      </c>
+      <c r="G7" s="24" t="s">
         <v>444</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="H7" s="27" t="s">
         <v>445</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="75">
       <c r="A8" s="30" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D8" s="75" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>160</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="24" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H8" s="27"/>
     </row>
@@ -11356,13 +11365,13 @@
         <v>77</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>34</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>36</v>
@@ -11413,7 +11422,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>14</v>
@@ -11428,10 +11437,10 @@
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="98" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D2" s="99" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E2" s="69" t="s">
         <v>5</v>
@@ -11445,7 +11454,7 @@
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="98" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D3" s="99" t="s">
         <v>76</v>
@@ -11462,7 +11471,7 @@
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="98" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D4" s="99" t="s">
         <v>330</v>
@@ -11479,10 +11488,10 @@
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="98" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D5" s="99" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E5" s="69" t="s">
         <v>5</v>
@@ -11496,10 +11505,10 @@
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="98" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D6" s="99" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E6" s="69" t="s">
         <v>5</v>
@@ -11513,10 +11522,10 @@
       </c>
       <c r="B7" s="43"/>
       <c r="C7" s="98" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D7" s="99" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E7" s="69" t="s">
         <v>5</v>
@@ -11530,10 +11539,10 @@
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="98" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D8" s="99" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E8" s="69" t="s">
         <v>5</v>
@@ -11549,10 +11558,10 @@
         <v>64</v>
       </c>
       <c r="C9" s="98" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D9" s="99" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E9" s="69" t="s">
         <v>5</v>
@@ -12372,7 +12381,7 @@
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1">
       <c r="A2" s="43" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B2" s="43" t="s">
         <v>64</v>
@@ -12428,7 +12437,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="43" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B3" s="43" t="s">
         <v>64</v>
@@ -12484,7 +12493,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="43" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B4" s="43" t="s">
         <v>64</v>
@@ -12540,7 +12549,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="43" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B5" s="43" t="s">
         <v>64</v>
@@ -12686,7 +12695,7 @@
         <v>340</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>221</v>
@@ -12712,16 +12721,16 @@
         <v>341</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E3" s="38" t="s">
         <v>222</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H3" s="55"/>
       <c r="I3" s="55"/>
@@ -12738,19 +12747,19 @@
         <v>341</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>223</v>
       </c>
       <c r="F4" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="H4" s="72" t="s">
         <v>374</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>381</v>
-      </c>
-      <c r="H4" s="72" t="s">
-        <v>375</v>
       </c>
       <c r="I4" s="55"/>
       <c r="J4" s="55"/>
@@ -12766,17 +12775,17 @@
         <v>342</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E5" s="38" t="s">
         <v>224</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H5" s="72" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I5" s="55" t="s">
         <v>1</v>
@@ -12794,17 +12803,17 @@
         <v>343</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>225</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G6" s="27"/>
       <c r="H6" s="72" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I6" s="55"/>
       <c r="J6" s="55" t="s">
@@ -12822,7 +12831,7 @@
         <v>344</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E7" s="38" t="s">
         <v>226</v>
@@ -12830,7 +12839,7 @@
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
       <c r="H7" s="72" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I7" s="55" t="s">
         <v>1</v>
@@ -12850,19 +12859,19 @@
         <v>345</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E8" s="38" t="s">
         <v>227</v>
       </c>
       <c r="F8" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="H8" s="72" t="s">
         <v>374</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>381</v>
-      </c>
-      <c r="H8" s="72" t="s">
-        <v>375</v>
       </c>
       <c r="I8" s="55"/>
       <c r="J8" s="55"/>
@@ -12981,10 +12990,10 @@
         <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D4" s="79" t="s">
         <v>435</v>
-      </c>
-      <c r="D4" s="79" t="s">
-        <v>436</v>
       </c>
       <c r="E4" s="63" t="s">
         <v>350</v>
@@ -13010,8 +13019,8 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13053,7 +13062,7 @@
         <v>360</v>
       </c>
       <c r="E2" s="63" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -13068,7 +13077,7 @@
         <v>362</v>
       </c>
       <c r="E3" s="63" t="s">
-        <v>363</v>
+        <v>770</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="75">
@@ -13077,13 +13086,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="37" t="s">
+        <v>363</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>365</v>
-      </c>
       <c r="E4" s="63" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -13092,28 +13101,28 @@
       </c>
       <c r="B5" s="58"/>
       <c r="C5" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="63" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30">
+      <c r="A6" s="100" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="100"/>
+      <c r="C6" s="101" t="s">
         <v>367</v>
       </c>
-      <c r="E5" s="63" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="37" t="s">
+      <c r="D6" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="E6" s="63" t="s">
-        <v>772</v>
+      <c r="E6" s="102" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45">
@@ -13122,13 +13131,13 @@
       </c>
       <c r="B7" s="58"/>
       <c r="C7" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>371</v>
-      </c>
       <c r="E7" s="59" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
   </sheetData>
@@ -13176,7 +13185,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="53" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>64</v>
@@ -13193,7 +13202,7 @@
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="53" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B3" s="53" t="s">
         <v>64</v>
@@ -13210,7 +13219,7 @@
     </row>
     <row r="4" spans="1:5" ht="30">
       <c r="A4" s="53" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B4" s="53" t="s">
         <v>64</v>
@@ -13227,7 +13236,7 @@
     </row>
     <row r="5" spans="1:5" ht="30">
       <c r="A5" s="53" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B5" s="53" t="s">
         <v>64</v>
@@ -13244,7 +13253,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="53" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B6" s="53" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Complete tweaking registration regression
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="218340" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="219270" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="AccountSetupRegression" sheetId="37" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2575" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2579" uniqueCount="776">
   <si>
     <t>Please enter a valid email</t>
   </si>
@@ -2459,6 +2459,9 @@
   <si>
     <t>PasswordValidation:Please enter a strong Password of at least 6 characters
 PasswordConfValidation:The Password and Confirmation Password do not match</t>
+  </si>
+  <si>
+    <t>get</t>
   </si>
 </sst>
 </file>
@@ -13019,8 +13022,8 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13052,7 +13055,7 @@
       <c r="A2" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="100" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="37" t="s">
@@ -13081,17 +13084,19 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="75">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="37" t="s">
-        <v>363</v>
+      <c r="B4" s="100" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="101" t="s">
+        <v>775</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="102" t="s">
         <v>771</v>
       </c>
     </row>
@@ -13099,7 +13104,9 @@
       <c r="A5" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="58"/>
+      <c r="B5" s="100" t="s">
+        <v>64</v>
+      </c>
       <c r="C5" s="37" t="s">
         <v>365</v>
       </c>
@@ -13114,7 +13121,9 @@
       <c r="A6" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="100" t="s">
+        <v>64</v>
+      </c>
       <c r="C6" s="101" t="s">
         <v>367</v>
       </c>
@@ -13129,7 +13138,9 @@
       <c r="A7" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="58"/>
+      <c r="B7" s="100" t="s">
+        <v>64</v>
+      </c>
       <c r="C7" s="5" t="s">
         <v>369</v>
       </c>

</xml_diff>

<commit_message>
added new users to latest Cart cases
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="264870" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="268590" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="AccountSetupRegression" sheetId="37" r:id="rId1"/>
-    <sheet name="CheckOutRegression" sheetId="7" r:id="rId2"/>
-    <sheet name="PDPRegression" sheetId="29" r:id="rId3"/>
-    <sheet name="CartRegression" sheetId="18" r:id="rId4"/>
-    <sheet name="PLPRegression" sheetId="21" r:id="rId5"/>
-    <sheet name="RegistrationRegression" sheetId="24" r:id="rId6"/>
-    <sheet name="AddressBookRegression" sheetId="19" r:id="rId7"/>
-    <sheet name="PaymentDetailsRegression" sheetId="25" r:id="rId8"/>
-    <sheet name="LoginRegression" sheetId="41" r:id="rId9"/>
+    <sheet name="CheckOutRegression" sheetId="7" r:id="rId1"/>
+    <sheet name="PDPRegression" sheetId="29" r:id="rId2"/>
+    <sheet name="CartRegression" sheetId="18" r:id="rId3"/>
+    <sheet name="PLPRegression" sheetId="21" r:id="rId4"/>
+    <sheet name="RegistrationRegression" sheetId="24" r:id="rId5"/>
+    <sheet name="AddressBookRegression" sheetId="19" r:id="rId6"/>
+    <sheet name="PaymentDetailsRegression" sheetId="25" r:id="rId7"/>
+    <sheet name="LoginRegression" sheetId="41" r:id="rId8"/>
+    <sheet name="AccountSetupRegression" sheetId="37" r:id="rId9"/>
     <sheet name="users" sheetId="13" r:id="rId10"/>
     <sheet name="products" sheetId="8" r:id="rId11"/>
     <sheet name="cards" sheetId="9" r:id="rId12"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="423">
   <si>
     <t>Accept</t>
   </si>
@@ -1322,6 +1322,90 @@
   </si>
   <si>
     <t>7783624</t>
+  </si>
+  <si>
+    <t>crt0050@OSH-automation.com</t>
+  </si>
+  <si>
+    <t>U-26</t>
+  </si>
+  <si>
+    <t>U-27</t>
+  </si>
+  <si>
+    <t>U-28</t>
+  </si>
+  <si>
+    <t>U-29</t>
+  </si>
+  <si>
+    <t>U-30</t>
+  </si>
+  <si>
+    <t>U-31</t>
+  </si>
+  <si>
+    <t>U-32</t>
+  </si>
+  <si>
+    <t>1234575</t>
+  </si>
+  <si>
+    <t>crt0051@OSH-automation.com</t>
+  </si>
+  <si>
+    <t>crt0052@OSH-automation.com</t>
+  </si>
+  <si>
+    <t>crt0053@OSH-automation.com</t>
+  </si>
+  <si>
+    <t>crt0054@OSH-automation.com</t>
+  </si>
+  <si>
+    <t>crt0055@OSH-automation.com</t>
+  </si>
+  <si>
+    <t>crt0056@OSH-automation.com</t>
+  </si>
+  <si>
+    <t>crt0057@OSH-automation.com</t>
+  </si>
+  <si>
+    <t>crt0058@OSH-automation.com</t>
+  </si>
+  <si>
+    <t>U-33</t>
+  </si>
+  <si>
+    <t>U-34</t>
+  </si>
+  <si>
+    <t>AC-25</t>
+  </si>
+  <si>
+    <t>AC-26</t>
+  </si>
+  <si>
+    <t>AC-27</t>
+  </si>
+  <si>
+    <t>AC-28</t>
+  </si>
+  <si>
+    <t>AC-29</t>
+  </si>
+  <si>
+    <t>AC-30</t>
+  </si>
+  <si>
+    <t>AC-31</t>
+  </si>
+  <si>
+    <t>AC-32</t>
+  </si>
+  <si>
+    <t>AC-33</t>
   </si>
 </sst>
 </file>
@@ -1375,7 +1459,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1396,6 +1480,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1547,7 +1637,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1738,6 +1828,26 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2084,609 +2194,640 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet25">
+  <sheetPr codeName="Sheet2">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E7"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="44"/>
-    <col min="3" max="3" width="9.5703125" style="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.85546875" style="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5703125" style="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" style="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" style="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6" style="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="44"/>
+    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="6" style="56" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="50" customFormat="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1">
+      <c r="A1" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="52" customFormat="1">
-      <c r="A2" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="37" t="s">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="60">
+      <c r="A2" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="G2" s="41" t="s">
         <v>376</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="52" customFormat="1">
-      <c r="A3" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="37" t="s">
+      <c r="H2" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="60">
+      <c r="A3" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="F3" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>376</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="60">
+      <c r="A4" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>376</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="60">
+      <c r="A5" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="G5" s="41" t="s">
         <v>376</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="52" customFormat="1">
-      <c r="A4" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="37" t="s">
+      <c r="H5" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="42"/>
+      <c r="K5" s="43"/>
+    </row>
+    <row r="6" spans="1:11" ht="60">
+      <c r="A6" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="G6" s="41" t="s">
         <v>376</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="52" customFormat="1">
-      <c r="A5" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="37" t="s">
+      <c r="H6" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="42"/>
+      <c r="K6" s="43" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="60">
+      <c r="A7" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="G7" s="41" t="s">
         <v>376</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="52" customFormat="1">
-      <c r="A6" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="37" t="s">
+      <c r="H7" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="60">
+      <c r="A8" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="F8" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="G8" s="41" t="s">
         <v>376</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="52" customFormat="1">
-      <c r="A7" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="37" t="s">
+      <c r="H8" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="60">
+      <c r="A9" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="F9" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>376</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="52" customFormat="1">
-      <c r="A8" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="37" t="s">
+      <c r="G9" s="41" t="s">
+        <v>377</v>
+      </c>
+      <c r="H9" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="60">
+      <c r="A10" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="G10" s="41" t="s">
         <v>377</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="52" customFormat="1">
-      <c r="A9" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="37" t="s">
+      <c r="H10" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="60">
+      <c r="A11" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="F11" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="G11" s="41" t="s">
         <v>377</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="52" customFormat="1">
-      <c r="A10" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="37" t="s">
+      <c r="H11" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="60">
+      <c r="A12" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="G12" s="41" t="s">
         <v>377</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="37" t="s">
+      <c r="H12" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="42"/>
+      <c r="K12" s="43"/>
+    </row>
+    <row r="13" spans="1:11" ht="60">
+      <c r="A13" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="G13" s="41" t="s">
         <v>377</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="17" t="s">
+      <c r="H13" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="42"/>
+      <c r="K13" s="43"/>
+    </row>
+    <row r="14" spans="1:11" ht="60">
+      <c r="A14" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>377</v>
+      </c>
+      <c r="H14" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="42"/>
+      <c r="K14" s="43"/>
+    </row>
+    <row r="15" spans="1:11" ht="60">
+      <c r="A15" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>377</v>
+      </c>
+      <c r="H15" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="42"/>
+      <c r="K15" s="43"/>
+    </row>
+    <row r="16" spans="1:11" ht="60">
+      <c r="A16" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>377</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="42"/>
+      <c r="K16" s="43"/>
+    </row>
+    <row r="17" spans="1:11" ht="60">
+      <c r="A17" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>377</v>
+      </c>
+      <c r="H17" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="42"/>
+      <c r="K17" s="43"/>
+    </row>
+    <row r="18" spans="1:11" ht="60">
+      <c r="A18" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>377</v>
+      </c>
+      <c r="H18" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="42"/>
+      <c r="K18" s="43"/>
+    </row>
+    <row r="19" spans="1:11" ht="60">
+      <c r="A19" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>377</v>
+      </c>
+      <c r="H19" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" s="42"/>
+      <c r="K19" s="43"/>
+    </row>
+    <row r="20" spans="1:11" ht="60">
+      <c r="A20" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>377</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="21" t="s">
-        <v>263</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="21" t="s">
-        <v>266</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="21" t="s">
-        <v>267</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="21" t="s">
-        <v>270</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="21" t="s">
-        <v>271</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="21" t="s">
-        <v>272</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="21" t="s">
-        <v>273</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2700,10 +2841,10 @@
   <sheetPr codeName="Sheet19">
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3312,6 +3453,213 @@
       </c>
       <c r="G26" s="19" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="17" t="s">
+        <v>396</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="68" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="68" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="68" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="17" t="s">
+        <v>399</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="68" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="68" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="67" t="s">
+        <v>401</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="68" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="67" t="s">
+        <v>402</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="68" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="67" t="s">
+        <v>412</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" s="68" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="67" t="s">
+        <v>413</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="G35" s="68" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -3808,650 +4156,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2">
-    <tabColor theme="8" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1:K20"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:G20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="6" style="56" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1">
-      <c r="A1" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="60">
-      <c r="A2" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G2" s="41" t="s">
-        <v>376</v>
-      </c>
-      <c r="H2" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" ht="60">
-      <c r="A3" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="G3" s="41" t="s">
-        <v>376</v>
-      </c>
-      <c r="H3" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="60">
-      <c r="A4" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="G4" s="41" t="s">
-        <v>376</v>
-      </c>
-      <c r="H4" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="60">
-      <c r="A5" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G5" s="41" t="s">
-        <v>376</v>
-      </c>
-      <c r="H5" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" s="42"/>
-      <c r="K5" s="43"/>
-    </row>
-    <row r="6" spans="1:11" ht="60">
-      <c r="A6" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G6" s="41" t="s">
-        <v>376</v>
-      </c>
-      <c r="H6" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" s="42"/>
-      <c r="K6" s="43" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="60">
-      <c r="A7" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G7" s="41" t="s">
-        <v>376</v>
-      </c>
-      <c r="H7" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="60">
-      <c r="A8" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G8" s="41" t="s">
-        <v>376</v>
-      </c>
-      <c r="H8" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="60">
-      <c r="A9" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H9" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="60">
-      <c r="A10" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G10" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H10" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="60">
-      <c r="A11" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H11" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="60">
-      <c r="A12" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G12" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H12" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="42"/>
-      <c r="K12" s="43"/>
-    </row>
-    <row r="13" spans="1:11" ht="60">
-      <c r="A13" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H13" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J13" s="42"/>
-      <c r="K13" s="43"/>
-    </row>
-    <row r="14" spans="1:11" ht="60">
-      <c r="A14" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G14" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H14" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="42"/>
-      <c r="K14" s="43"/>
-    </row>
-    <row r="15" spans="1:11" ht="60">
-      <c r="A15" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H15" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I15" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J15" s="42"/>
-      <c r="K15" s="43"/>
-    </row>
-    <row r="16" spans="1:11" ht="60">
-      <c r="A16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G16" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H16" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" s="42"/>
-      <c r="K16" s="43"/>
-    </row>
-    <row r="17" spans="1:11" ht="60">
-      <c r="A17" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H17" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I17" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17" s="42"/>
-      <c r="K17" s="43"/>
-    </row>
-    <row r="18" spans="1:11" ht="60">
-      <c r="A18" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H18" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I18" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" s="42"/>
-      <c r="K18" s="43"/>
-    </row>
-    <row r="19" spans="1:11" ht="60">
-      <c r="A19" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H19" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" s="42"/>
-      <c r="K19" s="43"/>
-    </row>
-    <row r="20" spans="1:11" ht="60">
-      <c r="A20" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>377</v>
-      </c>
-      <c r="H20" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42" t="s">
-        <v>312</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -4793,15 +4497,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4972,9 +4676,7 @@
       <c r="A5" s="64" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>50</v>
-      </c>
+      <c r="B5" s="42"/>
       <c r="C5" s="21" t="s">
         <v>386</v>
       </c>
@@ -5008,9 +4710,7 @@
       <c r="A6" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="42" t="s">
-        <v>50</v>
-      </c>
+      <c r="B6" s="42"/>
       <c r="C6" s="21" t="s">
         <v>387</v>
       </c>
@@ -5262,7 +4962,9 @@
       <c r="A13" s="64" t="s">
         <v>178</v>
       </c>
-      <c r="B13" s="43"/>
+      <c r="B13" s="43" t="s">
+        <v>50</v>
+      </c>
       <c r="C13" s="43" t="s">
         <v>186</v>
       </c>
@@ -5273,7 +4975,7 @@
         <v>294</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>318</v>
+        <v>396</v>
       </c>
       <c r="G13" s="43"/>
       <c r="H13" s="43"/>
@@ -5309,7 +5011,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="43" t="s">
-        <v>319</v>
+        <v>397</v>
       </c>
       <c r="G14" s="43"/>
       <c r="H14" s="42" t="s">
@@ -5349,7 +5051,7 @@
         <v>6</v>
       </c>
       <c r="F15" s="43" t="s">
-        <v>320</v>
+        <v>398</v>
       </c>
       <c r="G15" s="43"/>
       <c r="H15" s="42"/>
@@ -5374,7 +5076,9 @@
       <c r="A16" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C16" s="43" t="s">
         <v>186</v>
       </c>
@@ -5385,7 +5089,7 @@
         <v>6</v>
       </c>
       <c r="F16" s="43" t="s">
-        <v>318</v>
+        <v>399</v>
       </c>
       <c r="G16" s="43"/>
       <c r="H16" s="42"/>
@@ -5410,9 +5114,7 @@
       <c r="A17" s="64" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="42" t="s">
-        <v>50</v>
-      </c>
+      <c r="B17" s="42"/>
       <c r="C17" s="43" t="s">
         <v>186</v>
       </c>
@@ -5446,7 +5148,9 @@
       <c r="A18" s="64" t="s">
         <v>388</v>
       </c>
-      <c r="B18" s="42"/>
+      <c r="B18" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C18" s="43" t="s">
         <v>186</v>
       </c>
@@ -5457,7 +5161,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="43" t="s">
-        <v>320</v>
+        <v>400</v>
       </c>
       <c r="G18" s="43"/>
       <c r="H18" s="42"/>
@@ -5487,7 +5191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5">
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -5581,7 +5285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8">
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -5724,7 +5428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9">
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -5812,7 +5516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10">
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -5888,7 +5592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
@@ -6029,4 +5733,845 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet25">
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="44"/>
+    <col min="3" max="3" width="9.5703125" style="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.85546875" style="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5703125" style="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" style="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" style="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6" style="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="44"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="50" customFormat="1">
+      <c r="A1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="52" customFormat="1">
+      <c r="A2" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="52" customFormat="1">
+      <c r="A3" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="52" customFormat="1">
+      <c r="A4" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="52" customFormat="1">
+      <c r="A5" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="52" customFormat="1">
+      <c r="A6" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="52" customFormat="1">
+      <c r="A7" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="52" customFormat="1">
+      <c r="A8" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="52" customFormat="1">
+      <c r="A9" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="52" customFormat="1">
+      <c r="A10" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="69" t="s">
+        <v>414</v>
+      </c>
+      <c r="B25" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="F25" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="74" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="69" t="s">
+        <v>415</v>
+      </c>
+      <c r="B26" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="E26" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="F26" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="74" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="69" t="s">
+        <v>416</v>
+      </c>
+      <c r="B27" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="F27" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" s="74" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="69" t="s">
+        <v>417</v>
+      </c>
+      <c r="B28" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="E28" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="F28" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H28" s="74" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="69" t="s">
+        <v>418</v>
+      </c>
+      <c r="B29" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="F29" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="74" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="69" t="s">
+        <v>419</v>
+      </c>
+      <c r="B30" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="E30" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="F30" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="74" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="69" t="s">
+        <v>420</v>
+      </c>
+      <c r="B31" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="E31" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="F31" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" s="74" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="69" t="s">
+        <v>421</v>
+      </c>
+      <c r="B32" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="E32" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="F32" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" s="74" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="69" t="s">
+        <v>422</v>
+      </c>
+      <c r="B33" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="E33" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="F33" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="74" t="s">
+        <v>413</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified runners and browsers tabs name and Active column become runTest
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="269520" yWindow="0" windowWidth="16980" windowHeight="7020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="5610"/>
   </bookViews>
   <sheets>
-    <sheet name="Browsers" sheetId="42" r:id="rId1"/>
-    <sheet name="Runner" sheetId="43" r:id="rId2"/>
+    <sheet name="BrowsersRegression" sheetId="42" r:id="rId1"/>
+    <sheet name="RunnerRegression" sheetId="43" r:id="rId2"/>
     <sheet name="CheckOutRegression" sheetId="7" r:id="rId3"/>
     <sheet name="PDPRegression" sheetId="29" r:id="rId4"/>
     <sheet name="CartRegression" sheetId="18" r:id="rId5"/>
@@ -23,13 +23,13 @@
     <sheet name="cards" sheetId="9" r:id="rId14"/>
     <sheet name="addresses" sheetId="10" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="437">
   <si>
     <t>Accept</t>
   </si>
@@ -1413,46 +1413,43 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chrome </t>
-  </si>
-  <si>
-    <t>FireFox</t>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>addressBookRegression</t>
+  </si>
+  <si>
+    <t>cartRunner</t>
+  </si>
+  <si>
+    <t>checkoutRegression</t>
+  </si>
+  <si>
+    <t>LoginRegression</t>
+  </si>
+  <si>
+    <t>PaymentDetailsRegression</t>
+  </si>
+  <si>
+    <t>PDPRegression</t>
+  </si>
+  <si>
+    <t>PLPRegression</t>
+  </si>
+  <si>
+    <t>RegistrationRegression</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Firefox</t>
   </si>
   <si>
     <t>Chrome Grid</t>
   </si>
   <si>
-    <t>Regression</t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>addressBookRegression</t>
-  </si>
-  <si>
-    <t>cartRunner</t>
-  </si>
-  <si>
-    <t>checkoutRegression</t>
-  </si>
-  <si>
-    <t>LoginRegression</t>
-  </si>
-  <si>
-    <t>PaymentDetailsRegression</t>
-  </si>
-  <si>
-    <t>PDPRegression</t>
-  </si>
-  <si>
-    <t>PLPRegression</t>
-  </si>
-  <si>
-    <t>RegistrationRegression</t>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -1712,7 +1709,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1924,11 +1921,18 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2277,10 +2281,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A28:B31"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2288,36 +2292,41 @@
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="28" spans="1:2">
-      <c r="A28" s="5" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="75" t="s">
         <v>423</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="58" t="s">
-        <v>425</v>
-      </c>
-      <c r="B29" s="75" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="58" t="s">
-        <v>426</v>
-      </c>
-      <c r="B30" s="75"/>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="58" t="s">
-        <v>427</v>
-      </c>
-      <c r="B31" s="75"/>
+      <c r="B1" s="75" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="76" t="s">
+        <v>433</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="44" t="s">
+        <v>434</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="44" t="s">
+        <v>435</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>436</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3312,7 +3321,7 @@
   </sheetPr>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -4628,79 +4637,79 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="79" t="s">
+        <v>427</v>
+      </c>
+      <c r="B2" s="78" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="80" t="s">
+        <v>425</v>
+      </c>
+      <c r="B3" s="78"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="80" t="s">
+        <v>429</v>
+      </c>
+      <c r="B4" s="78"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="80" t="s">
+        <v>430</v>
+      </c>
+      <c r="B5" s="78"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="80" t="s">
+        <v>431</v>
+      </c>
+      <c r="B6" s="78"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="80" t="s">
+        <v>432</v>
+      </c>
+      <c r="B7" s="78"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="80" t="s">
         <v>428</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="76" t="s">
-        <v>432</v>
-      </c>
-      <c r="B2" s="75"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="77" t="s">
-        <v>430</v>
-      </c>
-      <c r="B3" s="75"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="77" t="s">
-        <v>434</v>
-      </c>
-      <c r="B4" s="75" t="s">
+      <c r="B8" s="78"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="80" t="s">
+        <v>426</v>
+      </c>
+      <c r="B9" s="78" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="77" t="s">
-        <v>435</v>
-      </c>
-      <c r="B5" s="75" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="77" t="s">
-        <v>436</v>
-      </c>
-      <c r="B6" s="75" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="77" t="s">
-        <v>437</v>
-      </c>
-      <c r="B7" s="75"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="77" t="s">
-        <v>433</v>
-      </c>
-      <c r="B8" s="75"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="77" t="s">
-        <v>431</v>
-      </c>
-      <c r="B9" s="75"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4712,7 +4721,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add envvars to runners
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="5610"/>
+    <workbookView xWindow="6615" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="BrowsersRegression" sheetId="42" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="437">
   <si>
     <t>Accept</t>
   </si>
@@ -1446,17 +1446,17 @@
     <t>Firefox</t>
   </si>
   <si>
-    <t>Chrome Grid</t>
-  </si>
-  <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>ChromeG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1495,15 +1495,8 @@
       <color theme="1"/>
       <name val="Monospace"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1514,11 +1507,6 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -1701,15 +1689,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1892,33 +1879,30 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1934,8 +1918,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2283,8 +2266,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2293,35 +2276,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="74" t="s">
         <v>423</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="74" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="75" t="s">
         <v>433</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="76"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="B3" s="77"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="44" t="s">
-        <v>434</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="44" t="s">
+      <c r="B4" s="77" t="s">
         <v>435</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -3075,236 +3054,236 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="69" t="s">
+      <c r="A25" s="68" t="s">
         <v>414</v>
       </c>
-      <c r="B25" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="70" t="s">
+      <c r="B25" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="71" t="s">
+      <c r="D25" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="E25" s="72" t="s">
+      <c r="E25" s="71" t="s">
         <v>376</v>
       </c>
-      <c r="F25" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="G25" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" s="74" t="s">
+      <c r="F25" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="73" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="69" t="s">
+      <c r="A26" s="68" t="s">
         <v>415</v>
       </c>
-      <c r="B26" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="70" t="s">
+      <c r="B26" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="71" t="s">
+      <c r="D26" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="E26" s="72" t="s">
+      <c r="E26" s="71" t="s">
         <v>376</v>
       </c>
-      <c r="F26" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="H26" s="74" t="s">
+      <c r="F26" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="73" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="68" t="s">
         <v>416</v>
       </c>
-      <c r="B27" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="70" t="s">
+      <c r="B27" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="71" t="s">
+      <c r="D27" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="E27" s="72" t="s">
+      <c r="E27" s="71" t="s">
         <v>376</v>
       </c>
-      <c r="F27" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="H27" s="74" t="s">
+      <c r="F27" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" s="73" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="69" t="s">
+      <c r="A28" s="68" t="s">
         <v>417</v>
       </c>
-      <c r="B28" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="70" t="s">
+      <c r="B28" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="71" t="s">
+      <c r="D28" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="E28" s="72" t="s">
+      <c r="E28" s="71" t="s">
         <v>376</v>
       </c>
-      <c r="F28" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="H28" s="74" t="s">
+      <c r="F28" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="H28" s="73" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="69" t="s">
+      <c r="A29" s="68" t="s">
         <v>418</v>
       </c>
-      <c r="B29" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="70" t="s">
+      <c r="B29" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="71" t="s">
+      <c r="D29" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="E29" s="72" t="s">
+      <c r="E29" s="71" t="s">
         <v>376</v>
       </c>
-      <c r="F29" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="G29" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="H29" s="74" t="s">
+      <c r="F29" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="73" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="69" t="s">
+      <c r="A30" s="68" t="s">
         <v>419</v>
       </c>
-      <c r="B30" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="70" t="s">
+      <c r="B30" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="71" t="s">
+      <c r="D30" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="E30" s="72" t="s">
+      <c r="E30" s="71" t="s">
         <v>376</v>
       </c>
-      <c r="F30" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="H30" s="74" t="s">
+      <c r="F30" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="73" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="68" t="s">
         <v>420</v>
       </c>
-      <c r="B31" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="70" t="s">
+      <c r="B31" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="71" t="s">
+      <c r="D31" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="E31" s="72" t="s">
+      <c r="E31" s="71" t="s">
         <v>376</v>
       </c>
-      <c r="F31" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="H31" s="74" t="s">
+      <c r="F31" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" s="73" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="69" t="s">
+      <c r="A32" s="68" t="s">
         <v>421</v>
       </c>
-      <c r="B32" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="70" t="s">
+      <c r="B32" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="71" t="s">
+      <c r="D32" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="E32" s="72" t="s">
+      <c r="E32" s="71" t="s">
         <v>376</v>
       </c>
-      <c r="F32" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="H32" s="74" t="s">
+      <c r="F32" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" s="73" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="69" t="s">
+      <c r="A33" s="68" t="s">
         <v>422</v>
       </c>
-      <c r="B33" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="70" t="s">
+      <c r="B33" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="71" t="s">
+      <c r="D33" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="E33" s="72" t="s">
+      <c r="E33" s="71" t="s">
         <v>376</v>
       </c>
-      <c r="F33" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="G33" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="H33" s="74" t="s">
+      <c r="F33" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="73" t="s">
         <v>413</v>
       </c>
     </row>
@@ -3952,7 +3931,7 @@
       <c r="F27" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="68" t="s">
+      <c r="G27" s="67" t="s">
         <v>395</v>
       </c>
     </row>
@@ -3975,7 +3954,7 @@
       <c r="F28" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G28" s="68" t="s">
+      <c r="G28" s="67" t="s">
         <v>404</v>
       </c>
     </row>
@@ -3998,7 +3977,7 @@
       <c r="F29" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G29" s="68" t="s">
+      <c r="G29" s="67" t="s">
         <v>405</v>
       </c>
     </row>
@@ -4021,7 +4000,7 @@
       <c r="F30" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G30" s="68" t="s">
+      <c r="G30" s="67" t="s">
         <v>406</v>
       </c>
     </row>
@@ -4044,12 +4023,12 @@
       <c r="F31" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G31" s="68" t="s">
+      <c r="G31" s="67" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="67" t="s">
+      <c r="A32" s="66" t="s">
         <v>401</v>
       </c>
       <c r="B32" s="18" t="s">
@@ -4067,12 +4046,12 @@
       <c r="F32" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G32" s="68" t="s">
+      <c r="G32" s="67" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="66" t="s">
         <v>402</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -4090,12 +4069,12 @@
       <c r="F33" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G33" s="68" t="s">
+      <c r="G33" s="67" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="67" t="s">
+      <c r="A34" s="66" t="s">
         <v>412</v>
       </c>
       <c r="B34" s="18" t="s">
@@ -4113,12 +4092,12 @@
       <c r="F34" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G34" s="68" t="s">
+      <c r="G34" s="67" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="67" t="s">
+      <c r="A35" s="66" t="s">
         <v>413</v>
       </c>
       <c r="B35" s="18" t="s">
@@ -4136,7 +4115,7 @@
       <c r="F35" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="G35" s="68" t="s">
+      <c r="G35" s="67" t="s">
         <v>411</v>
       </c>
     </row>
@@ -4156,8 +4135,8 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4638,7 +4617,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4656,54 +4635,66 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="78" t="s">
         <v>427</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="77" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="79" t="s">
         <v>425</v>
       </c>
-      <c r="B3" s="78"/>
+      <c r="B3" s="77" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="79" t="s">
         <v>429</v>
       </c>
-      <c r="B4" s="78"/>
+      <c r="B4" s="77" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="79" t="s">
         <v>430</v>
       </c>
-      <c r="B5" s="78"/>
+      <c r="B5" s="77" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="79" t="s">
         <v>431</v>
       </c>
-      <c r="B6" s="78"/>
+      <c r="B6" s="77" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="79" t="s">
         <v>432</v>
       </c>
-      <c r="B7" s="78"/>
+      <c r="B7" s="77" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="79" t="s">
         <v>428</v>
       </c>
-      <c r="B8" s="78"/>
+      <c r="B8" s="77" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="79" t="s">
         <v>426</v>
       </c>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="77" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4720,8 +4711,8 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A13" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4809,7 +4800,9 @@
       <c r="A3" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C3" s="8" t="s">
         <v>72</v>
       </c>
@@ -4840,7 +4833,9 @@
       <c r="A4" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C4" s="8" t="s">
         <v>15</v>
       </c>
@@ -4935,7 +4930,9 @@
       <c r="A7" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C7" s="8" t="s">
         <v>77</v>
       </c>
@@ -4966,7 +4963,9 @@
       <c r="A8" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C8" s="8" t="s">
         <v>78</v>
       </c>
@@ -4997,7 +4996,9 @@
       <c r="A9" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C9" s="8" t="s">
         <v>79</v>
       </c>
@@ -5028,7 +5029,9 @@
       <c r="A10" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C10" s="8" t="s">
         <v>80</v>
       </c>
@@ -5059,7 +5062,9 @@
       <c r="A11" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C11" s="8" t="s">
         <v>16</v>
       </c>
@@ -5090,7 +5095,9 @@
       <c r="A12" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C12" s="8" t="s">
         <v>81</v>
       </c>
@@ -5119,7 +5126,9 @@
       <c r="A13" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C13" s="8" t="s">
         <v>82</v>
       </c>
@@ -5148,7 +5157,9 @@
       <c r="A14" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C14" s="8" t="s">
         <v>83</v>
       </c>
@@ -5177,7 +5188,9 @@
       <c r="A15" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C15" s="8" t="s">
         <v>84</v>
       </c>
@@ -5206,7 +5219,9 @@
       <c r="A16" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C16" s="8" t="s">
         <v>85</v>
       </c>
@@ -5235,7 +5250,9 @@
       <c r="A17" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C17" s="8" t="s">
         <v>86</v>
       </c>
@@ -5264,7 +5281,9 @@
       <c r="A18" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C18" s="8" t="s">
         <v>86</v>
       </c>
@@ -5293,7 +5312,9 @@
       <c r="A19" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C19" s="8" t="s">
         <v>86</v>
       </c>
@@ -5364,8 +5385,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5406,7 +5427,9 @@
       <c r="A2" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C2" s="53" t="s">
         <v>142</v>
       </c>
@@ -5423,7 +5446,9 @@
       <c r="A3" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C3" s="53" t="s">
         <v>143</v>
       </c>
@@ -5440,7 +5465,9 @@
       <c r="A4" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C4" s="53" t="s">
         <v>144</v>
       </c>
@@ -5457,7 +5484,9 @@
       <c r="A5" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C5" s="53" t="s">
         <v>145</v>
       </c>
@@ -5474,7 +5503,9 @@
       <c r="A6" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C6" s="53" t="s">
         <v>146</v>
       </c>
@@ -5491,7 +5522,9 @@
       <c r="A7" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C7" s="53" t="s">
         <v>147</v>
       </c>
@@ -5508,7 +5541,9 @@
       <c r="A8" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C8" s="53" t="s">
         <v>148</v>
       </c>
@@ -5544,7 +5579,9 @@
       <c r="A10" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C10" s="53" t="s">
         <v>336</v>
       </c>
@@ -5563,7 +5600,9 @@
       <c r="A11" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C11" s="53" t="s">
         <v>337</v>
       </c>
@@ -5582,7 +5621,9 @@
       <c r="A12" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C12" s="53" t="s">
         <v>338</v>
       </c>
@@ -5601,7 +5642,9 @@
       <c r="A13" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C13" s="53" t="s">
         <v>339</v>
       </c>
@@ -5620,7 +5663,9 @@
       <c r="A14" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C14" s="53" t="s">
         <v>340</v>
       </c>
@@ -5639,7 +5684,9 @@
       <c r="A15" s="8" t="s">
         <v>373</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C15" s="53" t="s">
         <v>341</v>
       </c>
@@ -5658,7 +5705,9 @@
       <c r="A16" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C16" s="53" t="s">
         <v>342</v>
       </c>
@@ -5707,8 +5756,8 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5777,11 +5826,13 @@
       <c r="A2" s="64" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C2" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="65" t="s">
         <v>190</v>
       </c>
       <c r="E2" s="42" t="s">
@@ -5811,11 +5862,13 @@
       <c r="A3" s="64" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="65"/>
+      <c r="B3" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C3" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="65" t="s">
         <v>191</v>
       </c>
       <c r="E3" s="42" t="s">
@@ -5845,11 +5898,13 @@
       <c r="A4" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="65"/>
+      <c r="B4" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C4" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="65" t="s">
         <v>192</v>
       </c>
       <c r="E4" s="42" t="s">
@@ -5879,7 +5934,9 @@
       <c r="A5" s="64" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="42"/>
+      <c r="B5" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C5" s="21" t="s">
         <v>386</v>
       </c>
@@ -5913,7 +5970,9 @@
       <c r="A6" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="42"/>
+      <c r="B6" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C6" s="21" t="s">
         <v>387</v>
       </c>
@@ -5951,7 +6010,9 @@
       <c r="A7" s="64" t="s">
         <v>173</v>
       </c>
-      <c r="B7" s="65"/>
+      <c r="B7" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C7" s="42" t="s">
         <v>89</v>
       </c>
@@ -5989,11 +6050,13 @@
       <c r="A8" s="64" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="65"/>
+      <c r="B8" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C8" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D8" s="66" t="s">
+      <c r="D8" s="65" t="s">
         <v>194</v>
       </c>
       <c r="E8" s="42" t="s">
@@ -6023,11 +6086,13 @@
       <c r="A9" s="64" t="s">
         <v>175</v>
       </c>
-      <c r="B9" s="65"/>
+      <c r="B9" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C9" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="65" t="s">
         <v>195</v>
       </c>
       <c r="E9" s="42" t="s">
@@ -6057,11 +6122,13 @@
       <c r="A10" s="64" t="s">
         <v>176</v>
       </c>
-      <c r="B10" s="42"/>
+      <c r="B10" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C10" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="65" t="s">
         <v>329</v>
       </c>
       <c r="E10" s="42" t="s">
@@ -6093,11 +6160,13 @@
       <c r="A11" s="64" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="42"/>
+      <c r="B11" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C11" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="65" t="s">
         <v>330</v>
       </c>
       <c r="E11" s="42" t="s">
@@ -6129,11 +6198,13 @@
       <c r="A12" s="64" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="42"/>
+      <c r="B12" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C12" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="65" t="s">
         <v>331</v>
       </c>
       <c r="E12" s="42" t="s">
@@ -6165,13 +6236,13 @@
       <c r="A13" s="64" t="s">
         <v>178</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="42" t="s">
         <v>50</v>
       </c>
       <c r="C13" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D13" s="66" t="s">
+      <c r="D13" s="65" t="s">
         <v>332</v>
       </c>
       <c r="E13" s="43" t="s">
@@ -6203,7 +6274,9 @@
       <c r="A14" s="64" t="s">
         <v>179</v>
       </c>
-      <c r="B14" s="42"/>
+      <c r="B14" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C14" s="42" t="s">
         <v>89</v>
       </c>
@@ -6243,11 +6316,13 @@
       <c r="A15" s="64" t="s">
         <v>180</v>
       </c>
-      <c r="B15" s="42"/>
+      <c r="B15" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C15" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D15" s="66" t="s">
+      <c r="D15" s="65" t="s">
         <v>334</v>
       </c>
       <c r="E15" s="42" t="s">
@@ -6285,7 +6360,7 @@
       <c r="C16" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D16" s="66" t="s">
+      <c r="D16" s="65" t="s">
         <v>335</v>
       </c>
       <c r="E16" s="42" t="s">
@@ -6317,11 +6392,13 @@
       <c r="A17" s="64" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="42"/>
+      <c r="B17" s="42" t="s">
+        <v>50</v>
+      </c>
       <c r="C17" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D17" s="66" t="s">
+      <c r="D17" s="65" t="s">
         <v>188</v>
       </c>
       <c r="E17" s="42" t="s">
@@ -6357,7 +6434,7 @@
       <c r="C18" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="D18" s="66" t="s">
+      <c r="D18" s="65" t="s">
         <v>328</v>
       </c>
       <c r="E18" s="42" t="s">

</xml_diff>

<commit_message>
merge address book regression
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3C3D630F-7637-4E1E-9989-182092CF7ADB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9933DB98-C9B7-4A57-84FF-9DEF3EDCD8CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33945" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37725" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="440">
   <si>
     <t>Accept</t>
   </si>
@@ -4810,7 +4810,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -6736,8 +6736,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6775,9 +6775,7 @@
       <c r="A2" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>49</v>
-      </c>
+      <c r="B2" s="20"/>
       <c r="C2" s="20" t="s">
         <v>175</v>
       </c>
@@ -6785,7 +6783,7 @@
         <v>173</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>57</v>
@@ -6805,7 +6803,7 @@
         <v>176</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
Test for change password, added a new sheet in excel sheet
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="105705" yWindow="0" windowWidth="17790" windowHeight="5610" activeTab="4"/>
+    <workbookView xWindow="105705" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -24,7 +24,8 @@
     <sheet name="users" sheetId="13" r:id="rId15"/>
     <sheet name="products" sheetId="8" r:id="rId16"/>
     <sheet name="addresses" sheetId="10" r:id="rId17"/>
-    <sheet name="cards" sheetId="9" r:id="rId18"/>
+    <sheet name="PasswordRegression" sheetId="47" r:id="rId18"/>
+    <sheet name="cards" sheetId="9" r:id="rId19"/>
   </sheets>
   <calcPr calcId="152511"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="514">
   <si>
     <t>Accept</t>
   </si>
@@ -1549,11 +1550,147 @@
   <si>
     <t xml:space="preserve">HP_FooterTopSection,HP_FooterBottomSection,HP_FooterAccount </t>
   </si>
+  <si>
+    <t>currentPassword</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>confirmNewPassword</t>
+  </si>
+  <si>
+    <t>click cancel</t>
+  </si>
+  <si>
+    <t>click update
+revert changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click update </t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>Password Cancel</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>Password Update</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>Password Update: Without  current password</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>Password Update: Incorrect current password</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>Password Update: Without new password</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>Password Update: Invalid new password</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>Password Update: Without confirm new password</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>Password Update: Incorrect confirm new password</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>Password Update: Pasword not match password rules.</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>Password Update: Confirm password not matching.</t>
+  </si>
+  <si>
+    <t>U-52</t>
+  </si>
+  <si>
+    <t>mohammad-asad@live.com</t>
+  </si>
+  <si>
+    <t>m654321</t>
+  </si>
+  <si>
+    <t>m12345678</t>
+  </si>
+  <si>
+    <t>m123456789</t>
+  </si>
+  <si>
+    <t>m123456798</t>
+  </si>
+  <si>
+    <t>m6543222</t>
+  </si>
+  <si>
+    <t>global-alerts:Your password has been changed</t>
+  </si>
+  <si>
+    <t>currentPasswordErrors:Please enter your current password</t>
+  </si>
+  <si>
+    <t>newPasswordEerrors:Please enter a new password</t>
+  </si>
+  <si>
+    <t>confirmNewPasswordErrors:Please confirm your new password</t>
+  </si>
+  <si>
+    <t>global-alerts:Please correct the errors below.
+currentPasswordErrors:Please enter your current password</t>
+  </si>
+  <si>
+    <t>global-alerts:Please correct the errors below.
+newPasswordEerrors:Password does not meet minimum requirements.</t>
+  </si>
+  <si>
+    <t>global-alerts:Please correct the errors below.
+confirmNewPasswordErrors:Password does not meet minimum requirements.</t>
+  </si>
+  <si>
+    <t>global-alerts:Please correct the errors below.
+confirmNewPasswordErrors:Password and password confirmation do not match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click update
+alert </t>
+  </si>
+  <si>
+    <t>click update 
+alert</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -1781,7 +1918,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1997,6 +2134,40 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2528,7 +2699,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3652,10 +3823,10 @@
   <sheetPr codeName="Sheet19">
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3666,7 +3837,7 @@
     <col min="4" max="4" width="9.85546875" style="34" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="9.42578125" style="34" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="12.28515625" style="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.5703125" style="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.28515625" style="34" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
@@ -4864,6 +5035,29 @@
       </c>
       <c r="G52" s="4" t="s">
         <v>343</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="83" t="s">
+        <v>497</v>
+      </c>
+      <c r="B53" s="84" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="84" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="64" t="s">
+        <v>499</v>
+      </c>
+      <c r="G53" s="66" t="s">
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -4922,9 +5116,11 @@
     <hyperlink ref="G3" r:id="rId52"/>
     <hyperlink ref="G4" r:id="rId53"/>
     <hyperlink ref="G6" r:id="rId54"/>
+    <hyperlink ref="G2" r:id="rId55"/>
+    <hyperlink ref="G53" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId55"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId57"/>
 </worksheet>
 </file>
 
@@ -4936,7 +5132,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5296,6 +5492,347 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="73.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="80" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="81" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="89" t="s">
+        <v>471</v>
+      </c>
+      <c r="G1" s="89" t="s">
+        <v>472</v>
+      </c>
+      <c r="H1" s="89" t="s">
+        <v>473</v>
+      </c>
+      <c r="I1" s="90" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="24" customHeight="1">
+      <c r="A2" s="85" t="s">
+        <v>477</v>
+      </c>
+      <c r="B2" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="88" t="s">
+        <v>478</v>
+      </c>
+      <c r="D2" s="88" t="s">
+        <v>474</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F2" s="91" t="s">
+        <v>499</v>
+      </c>
+      <c r="G2" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="H2" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="I2" s="86"/>
+    </row>
+    <row r="3" spans="1:9" ht="31.5" customHeight="1">
+      <c r="A3" s="85" t="s">
+        <v>479</v>
+      </c>
+      <c r="B3" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="88" t="s">
+        <v>480</v>
+      </c>
+      <c r="D3" s="88" t="s">
+        <v>475</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F3" s="91" t="s">
+        <v>499</v>
+      </c>
+      <c r="G3" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="H3" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="I3" s="87" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="23.25" customHeight="1">
+      <c r="A4" s="85" t="s">
+        <v>481</v>
+      </c>
+      <c r="B4" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="88" t="s">
+        <v>482</v>
+      </c>
+      <c r="D4" s="88" t="s">
+        <v>476</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F4" s="91"/>
+      <c r="G4" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="H4" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="I4" s="87" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30">
+      <c r="A5" s="85" t="s">
+        <v>483</v>
+      </c>
+      <c r="B5" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="88" t="s">
+        <v>484</v>
+      </c>
+      <c r="D5" s="88" t="s">
+        <v>513</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F5" s="91" t="s">
+        <v>503</v>
+      </c>
+      <c r="G5" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="H5" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="I5" s="87" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="85" t="s">
+        <v>485</v>
+      </c>
+      <c r="B6" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="88" t="s">
+        <v>486</v>
+      </c>
+      <c r="D6" s="88" t="s">
+        <v>476</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F6" s="91" t="s">
+        <v>499</v>
+      </c>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="I6" s="87" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30">
+      <c r="A7" s="85" t="s">
+        <v>487</v>
+      </c>
+      <c r="B7" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>488</v>
+      </c>
+      <c r="D7" s="88" t="s">
+        <v>513</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F7" s="91" t="s">
+        <v>499</v>
+      </c>
+      <c r="G7" s="85">
+        <v>123</v>
+      </c>
+      <c r="H7" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="I7" s="87" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="85" t="s">
+        <v>489</v>
+      </c>
+      <c r="B8" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="88" t="s">
+        <v>490</v>
+      </c>
+      <c r="D8" s="88" t="s">
+        <v>476</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F8" s="91" t="s">
+        <v>499</v>
+      </c>
+      <c r="G8" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="H8" s="85"/>
+      <c r="I8" s="87" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30">
+      <c r="A9" s="85" t="s">
+        <v>491</v>
+      </c>
+      <c r="B9" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="88" t="s">
+        <v>492</v>
+      </c>
+      <c r="D9" s="88" t="s">
+        <v>512</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F9" s="91" t="s">
+        <v>499</v>
+      </c>
+      <c r="G9" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="H9" s="85">
+        <v>123</v>
+      </c>
+      <c r="I9" s="87" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30">
+      <c r="A10" s="85" t="s">
+        <v>493</v>
+      </c>
+      <c r="B10" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="88" t="s">
+        <v>494</v>
+      </c>
+      <c r="D10" s="88" t="s">
+        <v>513</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F10" s="91" t="s">
+        <v>499</v>
+      </c>
+      <c r="G10" s="85">
+        <v>123</v>
+      </c>
+      <c r="H10" s="85">
+        <v>123</v>
+      </c>
+      <c r="I10" s="87" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30">
+      <c r="A11" s="85" t="s">
+        <v>495</v>
+      </c>
+      <c r="B11" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="88" t="s">
+        <v>496</v>
+      </c>
+      <c r="D11" s="88" t="s">
+        <v>513</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F11" s="91" t="s">
+        <v>499</v>
+      </c>
+      <c r="G11" s="85" t="s">
+        <v>501</v>
+      </c>
+      <c r="H11" s="85" t="s">
+        <v>502</v>
+      </c>
+      <c r="I11" s="87" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="E12" s="82"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet22">
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -6341,8 +6878,8 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Test for change password, done the requested changes
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="515">
   <si>
     <t>Accept</t>
   </si>
@@ -1651,9 +1651,6 @@
     <t>m6543222</t>
   </si>
   <si>
-    <t>global-alerts:Your password has been changed</t>
-  </si>
-  <si>
     <t>currentPasswordErrors:Please enter your current password</t>
   </si>
   <si>
@@ -1661,22 +1658,6 @@
   </si>
   <si>
     <t>confirmNewPasswordErrors:Please confirm your new password</t>
-  </si>
-  <si>
-    <t>global-alerts:Please correct the errors below.
-currentPasswordErrors:Please enter your current password</t>
-  </si>
-  <si>
-    <t>global-alerts:Please correct the errors below.
-newPasswordEerrors:Password does not meet minimum requirements.</t>
-  </si>
-  <si>
-    <t>global-alerts:Please correct the errors below.
-confirmNewPasswordErrors:Password does not meet minimum requirements.</t>
-  </si>
-  <si>
-    <t>global-alerts:Please correct the errors below.
-confirmNewPasswordErrors:Password and password confirmation do not match</t>
   </si>
   <si>
     <t xml:space="preserve">click update
@@ -1685,6 +1666,28 @@
   <si>
     <t>click update 
 alert</t>
+  </si>
+  <si>
+    <t>globalAlerts</t>
+  </si>
+  <si>
+    <t>globalAlerts:Your password has been changed</t>
+  </si>
+  <si>
+    <t>globalAlerts:Please correct the errors below.
+currentPasswordErrors:Please enter your current password</t>
+  </si>
+  <si>
+    <t>globalAlerts:Please correct the errors below.
+newPasswordEerrors:Password does not meet minimum requirements.</t>
+  </si>
+  <si>
+    <t>globalAlerts:Please correct the errors below.
+confirmNewPasswordErrors:Password does not meet minimum requirements.</t>
+  </si>
+  <si>
+    <t>globalAlerts:Please correct the errors below.
+confirmNewPasswordErrors:Password and password confirmation do not match</t>
   </si>
 </sst>
 </file>
@@ -5495,7 +5498,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5537,7 +5540,7 @@
         <v>473</v>
       </c>
       <c r="I1" s="90" t="s">
-        <v>77</v>
+        <v>509</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="24" customHeight="1">
@@ -5593,7 +5596,7 @@
         <v>500</v>
       </c>
       <c r="I3" s="87" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="23.25" customHeight="1">
@@ -5620,7 +5623,7 @@
         <v>500</v>
       </c>
       <c r="I4" s="87" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30">
@@ -5634,7 +5637,7 @@
         <v>484</v>
       </c>
       <c r="D5" s="88" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="E5" s="32" t="s">
         <v>497</v>
@@ -5649,7 +5652,7 @@
         <v>500</v>
       </c>
       <c r="I5" s="87" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -5676,7 +5679,7 @@
         <v>500</v>
       </c>
       <c r="I6" s="87" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30">
@@ -5690,7 +5693,7 @@
         <v>488</v>
       </c>
       <c r="D7" s="88" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="E7" s="32" t="s">
         <v>497</v>
@@ -5705,7 +5708,7 @@
         <v>500</v>
       </c>
       <c r="I7" s="87" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -5732,7 +5735,7 @@
       </c>
       <c r="H8" s="85"/>
       <c r="I8" s="87" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30">
@@ -5746,7 +5749,7 @@
         <v>492</v>
       </c>
       <c r="D9" s="88" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>497</v>
@@ -5761,7 +5764,7 @@
         <v>123</v>
       </c>
       <c r="I9" s="87" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30">
@@ -5775,7 +5778,7 @@
         <v>494</v>
       </c>
       <c r="D10" s="88" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>497</v>
@@ -5790,7 +5793,7 @@
         <v>123</v>
       </c>
       <c r="I10" s="87" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30">
@@ -5804,7 +5807,7 @@
         <v>496</v>
       </c>
       <c r="D11" s="88" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="E11" s="32" t="s">
         <v>497</v>
@@ -5819,7 +5822,7 @@
         <v>502</v>
       </c>
       <c r="I11" s="87" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="12" spans="1:9">

</xml_diff>

<commit_message>
Sorting By price (HTL) fix
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="105705" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="12" activeTab="17"/>
+    <workbookView xWindow="105705" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -1464,9 +1464,6 @@
 old-user</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>WL-01</t>
   </si>
   <si>
@@ -1688,6 +1685,9 @@
   <si>
     <t>globalAlerts:Please correct the errors below.
 confirmNewPasswordErrors:Password and password confirmation do not match</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -2920,16 +2920,16 @@
     </row>
     <row r="2" spans="1:6" ht="30">
       <c r="A2" s="8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="75" t="s">
+        <v>447</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>448</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>449</v>
       </c>
       <c r="E2" s="76" t="s">
         <v>165</v>
@@ -5042,7 +5042,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="83" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B53" s="84" t="s">
         <v>55</v>
@@ -5057,10 +5057,10 @@
         <v>1</v>
       </c>
       <c r="F53" s="64" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G53" s="66" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -5497,7 +5497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -5531,260 +5531,260 @@
         <v>9</v>
       </c>
       <c r="F1" s="89" t="s">
+        <v>470</v>
+      </c>
+      <c r="G1" s="89" t="s">
         <v>471</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="H1" s="89" t="s">
         <v>472</v>
       </c>
-      <c r="H1" s="89" t="s">
-        <v>473</v>
-      </c>
       <c r="I1" s="90" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="24" customHeight="1">
       <c r="A2" s="85" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B2" s="85" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="88" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D2" s="88" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F2" s="91" t="s">
+        <v>498</v>
+      </c>
+      <c r="G2" s="85" t="s">
         <v>499</v>
       </c>
-      <c r="G2" s="85" t="s">
-        <v>500</v>
-      </c>
       <c r="H2" s="85" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I2" s="86"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" customHeight="1">
       <c r="A3" s="85" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B3" s="85" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="88" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D3" s="88" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F3" s="91" t="s">
+        <v>498</v>
+      </c>
+      <c r="G3" s="85" t="s">
         <v>499</v>
       </c>
-      <c r="G3" s="85" t="s">
-        <v>500</v>
-      </c>
       <c r="H3" s="85" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I3" s="87" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="23.25" customHeight="1">
       <c r="A4" s="85" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B4" s="85" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="88" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D4" s="88" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F4" s="91"/>
       <c r="G4" s="85" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H4" s="85" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I4" s="87" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30">
       <c r="A5" s="85" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B5" s="85" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="88" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D5" s="88" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F5" s="91" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G5" s="85" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H5" s="85" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I5" s="87" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="85" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B6" s="85" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="88" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D6" s="88" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F6" s="91" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G6" s="85"/>
       <c r="H6" s="85" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I6" s="87" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30">
       <c r="A7" s="85" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B7" s="85" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="88" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D7" s="88" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F7" s="91" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G7" s="85">
         <v>123</v>
       </c>
       <c r="H7" s="85" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I7" s="87" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="85" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B8" s="85" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="88" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D8" s="88" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F8" s="91" t="s">
+        <v>498</v>
+      </c>
+      <c r="G8" s="85" t="s">
         <v>499</v>
-      </c>
-      <c r="G8" s="85" t="s">
-        <v>500</v>
       </c>
       <c r="H8" s="85"/>
       <c r="I8" s="87" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30">
       <c r="A9" s="85" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B9" s="85" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="88" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D9" s="88" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F9" s="91" t="s">
+        <v>498</v>
+      </c>
+      <c r="G9" s="85" t="s">
         <v>499</v>
-      </c>
-      <c r="G9" s="85" t="s">
-        <v>500</v>
       </c>
       <c r="H9" s="85">
         <v>123</v>
       </c>
       <c r="I9" s="87" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30">
       <c r="A10" s="85" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B10" s="85" t="s">
         <v>47</v>
       </c>
       <c r="C10" s="88" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D10" s="88" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F10" s="91" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G10" s="85">
         <v>123</v>
@@ -5793,36 +5793,36 @@
         <v>123</v>
       </c>
       <c r="I10" s="87" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30">
       <c r="A11" s="85" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B11" s="85" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="88" t="s">
+        <v>495</v>
+      </c>
+      <c r="D11" s="88" t="s">
+        <v>507</v>
+      </c>
+      <c r="E11" s="32" t="s">
         <v>496</v>
       </c>
-      <c r="D11" s="88" t="s">
-        <v>508</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>497</v>
-      </c>
       <c r="F11" s="91" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G11" s="85" t="s">
+        <v>500</v>
+      </c>
+      <c r="H11" s="85" t="s">
         <v>501</v>
       </c>
-      <c r="H11" s="85" t="s">
-        <v>502</v>
-      </c>
       <c r="I11" s="87" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -6616,7 +6616,7 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="90">
       <c r="A2" s="8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
@@ -6625,7 +6625,7 @@
         <v>63</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>234</v>
@@ -6906,109 +6906,109 @@
         <v>10</v>
       </c>
       <c r="E1" s="48" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="47" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B2" s="78" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="47" t="s">
+        <v>452</v>
+      </c>
+      <c r="D2" s="77" t="s">
         <v>453</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="E2" s="77" t="s">
         <v>454</v>
-      </c>
-      <c r="E2" s="77" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45">
       <c r="A3" s="47" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B3" s="78" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="47" t="s">
+        <v>455</v>
+      </c>
+      <c r="D3" s="77" t="s">
         <v>456</v>
       </c>
-      <c r="D3" s="77" t="s">
-        <v>457</v>
-      </c>
       <c r="E3" s="77" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60">
       <c r="A4" s="47" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B4" s="78" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="47" t="s">
+        <v>457</v>
+      </c>
+      <c r="D4" s="77" t="s">
         <v>458</v>
       </c>
-      <c r="D4" s="77" t="s">
-        <v>459</v>
-      </c>
       <c r="E4" s="77" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
       <c r="A5" s="47" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B5" s="78" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D5" s="77" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E5" s="77" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45">
       <c r="A6" s="47" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B6" s="78" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D6" s="77" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E6" s="77" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60">
       <c r="A7" s="47" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B7" s="78" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D7" s="77" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E7" s="77" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -8002,8 +8002,8 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8040,13 +8040,13 @@
         <v>47</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>145</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>446</v>
+        <v>514</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -8057,13 +8057,13 @@
         <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>283</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>446</v>
+        <v>514</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -8080,7 +8080,7 @@
         <v>151</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>446</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed an issue where in the case of trying to change password without typing the current password,results in changing the password and not revert the changes.
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5AB38C0A-3C06-4B2B-8072-9EF8F8306269}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="123615" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="10" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="123615" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="12" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="530">
   <si>
     <t>Accept</t>
   </si>
@@ -1738,11 +1737,20 @@
   <si>
     <t>tester_0052@ocm.com</t>
   </si>
+  <si>
+    <t>click update 
+incorrect Cpassword
+alert</t>
+  </si>
+  <si>
+    <t>click update 
+without Cpassword</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -2333,23 +2341,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2385,23 +2376,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2577,7 +2551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="-0.499984740745262"/>
   </sheetPr>
@@ -2629,7 +2603,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -2786,9 +2760,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -2796,7 +2770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -2818,7 +2792,7 @@
     <col min="8" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7">
       <c r="A1" s="13" t="s">
         <v>61</v>
       </c>
@@ -2894,7 +2868,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -2970,7 +2944,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -3153,7 +3127,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -3218,14 +3192,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3314,19 +3288,21 @@
         <v>456</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="23.25" customHeight="1">
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" s="84" t="s">
         <v>430</v>
       </c>
-      <c r="B4" s="82"/>
+      <c r="B4" s="82" t="s">
+        <v>47</v>
+      </c>
       <c r="C4" s="89" t="s">
         <v>431</v>
       </c>
       <c r="D4" s="85" t="s">
-        <v>425</v>
+        <v>529</v>
       </c>
       <c r="E4" s="82" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F4" s="84" t="s">
         <v>447</v>
@@ -3338,19 +3314,21 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="60">
       <c r="A5" s="84" t="s">
         <v>432</v>
       </c>
-      <c r="B5" s="82"/>
+      <c r="B5" s="82" t="s">
+        <v>47</v>
+      </c>
       <c r="C5" s="89" t="s">
         <v>433</v>
       </c>
       <c r="D5" s="85" t="s">
-        <v>454</v>
+        <v>528</v>
       </c>
       <c r="E5" s="82" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F5" s="84" t="s">
         <v>447</v>
@@ -3366,7 +3344,9 @@
       <c r="A6" s="84" t="s">
         <v>434</v>
       </c>
-      <c r="B6" s="82"/>
+      <c r="B6" s="82" t="s">
+        <v>47</v>
+      </c>
       <c r="C6" s="89" t="s">
         <v>435</v>
       </c>
@@ -3374,7 +3354,7 @@
         <v>425</v>
       </c>
       <c r="E6" s="82" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F6" s="84"/>
       <c r="G6" s="84" t="s">
@@ -3388,7 +3368,9 @@
       <c r="A7" s="84" t="s">
         <v>436</v>
       </c>
-      <c r="B7" s="82"/>
+      <c r="B7" s="82" t="s">
+        <v>47</v>
+      </c>
       <c r="C7" s="89" t="s">
         <v>437</v>
       </c>
@@ -3396,7 +3378,7 @@
         <v>454</v>
       </c>
       <c r="E7" s="82" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F7" s="84">
         <v>123</v>
@@ -3412,7 +3394,9 @@
       <c r="A8" s="84" t="s">
         <v>438</v>
       </c>
-      <c r="B8" s="82"/>
+      <c r="B8" s="82" t="s">
+        <v>47</v>
+      </c>
       <c r="C8" s="89" t="s">
         <v>439</v>
       </c>
@@ -3420,7 +3404,7 @@
         <v>425</v>
       </c>
       <c r="E8" s="82" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F8" s="84" t="s">
         <v>447</v>
@@ -3434,7 +3418,9 @@
       <c r="A9" s="84" t="s">
         <v>440</v>
       </c>
-      <c r="B9" s="82"/>
+      <c r="B9" s="82" t="s">
+        <v>47</v>
+      </c>
       <c r="C9" s="89" t="s">
         <v>441</v>
       </c>
@@ -3442,7 +3428,7 @@
         <v>453</v>
       </c>
       <c r="E9" s="82" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F9" s="84" t="s">
         <v>447</v>
@@ -3466,7 +3452,7 @@
         <v>454</v>
       </c>
       <c r="E10" s="82" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F10" s="84">
         <v>123</v>
@@ -3490,7 +3476,7 @@
         <v>454</v>
       </c>
       <c r="E11" s="82" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F11" s="84" t="s">
         <v>448</v>
@@ -3509,7 +3495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet25">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -4376,14 +4362,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet19">
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5665,65 +5651,65 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0E00-000002000000}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0E00-000003000000}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0E00-000004000000}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0E00-000005000000}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0E00-000006000000}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0E00-000007000000}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0E00-000008000000}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0E00-000009000000}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0E00-00000A000000}"/>
-    <hyperlink ref="F13" r:id="rId12" xr:uid="{00000000-0004-0000-0E00-00000B000000}"/>
-    <hyperlink ref="F14" r:id="rId13" xr:uid="{00000000-0004-0000-0E00-00000C000000}"/>
-    <hyperlink ref="F15" r:id="rId14" xr:uid="{00000000-0004-0000-0E00-00000D000000}"/>
-    <hyperlink ref="F16" r:id="rId15" xr:uid="{00000000-0004-0000-0E00-00000E000000}"/>
-    <hyperlink ref="F17" r:id="rId16" xr:uid="{00000000-0004-0000-0E00-00000F000000}"/>
-    <hyperlink ref="F18" r:id="rId17" xr:uid="{00000000-0004-0000-0E00-000010000000}"/>
-    <hyperlink ref="F19" r:id="rId18" xr:uid="{00000000-0004-0000-0E00-000011000000}"/>
-    <hyperlink ref="F20" r:id="rId19" xr:uid="{00000000-0004-0000-0E00-000012000000}"/>
-    <hyperlink ref="F21" r:id="rId20" xr:uid="{00000000-0004-0000-0E00-000013000000}"/>
-    <hyperlink ref="F22" r:id="rId21" xr:uid="{00000000-0004-0000-0E00-000014000000}"/>
-    <hyperlink ref="F23" r:id="rId22" xr:uid="{00000000-0004-0000-0E00-000015000000}"/>
-    <hyperlink ref="F24" r:id="rId23" xr:uid="{00000000-0004-0000-0E00-000016000000}"/>
-    <hyperlink ref="F25" r:id="rId24" xr:uid="{00000000-0004-0000-0E00-000017000000}"/>
-    <hyperlink ref="F26" r:id="rId25" xr:uid="{00000000-0004-0000-0E00-000018000000}"/>
-    <hyperlink ref="F27" r:id="rId26" xr:uid="{00000000-0004-0000-0E00-000019000000}"/>
-    <hyperlink ref="F28" r:id="rId27" xr:uid="{00000000-0004-0000-0E00-00001A000000}"/>
-    <hyperlink ref="F29" r:id="rId28" xr:uid="{00000000-0004-0000-0E00-00001B000000}"/>
-    <hyperlink ref="F30" r:id="rId29" xr:uid="{00000000-0004-0000-0E00-00001C000000}"/>
-    <hyperlink ref="F31" r:id="rId30" xr:uid="{00000000-0004-0000-0E00-00001D000000}"/>
-    <hyperlink ref="F32" r:id="rId31" xr:uid="{00000000-0004-0000-0E00-00001E000000}"/>
-    <hyperlink ref="F33" r:id="rId32" xr:uid="{00000000-0004-0000-0E00-00001F000000}"/>
-    <hyperlink ref="F34" r:id="rId33" xr:uid="{00000000-0004-0000-0E00-000020000000}"/>
-    <hyperlink ref="F35" r:id="rId34" xr:uid="{00000000-0004-0000-0E00-000021000000}"/>
-    <hyperlink ref="F36" r:id="rId35" xr:uid="{00000000-0004-0000-0E00-000022000000}"/>
-    <hyperlink ref="F37" r:id="rId36" xr:uid="{00000000-0004-0000-0E00-000023000000}"/>
-    <hyperlink ref="F38" r:id="rId37" xr:uid="{00000000-0004-0000-0E00-000024000000}"/>
-    <hyperlink ref="F39" r:id="rId38" xr:uid="{00000000-0004-0000-0E00-000025000000}"/>
-    <hyperlink ref="F40" r:id="rId39" xr:uid="{00000000-0004-0000-0E00-000026000000}"/>
-    <hyperlink ref="F41" r:id="rId40" xr:uid="{00000000-0004-0000-0E00-000027000000}"/>
-    <hyperlink ref="F42" r:id="rId41" xr:uid="{00000000-0004-0000-0E00-000028000000}"/>
-    <hyperlink ref="F43" r:id="rId42" xr:uid="{00000000-0004-0000-0E00-000029000000}"/>
-    <hyperlink ref="F44" r:id="rId43" xr:uid="{00000000-0004-0000-0E00-00002A000000}"/>
-    <hyperlink ref="F45" r:id="rId44" xr:uid="{00000000-0004-0000-0E00-00002B000000}"/>
-    <hyperlink ref="F46" r:id="rId45" xr:uid="{00000000-0004-0000-0E00-00002C000000}"/>
-    <hyperlink ref="F47" r:id="rId46" xr:uid="{00000000-0004-0000-0E00-00002D000000}"/>
-    <hyperlink ref="F48" r:id="rId47" xr:uid="{00000000-0004-0000-0E00-00002E000000}"/>
-    <hyperlink ref="F49" r:id="rId48" xr:uid="{00000000-0004-0000-0E00-00002F000000}"/>
-    <hyperlink ref="F50" r:id="rId49" xr:uid="{00000000-0004-0000-0E00-000030000000}"/>
-    <hyperlink ref="F51" r:id="rId50" xr:uid="{00000000-0004-0000-0E00-000031000000}"/>
-    <hyperlink ref="F52" r:id="rId51" xr:uid="{00000000-0004-0000-0E00-000032000000}"/>
-    <hyperlink ref="G3" r:id="rId52" xr:uid="{00000000-0004-0000-0E00-000033000000}"/>
-    <hyperlink ref="G4" r:id="rId53" display="tester_001@ocm.com" xr:uid="{00000000-0004-0000-0E00-000034000000}"/>
-    <hyperlink ref="G6" r:id="rId54" display="tester_003@ocm.com" xr:uid="{00000000-0004-0000-0E00-000035000000}"/>
-    <hyperlink ref="G53" r:id="rId55" display="tester_0050@ocm.com" xr:uid="{90A5ED5C-5A0B-4E20-B129-BE70E2C3E504}"/>
-    <hyperlink ref="F53" r:id="rId56" xr:uid="{86FC3A4E-AC83-4774-B70D-9DC98DA98841}"/>
-    <hyperlink ref="G7" r:id="rId57" xr:uid="{6A9CAB07-8275-4AD3-ACAF-BC279A954965}"/>
-    <hyperlink ref="F54" r:id="rId58" xr:uid="{E868A8CA-8BEF-426B-8F32-9268DFED2017}"/>
-    <hyperlink ref="F55" r:id="rId59" xr:uid="{91AE7CA6-1EA6-4F9C-996D-FD56841970C9}"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId4"/>
+    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F8" r:id="rId6"/>
+    <hyperlink ref="F9" r:id="rId7"/>
+    <hyperlink ref="F10" r:id="rId8"/>
+    <hyperlink ref="F11" r:id="rId9"/>
+    <hyperlink ref="F12" r:id="rId10"/>
+    <hyperlink ref="F13" r:id="rId11"/>
+    <hyperlink ref="F14" r:id="rId12"/>
+    <hyperlink ref="F15" r:id="rId13"/>
+    <hyperlink ref="F16" r:id="rId14"/>
+    <hyperlink ref="F17" r:id="rId15"/>
+    <hyperlink ref="F18" r:id="rId16"/>
+    <hyperlink ref="F19" r:id="rId17"/>
+    <hyperlink ref="F20" r:id="rId18"/>
+    <hyperlink ref="F21" r:id="rId19"/>
+    <hyperlink ref="F22" r:id="rId20"/>
+    <hyperlink ref="F23" r:id="rId21"/>
+    <hyperlink ref="F24" r:id="rId22"/>
+    <hyperlink ref="F25" r:id="rId23"/>
+    <hyperlink ref="F26" r:id="rId24"/>
+    <hyperlink ref="F27" r:id="rId25"/>
+    <hyperlink ref="F28" r:id="rId26"/>
+    <hyperlink ref="F29" r:id="rId27"/>
+    <hyperlink ref="F30" r:id="rId28"/>
+    <hyperlink ref="F31" r:id="rId29"/>
+    <hyperlink ref="F32" r:id="rId30"/>
+    <hyperlink ref="F33" r:id="rId31"/>
+    <hyperlink ref="F34" r:id="rId32"/>
+    <hyperlink ref="F35" r:id="rId33"/>
+    <hyperlink ref="F36" r:id="rId34"/>
+    <hyperlink ref="F37" r:id="rId35"/>
+    <hyperlink ref="F38" r:id="rId36"/>
+    <hyperlink ref="F39" r:id="rId37"/>
+    <hyperlink ref="F40" r:id="rId38"/>
+    <hyperlink ref="F41" r:id="rId39"/>
+    <hyperlink ref="F42" r:id="rId40"/>
+    <hyperlink ref="F43" r:id="rId41"/>
+    <hyperlink ref="F44" r:id="rId42"/>
+    <hyperlink ref="F45" r:id="rId43"/>
+    <hyperlink ref="F46" r:id="rId44"/>
+    <hyperlink ref="F47" r:id="rId45"/>
+    <hyperlink ref="F48" r:id="rId46"/>
+    <hyperlink ref="F49" r:id="rId47"/>
+    <hyperlink ref="F50" r:id="rId48"/>
+    <hyperlink ref="F51" r:id="rId49"/>
+    <hyperlink ref="F52" r:id="rId50"/>
+    <hyperlink ref="G3" r:id="rId51"/>
+    <hyperlink ref="G4" r:id="rId52" display="tester_001@ocm.com"/>
+    <hyperlink ref="G6" r:id="rId53" display="tester_003@ocm.com"/>
+    <hyperlink ref="G53" r:id="rId54" display="tester_0050@ocm.com"/>
+    <hyperlink ref="F53" r:id="rId55"/>
+    <hyperlink ref="G7" r:id="rId56"/>
+    <hyperlink ref="F54" r:id="rId57"/>
+    <hyperlink ref="F55" r:id="rId58"/>
+    <hyperlink ref="F2" r:id="rId59"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId60"/>
@@ -5731,7 +5717,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet20">
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -5915,7 +5901,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" display="https://ocm-s.com/OCM/bedding/full--full-xl--queen--and-king-bedding/luxurious-tie-dye-duvet-cover-set/p/ds_thd_yds_nav_fqn" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId1" display="https://ocm-s.com/OCM/bedding/full--full-xl--queen--and-king-bedding/luxurious-tie-dye-duvet-cover-set/p/ds_thd_yds_nav_fqn"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -5923,7 +5909,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet23">
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -6097,7 +6083,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="-0.499984740745262"/>
   </sheetPr>
@@ -6192,7 +6178,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet22">
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -6359,7 +6345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -6818,7 +6804,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -7137,7 +7123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -7279,7 +7265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -7739,7 +7725,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -8258,7 +8244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4846C5-6A36-4CE0-A412-B02197969EA2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -8372,7 +8358,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0251AD1-1C72-43A9-886A-E41E0204D5CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>

</xml_diff>

<commit_message>
Checkout changes to make it work on IE adding dynamic add to cart function
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="123615" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="12" activeTab="14"/>
+    <workbookView xWindow="123615" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -1232,9 +1232,6 @@
 Verify order subtotal</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2nd Day</t>
-  </si>
-  <si>
     <t>Overnight</t>
   </si>
   <si>
@@ -1746,12 +1743,15 @@
     <t>click update 
 without Cpassword</t>
   </si>
+  <si>
+    <t>2nd Day</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1789,6 +1789,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Monospace"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1984,7 +1997,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2240,6 +2253,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2812,7 +2831,7 @@
         <v>72</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30">
@@ -2829,13 +2848,13 @@
         <v>139</v>
       </c>
       <c r="E2" s="83" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F2" s="93" t="s">
         <v>53</v>
       </c>
       <c r="G2" s="93" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60">
@@ -2852,13 +2871,13 @@
         <v>142</v>
       </c>
       <c r="E3" s="83" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F3" s="93" t="s">
         <v>53</v>
       </c>
       <c r="G3" s="93" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -3169,16 +3188,16 @@
     </row>
     <row r="2" spans="1:6" ht="30">
       <c r="A2" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="74" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>398</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>399</v>
       </c>
       <c r="E2" s="75" t="s">
         <v>165</v>
@@ -3198,8 +3217,8 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3231,151 +3250,153 @@
         <v>9</v>
       </c>
       <c r="F1" s="86" t="s">
+        <v>420</v>
+      </c>
+      <c r="G1" s="86" t="s">
         <v>421</v>
       </c>
-      <c r="G1" s="86" t="s">
-        <v>422</v>
-      </c>
       <c r="H1" s="87" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1">
       <c r="A2" s="84" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="89" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="89" t="s">
-        <v>427</v>
-      </c>
       <c r="D2" s="85" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E2" s="82" t="s">
         <v>165</v>
       </c>
       <c r="F2" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G2" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H2" s="90"/>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
       <c r="A3" s="84" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B3" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D3" s="85" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E3" s="82" t="s">
         <v>171</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G3" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H3" s="91" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" s="84" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B4" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="89" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D4" s="85" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E4" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F4" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G4" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H4" s="91" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60">
       <c r="A5" s="84" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B5" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D5" s="85" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E5" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F5" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G5" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H5" s="91" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="84" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B6" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="89" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D6" s="85" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E6" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F6" s="84"/>
       <c r="G6" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H6" s="91" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7" s="84" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B7" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="89" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D7" s="85" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E7" s="82" t="s">
         <v>173</v>
@@ -3384,72 +3405,74 @@
         <v>123</v>
       </c>
       <c r="G7" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H7" s="91" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="84" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B8" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="89" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D8" s="85" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E8" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F8" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G8" s="84"/>
       <c r="H8" s="91" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
       <c r="A9" s="84" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B9" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="89" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D9" s="85" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E9" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F9" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G9" s="84">
         <v>123</v>
       </c>
       <c r="H9" s="91" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30">
       <c r="A10" s="84" t="s">
+        <v>441</v>
+      </c>
+      <c r="B10" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="89" t="s">
         <v>442</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="89" t="s">
-        <v>443</v>
-      </c>
       <c r="D10" s="85" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E10" s="82" t="s">
         <v>173</v>
@@ -3461,31 +3484,33 @@
         <v>123</v>
       </c>
       <c r="H10" s="91" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30">
       <c r="A11" s="84" t="s">
+        <v>443</v>
+      </c>
+      <c r="B11" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="89" t="s">
         <v>444</v>
       </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="89" t="s">
-        <v>445</v>
-      </c>
       <c r="D11" s="85" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E11" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F11" s="84" t="s">
+        <v>447</v>
+      </c>
+      <c r="G11" s="84" t="s">
         <v>448</v>
       </c>
-      <c r="G11" s="84" t="s">
-        <v>449</v>
-      </c>
       <c r="H11" s="91" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -3502,7 +3527,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="B3" sqref="B3:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3551,7 +3576,9 @@
       <c r="A2" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="50" t="s">
+        <v>47</v>
+      </c>
       <c r="C2" s="51" t="s">
         <v>234</v>
       </c>
@@ -3576,7 +3603,7 @@
     </row>
     <row r="3" spans="1:9" s="40" customFormat="1">
       <c r="A3" s="20" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="51" t="s">
@@ -3603,7 +3630,7 @@
     </row>
     <row r="4" spans="1:9" s="40" customFormat="1">
       <c r="A4" s="20" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B4" s="50"/>
       <c r="C4" s="51" t="s">
@@ -3630,7 +3657,7 @@
     </row>
     <row r="5" spans="1:9" s="40" customFormat="1">
       <c r="A5" s="20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="51" t="s">
@@ -3657,11 +3684,9 @@
     </row>
     <row r="6" spans="1:9" s="40" customFormat="1">
       <c r="A6" s="20" t="s">
-        <v>385</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>47</v>
-      </c>
+        <v>384</v>
+      </c>
+      <c r="B6" s="50"/>
       <c r="C6" s="51" t="s">
         <v>234</v>
       </c>
@@ -3686,7 +3711,7 @@
     </row>
     <row r="7" spans="1:9" s="40" customFormat="1">
       <c r="A7" s="20" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="51" t="s">
@@ -3713,7 +3738,7 @@
     </row>
     <row r="8" spans="1:9" s="40" customFormat="1">
       <c r="A8" s="20" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="51" t="s">
@@ -3740,7 +3765,7 @@
     </row>
     <row r="9" spans="1:9" s="40" customFormat="1">
       <c r="A9" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="51" t="s">
@@ -3767,7 +3792,7 @@
     </row>
     <row r="10" spans="1:9" s="40" customFormat="1">
       <c r="A10" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="51" t="s">
@@ -3794,7 +3819,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="51" t="s">
@@ -3821,7 +3846,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="51" t="s">
@@ -3848,7 +3873,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B13" s="50"/>
       <c r="C13" s="51" t="s">
@@ -3875,7 +3900,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B14" s="50"/>
       <c r="C14" s="51" t="s">
@@ -3902,7 +3927,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="20" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B15" s="50"/>
       <c r="C15" s="51" t="s">
@@ -3929,7 +3954,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="20" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B16" s="50"/>
       <c r="C16" s="51" t="s">
@@ -3956,7 +3981,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="20" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B17" s="50"/>
       <c r="C17" s="51" t="s">
@@ -3978,7 +4003,7 @@
         <v>53</v>
       </c>
       <c r="I17" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -4369,7 +4394,7 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4385,25 +4410,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="96" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4427,7 +4452,7 @@
         <v>292</v>
       </c>
       <c r="G2" s="61" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4473,7 +4498,7 @@
         <v>292</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4496,7 +4521,7 @@
         <v>292</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4519,7 +4544,7 @@
         <v>292</v>
       </c>
       <c r="G6" s="65" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4542,7 +4567,7 @@
         <v>292</v>
       </c>
       <c r="G7" s="92" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4565,7 +4590,7 @@
         <v>292</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4588,7 +4613,7 @@
         <v>292</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4611,7 +4636,7 @@
         <v>292</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4634,7 +4659,7 @@
         <v>292</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -4657,7 +4682,7 @@
         <v>292</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4680,7 +4705,7 @@
         <v>292</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4703,7 +4728,7 @@
         <v>292</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4726,7 +4751,7 @@
         <v>292</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4749,7 +4774,7 @@
         <v>292</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -4772,7 +4797,7 @@
         <v>292</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -4795,7 +4820,7 @@
         <v>292</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4818,7 +4843,7 @@
         <v>292</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -4841,7 +4866,7 @@
         <v>292</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4864,7 +4889,7 @@
         <v>292</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -4887,7 +4912,7 @@
         <v>292</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -4910,7 +4935,7 @@
         <v>292</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -4933,7 +4958,7 @@
         <v>292</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -4956,7 +4981,7 @@
         <v>292</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -5002,7 +5027,7 @@
         <v>292</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -5025,7 +5050,7 @@
         <v>292</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -5048,7 +5073,7 @@
         <v>292</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -5071,7 +5096,7 @@
         <v>292</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -5094,7 +5119,7 @@
         <v>292</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5117,7 +5142,7 @@
         <v>292</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -5140,7 +5165,7 @@
         <v>292</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -5163,7 +5188,7 @@
         <v>292</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -5186,7 +5211,7 @@
         <v>292</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -5209,7 +5234,7 @@
         <v>292</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -5232,7 +5257,7 @@
         <v>292</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -5255,7 +5280,7 @@
         <v>292</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -5278,7 +5303,7 @@
         <v>292</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -5301,7 +5326,7 @@
         <v>292</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -5324,7 +5349,7 @@
         <v>292</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -5347,7 +5372,7 @@
         <v>292</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -5370,7 +5395,7 @@
         <v>292</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -5393,7 +5418,7 @@
         <v>292</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -5416,7 +5441,7 @@
         <v>292</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -5439,7 +5464,7 @@
         <v>292</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -5462,7 +5487,7 @@
         <v>292</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -5485,7 +5510,7 @@
         <v>292</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -5508,7 +5533,7 @@
         <v>292</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -5531,7 +5556,7 @@
         <v>292</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -5554,7 +5579,7 @@
         <v>292</v>
       </c>
       <c r="G51" s="81" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -5577,12 +5602,12 @@
         <v>292</v>
       </c>
       <c r="G52" s="81" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B53" s="83" t="s">
         <v>55</v>
@@ -5600,12 +5625,12 @@
         <v>292</v>
       </c>
       <c r="G53" s="65" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="82" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B54" s="83" t="s">
         <v>55</v>
@@ -5623,12 +5648,12 @@
         <v>292</v>
       </c>
       <c r="G54" s="46" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="82" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B55" s="83" t="s">
         <v>55</v>
@@ -5646,7 +5671,7 @@
         <v>292</v>
       </c>
       <c r="G55" s="46" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -5704,7 +5729,7 @@
     <hyperlink ref="G3" r:id="rId51"/>
     <hyperlink ref="G4" r:id="rId52" display="tester_001@ocm.com"/>
     <hyperlink ref="G6" r:id="rId53" display="tester_003@ocm.com"/>
-    <hyperlink ref="G53" r:id="rId54" display="tester_0050@ocm.com"/>
+    <hyperlink ref="G53" r:id="rId54"/>
     <hyperlink ref="F53" r:id="rId55"/>
     <hyperlink ref="G7" r:id="rId56"/>
     <hyperlink ref="F54" r:id="rId57"/>
@@ -5724,7 +5749,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6032,7 +6057,7 @@
         <v>55</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>52</v>
@@ -6229,10 +6254,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>41</v>
@@ -6249,10 +6274,10 @@
         <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>42</v>
@@ -6269,10 +6294,10 @@
         <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>43</v>
@@ -6289,10 +6314,10 @@
         <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>44</v>
@@ -6309,10 +6334,10 @@
         <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>45</v>
@@ -6320,10 +6345,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" s="73" t="s">
         <v>376</v>
-      </c>
-      <c r="B7" s="73" t="s">
-        <v>377</v>
       </c>
       <c r="C7" s="46">
         <v>1</v>
@@ -6335,7 +6360,7 @@
         <v>66</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -6352,7 +6377,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6414,16 +6439,16 @@
         <v>63</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>53</v>
@@ -6433,7 +6458,7 @@
       </c>
       <c r="J2" s="32"/>
       <c r="K2" s="32" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="60">
@@ -6447,13 +6472,13 @@
         <v>64</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G3" s="31" t="s">
         <v>231</v>
@@ -6480,13 +6505,13 @@
         <v>15</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G4" s="31" t="s">
         <v>232</v>
@@ -6513,13 +6538,13 @@
         <v>15</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>370</v>
+        <v>529</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>231</v>
@@ -6546,13 +6571,13 @@
         <v>65</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>370</v>
+        <v>529</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>231</v>
@@ -6572,23 +6597,21 @@
       <c r="A7" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H7" s="32" t="s">
         <v>53</v>
@@ -6605,20 +6628,18 @@
       <c r="A8" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
         <v>64</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>231</v>
@@ -6638,20 +6659,18 @@
       <c r="A9" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>232</v>
@@ -6864,7 +6883,7 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="90">
       <c r="A2" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
@@ -6873,13 +6892,13 @@
         <v>63</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>234</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G2" s="31" t="s">
         <v>231</v>
@@ -7154,109 +7173,109 @@
         <v>10</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="46" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B2" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="46" t="s">
+        <v>402</v>
+      </c>
+      <c r="D2" s="76" t="s">
         <v>403</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="E2" s="76" t="s">
         <v>404</v>
-      </c>
-      <c r="E2" s="76" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45">
       <c r="A3" s="46" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B3" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="46" t="s">
+        <v>405</v>
+      </c>
+      <c r="D3" s="76" t="s">
         <v>406</v>
       </c>
-      <c r="D3" s="76" t="s">
-        <v>407</v>
-      </c>
       <c r="E3" s="76" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60">
       <c r="A4" s="46" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B4" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="46" t="s">
+        <v>407</v>
+      </c>
+      <c r="D4" s="76" t="s">
         <v>408</v>
       </c>
-      <c r="D4" s="76" t="s">
-        <v>409</v>
-      </c>
       <c r="E4" s="76" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
       <c r="A5" s="46" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B5" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D5" s="76" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E5" s="76" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45">
       <c r="A6" s="46" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B6" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D6" s="76" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E6" s="76" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60">
       <c r="A7" s="46" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B7" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D7" s="76" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E7" s="76" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -7731,8 +7750,8 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7789,7 +7808,9 @@
       <c r="A2" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="32" t="s">
+        <v>47</v>
+      </c>
       <c r="C2" s="33" t="s">
         <v>362</v>
       </c>
@@ -7797,7 +7818,7 @@
         <v>351</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F2" s="33"/>
       <c r="G2" s="32"/>
@@ -8183,9 +8204,7 @@
       <c r="A16" s="48" t="s">
         <v>360</v>
       </c>
-      <c r="B16" s="32" t="s">
-        <v>47</v>
-      </c>
+      <c r="B16" s="32"/>
       <c r="C16" s="33" t="s">
         <v>132</v>
       </c>
@@ -8299,7 +8318,7 @@
         <v>362</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E2" s="32" t="s">
         <v>234</v>
@@ -8320,7 +8339,7 @@
         <v>132</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>234</v>
@@ -8341,7 +8360,7 @@
         <v>132</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>234</v>
@@ -8412,10 +8431,10 @@
         <v>145</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F2" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -8432,10 +8451,10 @@
         <v>283</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F3" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -8452,15 +8471,15 @@
         <v>151</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F4" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>47</v>
@@ -8469,18 +8488,18 @@
         <v>75</v>
       </c>
       <c r="D5" s="88" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F5" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>47</v>
@@ -8489,18 +8508,18 @@
         <v>74</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F6" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30">
       <c r="A7" s="8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>47</v>
@@ -8509,13 +8528,13 @@
         <v>150</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F7" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix users per browsers
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CB96F23A-70B4-4E3C-993D-78508B2D9396}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F2485F6F-08FD-4B26-99A5-EA4D865CC1A9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="141285" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="142215" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="10" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -1544,102 +1544,6 @@
     <t>mobile_Nexus 5</t>
   </si>
   <si>
-    <t>auto_001@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_002@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_003@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_004@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_005@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_006@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_007@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_008@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_009@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0010@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0011@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0012@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0013@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0014@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0015@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0016@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0017@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0018@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0019@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0020@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0021@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0022@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0023@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0024@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0025@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0026@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0027@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0028@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0029@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0030@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0031@ocm.com</t>
-  </si>
-  <si>
-    <t>auto_0032@ocm.com</t>
-  </si>
-  <si>
     <t>AC-17</t>
   </si>
   <si>
@@ -1689,6 +1593,102 @@
   </si>
   <si>
     <t>2nd Day</t>
+  </si>
+  <si>
+    <t>auto_tester_001@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_002@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_003@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_004@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_005@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_006@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_007@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_008@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_009@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0010@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0011@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0012@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0013@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0014@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0015@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0016@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0017@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0018@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0019@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0020@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0021@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0022@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0023@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0024@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0025@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0026@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0027@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0028@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0029@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0030@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0031@ocm.com</t>
+  </si>
+  <si>
+    <t>auto_tester_0032@ocm.com</t>
   </si>
 </sst>
 </file>
@@ -3448,8 +3448,8 @@
   </sheetPr>
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B33"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3960,7 +3960,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="20" t="s">
-        <v>494</v>
+        <v>462</v>
       </c>
       <c r="B18" s="50" t="s">
         <v>47</v>
@@ -3989,7 +3989,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="20" t="s">
-        <v>495</v>
+        <v>463</v>
       </c>
       <c r="B19" s="50" t="s">
         <v>47</v>
@@ -4018,7 +4018,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="20" t="s">
-        <v>496</v>
+        <v>464</v>
       </c>
       <c r="B20" s="50" t="s">
         <v>47</v>
@@ -4047,7 +4047,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="20" t="s">
-        <v>497</v>
+        <v>465</v>
       </c>
       <c r="B21" s="50" t="s">
         <v>47</v>
@@ -4076,7 +4076,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="20" t="s">
-        <v>498</v>
+        <v>466</v>
       </c>
       <c r="B22" s="50" t="s">
         <v>47</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="20" t="s">
-        <v>499</v>
+        <v>467</v>
       </c>
       <c r="B23" s="50" t="s">
         <v>47</v>
@@ -4134,7 +4134,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="20" t="s">
-        <v>500</v>
+        <v>468</v>
       </c>
       <c r="B24" s="50" t="s">
         <v>47</v>
@@ -4163,7 +4163,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="20" t="s">
-        <v>501</v>
+        <v>469</v>
       </c>
       <c r="B25" s="50" t="s">
         <v>47</v>
@@ -4192,7 +4192,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="20" t="s">
-        <v>502</v>
+        <v>470</v>
       </c>
       <c r="B26" s="50" t="s">
         <v>47</v>
@@ -4221,7 +4221,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="20" t="s">
-        <v>503</v>
+        <v>471</v>
       </c>
       <c r="B27" s="50" t="s">
         <v>47</v>
@@ -4250,7 +4250,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="20" t="s">
-        <v>504</v>
+        <v>472</v>
       </c>
       <c r="B28" s="50" t="s">
         <v>47</v>
@@ -4279,7 +4279,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="20" t="s">
-        <v>505</v>
+        <v>473</v>
       </c>
       <c r="B29" s="50" t="s">
         <v>47</v>
@@ -4308,7 +4308,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="20" t="s">
-        <v>506</v>
+        <v>474</v>
       </c>
       <c r="B30" s="50" t="s">
         <v>47</v>
@@ -4337,7 +4337,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="20" t="s">
-        <v>507</v>
+        <v>475</v>
       </c>
       <c r="B31" s="50" t="s">
         <v>47</v>
@@ -4366,7 +4366,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="20" t="s">
-        <v>508</v>
+        <v>476</v>
       </c>
       <c r="B32" s="50" t="s">
         <v>47</v>
@@ -4395,7 +4395,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="20" t="s">
-        <v>509</v>
+        <v>477</v>
       </c>
       <c r="B33" s="50" t="s">
         <v>47</v>
@@ -4633,8 +4633,8 @@
   </sheetPr>
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4645,7 +4645,7 @@
     <col min="4" max="4" width="9.85546875" style="34" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="9.42578125" style="34" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="12.28515625" style="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.28515625" style="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.7109375" style="34" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
@@ -4692,7 +4692,7 @@
         <v>272</v>
       </c>
       <c r="G2" s="63" t="s">
-        <v>462</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4715,7 +4715,7 @@
         <v>272</v>
       </c>
       <c r="G3" s="63" t="s">
-        <v>463</v>
+        <v>480</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4738,7 +4738,7 @@
         <v>272</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4761,7 +4761,7 @@
         <v>272</v>
       </c>
       <c r="G5" s="63" t="s">
-        <v>465</v>
+        <v>482</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4784,7 +4784,7 @@
         <v>272</v>
       </c>
       <c r="G6" s="59" t="s">
-        <v>466</v>
+        <v>483</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4807,7 +4807,7 @@
         <v>272</v>
       </c>
       <c r="G7" s="63" t="s">
-        <v>467</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4830,7 +4830,7 @@
         <v>272</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>468</v>
+        <v>485</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4853,7 +4853,7 @@
         <v>272</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>469</v>
+        <v>486</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4876,7 +4876,7 @@
         <v>272</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>470</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4899,7 +4899,7 @@
         <v>272</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>471</v>
+        <v>488</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -4922,7 +4922,7 @@
         <v>272</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>472</v>
+        <v>489</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4945,7 +4945,7 @@
         <v>272</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>473</v>
+        <v>490</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4968,7 +4968,7 @@
         <v>272</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>474</v>
+        <v>491</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4991,7 +4991,7 @@
         <v>272</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>475</v>
+        <v>492</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -5014,7 +5014,7 @@
         <v>272</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>476</v>
+        <v>493</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -5037,7 +5037,7 @@
         <v>272</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>477</v>
+        <v>494</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -5060,7 +5060,7 @@
         <v>272</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>478</v>
+        <v>495</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -5083,7 +5083,7 @@
         <v>272</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>479</v>
+        <v>496</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -5106,7 +5106,7 @@
         <v>272</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>480</v>
+        <v>497</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -5129,7 +5129,7 @@
         <v>272</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>481</v>
+        <v>498</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -5152,7 +5152,7 @@
         <v>272</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>482</v>
+        <v>499</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -5175,7 +5175,7 @@
         <v>272</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>483</v>
+        <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -5198,7 +5198,7 @@
         <v>272</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>484</v>
+        <v>501</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -5221,7 +5221,7 @@
         <v>272</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>485</v>
+        <v>502</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -5244,7 +5244,7 @@
         <v>272</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>486</v>
+        <v>503</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -5267,7 +5267,7 @@
         <v>272</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>487</v>
+        <v>504</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -5290,7 +5290,7 @@
         <v>272</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>488</v>
+        <v>505</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -5313,7 +5313,7 @@
         <v>272</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>489</v>
+        <v>506</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -5336,7 +5336,7 @@
         <v>272</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>490</v>
+        <v>507</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -5359,7 +5359,7 @@
         <v>272</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>491</v>
+        <v>508</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5382,7 +5382,7 @@
         <v>272</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>492</v>
+        <v>509</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -5405,7 +5405,7 @@
         <v>272</v>
       </c>
       <c r="G33" s="63" t="s">
-        <v>493</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -5442,7 +5442,7 @@
     <hyperlink ref="F32" r:id="rId30" xr:uid="{00000000-0004-0000-1000-00001D000000}"/>
     <hyperlink ref="F33" r:id="rId31" xr:uid="{00000000-0004-0000-1000-00001E000000}"/>
     <hyperlink ref="F2" r:id="rId32" xr:uid="{00000000-0004-0000-1000-00003A000000}"/>
-    <hyperlink ref="G33" r:id="rId33" xr:uid="{B67C255D-F8C7-4B1E-B042-5C06CEDEE13E}"/>
+    <hyperlink ref="G33" r:id="rId33" display="auto_0032@ocm.com" xr:uid="{B67C255D-F8C7-4B1E-B042-5C06CEDEE13E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId34"/>
@@ -6254,7 +6254,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>510</v>
+        <v>478</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>231</v>
@@ -6285,7 +6285,7 @@
         <v>234</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>510</v>
+        <v>478</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
Checkout changes to make it work on IE,
adding dynamic add to cart function
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="123615" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="12" activeTab="14"/>
+    <workbookView xWindow="123615" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -1232,9 +1232,6 @@
 Verify order subtotal</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2nd Day</t>
-  </si>
-  <si>
     <t>Overnight</t>
   </si>
   <si>
@@ -1746,12 +1743,15 @@
     <t>click update 
 without Cpassword</t>
   </si>
+  <si>
+    <t>2nd Day</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1789,6 +1789,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Monospace"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1984,7 +1997,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2240,6 +2253,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2812,7 +2831,7 @@
         <v>72</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30">
@@ -2829,13 +2848,13 @@
         <v>139</v>
       </c>
       <c r="E2" s="83" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F2" s="93" t="s">
         <v>53</v>
       </c>
       <c r="G2" s="93" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60">
@@ -2852,13 +2871,13 @@
         <v>142</v>
       </c>
       <c r="E3" s="83" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F3" s="93" t="s">
         <v>53</v>
       </c>
       <c r="G3" s="93" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -3169,16 +3188,16 @@
     </row>
     <row r="2" spans="1:6" ht="30">
       <c r="A2" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="74" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>398</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>399</v>
       </c>
       <c r="E2" s="75" t="s">
         <v>165</v>
@@ -3198,8 +3217,8 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3231,151 +3250,153 @@
         <v>9</v>
       </c>
       <c r="F1" s="86" t="s">
+        <v>420</v>
+      </c>
+      <c r="G1" s="86" t="s">
         <v>421</v>
       </c>
-      <c r="G1" s="86" t="s">
-        <v>422</v>
-      </c>
       <c r="H1" s="87" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1">
       <c r="A2" s="84" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="89" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="89" t="s">
-        <v>427</v>
-      </c>
       <c r="D2" s="85" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E2" s="82" t="s">
         <v>165</v>
       </c>
       <c r="F2" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G2" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H2" s="90"/>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
       <c r="A3" s="84" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B3" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D3" s="85" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E3" s="82" t="s">
         <v>171</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G3" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H3" s="91" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" s="84" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B4" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="89" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D4" s="85" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E4" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F4" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G4" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H4" s="91" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60">
       <c r="A5" s="84" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B5" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D5" s="85" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E5" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F5" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G5" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H5" s="91" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="84" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B6" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="89" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D6" s="85" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E6" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F6" s="84"/>
       <c r="G6" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H6" s="91" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7" s="84" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B7" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="89" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D7" s="85" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E7" s="82" t="s">
         <v>173</v>
@@ -3384,72 +3405,74 @@
         <v>123</v>
       </c>
       <c r="G7" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H7" s="91" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="84" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B8" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="89" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D8" s="85" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E8" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F8" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G8" s="84"/>
       <c r="H8" s="91" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
       <c r="A9" s="84" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B9" s="82" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="89" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D9" s="85" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E9" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F9" s="84" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G9" s="84">
         <v>123</v>
       </c>
       <c r="H9" s="91" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30">
       <c r="A10" s="84" t="s">
+        <v>441</v>
+      </c>
+      <c r="B10" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="89" t="s">
         <v>442</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="89" t="s">
-        <v>443</v>
-      </c>
       <c r="D10" s="85" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E10" s="82" t="s">
         <v>173</v>
@@ -3461,31 +3484,33 @@
         <v>123</v>
       </c>
       <c r="H10" s="91" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30">
       <c r="A11" s="84" t="s">
+        <v>443</v>
+      </c>
+      <c r="B11" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="89" t="s">
         <v>444</v>
       </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="89" t="s">
-        <v>445</v>
-      </c>
       <c r="D11" s="85" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E11" s="82" t="s">
         <v>173</v>
       </c>
       <c r="F11" s="84" t="s">
+        <v>447</v>
+      </c>
+      <c r="G11" s="84" t="s">
         <v>448</v>
       </c>
-      <c r="G11" s="84" t="s">
-        <v>449</v>
-      </c>
       <c r="H11" s="91" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -3502,7 +3527,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="B3" sqref="B3:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3551,7 +3576,9 @@
       <c r="A2" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="50" t="s">
+        <v>47</v>
+      </c>
       <c r="C2" s="51" t="s">
         <v>234</v>
       </c>
@@ -3576,7 +3603,7 @@
     </row>
     <row r="3" spans="1:9" s="40" customFormat="1">
       <c r="A3" s="20" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="51" t="s">
@@ -3603,7 +3630,7 @@
     </row>
     <row r="4" spans="1:9" s="40" customFormat="1">
       <c r="A4" s="20" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B4" s="50"/>
       <c r="C4" s="51" t="s">
@@ -3630,7 +3657,7 @@
     </row>
     <row r="5" spans="1:9" s="40" customFormat="1">
       <c r="A5" s="20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="51" t="s">
@@ -3657,11 +3684,9 @@
     </row>
     <row r="6" spans="1:9" s="40" customFormat="1">
       <c r="A6" s="20" t="s">
-        <v>385</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>47</v>
-      </c>
+        <v>384</v>
+      </c>
+      <c r="B6" s="50"/>
       <c r="C6" s="51" t="s">
         <v>234</v>
       </c>
@@ -3686,7 +3711,7 @@
     </row>
     <row r="7" spans="1:9" s="40" customFormat="1">
       <c r="A7" s="20" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="51" t="s">
@@ -3713,7 +3738,7 @@
     </row>
     <row r="8" spans="1:9" s="40" customFormat="1">
       <c r="A8" s="20" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="51" t="s">
@@ -3740,7 +3765,7 @@
     </row>
     <row r="9" spans="1:9" s="40" customFormat="1">
       <c r="A9" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="51" t="s">
@@ -3767,7 +3792,7 @@
     </row>
     <row r="10" spans="1:9" s="40" customFormat="1">
       <c r="A10" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="51" t="s">
@@ -3794,7 +3819,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="51" t="s">
@@ -3821,7 +3846,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="51" t="s">
@@ -3848,7 +3873,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B13" s="50"/>
       <c r="C13" s="51" t="s">
@@ -3875,7 +3900,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B14" s="50"/>
       <c r="C14" s="51" t="s">
@@ -3902,7 +3927,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="20" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B15" s="50"/>
       <c r="C15" s="51" t="s">
@@ -3929,7 +3954,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="20" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B16" s="50"/>
       <c r="C16" s="51" t="s">
@@ -3956,7 +3981,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="20" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B17" s="50"/>
       <c r="C17" s="51" t="s">
@@ -3978,7 +4003,7 @@
         <v>53</v>
       </c>
       <c r="I17" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -4369,7 +4394,7 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4385,25 +4410,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="96" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4427,7 +4452,7 @@
         <v>292</v>
       </c>
       <c r="G2" s="61" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4473,7 +4498,7 @@
         <v>292</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4496,7 +4521,7 @@
         <v>292</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4519,7 +4544,7 @@
         <v>292</v>
       </c>
       <c r="G6" s="65" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4542,7 +4567,7 @@
         <v>292</v>
       </c>
       <c r="G7" s="92" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4565,7 +4590,7 @@
         <v>292</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4588,7 +4613,7 @@
         <v>292</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4611,7 +4636,7 @@
         <v>292</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4634,7 +4659,7 @@
         <v>292</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -4657,7 +4682,7 @@
         <v>292</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4680,7 +4705,7 @@
         <v>292</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4703,7 +4728,7 @@
         <v>292</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4726,7 +4751,7 @@
         <v>292</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4749,7 +4774,7 @@
         <v>292</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -4772,7 +4797,7 @@
         <v>292</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -4795,7 +4820,7 @@
         <v>292</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4818,7 +4843,7 @@
         <v>292</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -4841,7 +4866,7 @@
         <v>292</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4864,7 +4889,7 @@
         <v>292</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -4887,7 +4912,7 @@
         <v>292</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -4910,7 +4935,7 @@
         <v>292</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -4933,7 +4958,7 @@
         <v>292</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -4956,7 +4981,7 @@
         <v>292</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -5002,7 +5027,7 @@
         <v>292</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -5025,7 +5050,7 @@
         <v>292</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -5048,7 +5073,7 @@
         <v>292</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -5071,7 +5096,7 @@
         <v>292</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -5094,7 +5119,7 @@
         <v>292</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5117,7 +5142,7 @@
         <v>292</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -5140,7 +5165,7 @@
         <v>292</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -5163,7 +5188,7 @@
         <v>292</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -5186,7 +5211,7 @@
         <v>292</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -5209,7 +5234,7 @@
         <v>292</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -5232,7 +5257,7 @@
         <v>292</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -5255,7 +5280,7 @@
         <v>292</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -5278,7 +5303,7 @@
         <v>292</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -5301,7 +5326,7 @@
         <v>292</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -5324,7 +5349,7 @@
         <v>292</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -5347,7 +5372,7 @@
         <v>292</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -5370,7 +5395,7 @@
         <v>292</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -5393,7 +5418,7 @@
         <v>292</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -5416,7 +5441,7 @@
         <v>292</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -5439,7 +5464,7 @@
         <v>292</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -5462,7 +5487,7 @@
         <v>292</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -5485,7 +5510,7 @@
         <v>292</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -5508,7 +5533,7 @@
         <v>292</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -5531,7 +5556,7 @@
         <v>292</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -5554,7 +5579,7 @@
         <v>292</v>
       </c>
       <c r="G51" s="81" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -5577,12 +5602,12 @@
         <v>292</v>
       </c>
       <c r="G52" s="81" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B53" s="83" t="s">
         <v>55</v>
@@ -5600,12 +5625,12 @@
         <v>292</v>
       </c>
       <c r="G53" s="65" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="82" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B54" s="83" t="s">
         <v>55</v>
@@ -5623,12 +5648,12 @@
         <v>292</v>
       </c>
       <c r="G54" s="46" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="82" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B55" s="83" t="s">
         <v>55</v>
@@ -5646,7 +5671,7 @@
         <v>292</v>
       </c>
       <c r="G55" s="46" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -5704,7 +5729,7 @@
     <hyperlink ref="G3" r:id="rId51"/>
     <hyperlink ref="G4" r:id="rId52" display="tester_001@ocm.com"/>
     <hyperlink ref="G6" r:id="rId53" display="tester_003@ocm.com"/>
-    <hyperlink ref="G53" r:id="rId54" display="tester_0050@ocm.com"/>
+    <hyperlink ref="G53" r:id="rId54"/>
     <hyperlink ref="F53" r:id="rId55"/>
     <hyperlink ref="G7" r:id="rId56"/>
     <hyperlink ref="F54" r:id="rId57"/>
@@ -5724,7 +5749,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6032,7 +6057,7 @@
         <v>55</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>52</v>
@@ -6229,10 +6254,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>41</v>
@@ -6249,10 +6274,10 @@
         <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>42</v>
@@ -6269,10 +6294,10 @@
         <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>43</v>
@@ -6289,10 +6314,10 @@
         <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>44</v>
@@ -6309,10 +6334,10 @@
         <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>45</v>
@@ -6320,10 +6345,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" s="73" t="s">
         <v>376</v>
-      </c>
-      <c r="B7" s="73" t="s">
-        <v>377</v>
       </c>
       <c r="C7" s="46">
         <v>1</v>
@@ -6335,7 +6360,7 @@
         <v>66</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -6352,7 +6377,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6414,16 +6439,16 @@
         <v>63</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>53</v>
@@ -6433,7 +6458,7 @@
       </c>
       <c r="J2" s="32"/>
       <c r="K2" s="32" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="60">
@@ -6447,13 +6472,13 @@
         <v>64</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G3" s="31" t="s">
         <v>231</v>
@@ -6480,13 +6505,13 @@
         <v>15</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G4" s="31" t="s">
         <v>232</v>
@@ -6513,13 +6538,13 @@
         <v>15</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>370</v>
+        <v>529</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>231</v>
@@ -6546,13 +6571,13 @@
         <v>65</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>370</v>
+        <v>529</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>231</v>
@@ -6572,23 +6597,21 @@
       <c r="A7" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H7" s="32" t="s">
         <v>53</v>
@@ -6605,20 +6628,18 @@
       <c r="A8" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
         <v>64</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>231</v>
@@ -6638,20 +6659,18 @@
       <c r="A9" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>232</v>
@@ -6864,7 +6883,7 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="90">
       <c r="A2" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
@@ -6873,13 +6892,13 @@
         <v>63</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>234</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G2" s="31" t="s">
         <v>231</v>
@@ -7154,109 +7173,109 @@
         <v>10</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="46" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B2" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="46" t="s">
+        <v>402</v>
+      </c>
+      <c r="D2" s="76" t="s">
         <v>403</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="E2" s="76" t="s">
         <v>404</v>
-      </c>
-      <c r="E2" s="76" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45">
       <c r="A3" s="46" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B3" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="46" t="s">
+        <v>405</v>
+      </c>
+      <c r="D3" s="76" t="s">
         <v>406</v>
       </c>
-      <c r="D3" s="76" t="s">
-        <v>407</v>
-      </c>
       <c r="E3" s="76" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60">
       <c r="A4" s="46" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B4" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="46" t="s">
+        <v>407</v>
+      </c>
+      <c r="D4" s="76" t="s">
         <v>408</v>
       </c>
-      <c r="D4" s="76" t="s">
-        <v>409</v>
-      </c>
       <c r="E4" s="76" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
       <c r="A5" s="46" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B5" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D5" s="76" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E5" s="76" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45">
       <c r="A6" s="46" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B6" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D6" s="76" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E6" s="76" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60">
       <c r="A7" s="46" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B7" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D7" s="76" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E7" s="76" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -7731,8 +7750,8 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7789,7 +7808,9 @@
       <c r="A2" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="32" t="s">
+        <v>47</v>
+      </c>
       <c r="C2" s="33" t="s">
         <v>362</v>
       </c>
@@ -7797,7 +7818,7 @@
         <v>351</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F2" s="33"/>
       <c r="G2" s="32"/>
@@ -8183,9 +8204,7 @@
       <c r="A16" s="48" t="s">
         <v>360</v>
       </c>
-      <c r="B16" s="32" t="s">
-        <v>47</v>
-      </c>
+      <c r="B16" s="32"/>
       <c r="C16" s="33" t="s">
         <v>132</v>
       </c>
@@ -8299,7 +8318,7 @@
         <v>362</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E2" s="32" t="s">
         <v>234</v>
@@ -8320,7 +8339,7 @@
         <v>132</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>234</v>
@@ -8341,7 +8360,7 @@
         <v>132</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>234</v>
@@ -8412,10 +8431,10 @@
         <v>145</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F2" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -8432,10 +8451,10 @@
         <v>283</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F3" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -8452,15 +8471,15 @@
         <v>151</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F4" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>47</v>
@@ -8469,18 +8488,18 @@
         <v>75</v>
       </c>
       <c r="D5" s="88" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F5" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>47</v>
@@ -8489,18 +8508,18 @@
         <v>74</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F6" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30">
       <c r="A7" s="8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>47</v>
@@ -8509,13 +8528,13 @@
         <v>150</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F7" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes for screen shot
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1E67C636-324B-4976-BB09-B0CDCC4407A2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0816BB33-0D4A-4CCA-806A-ABBD6A02F1A8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="174120" yWindow="0" windowWidth="17790" windowHeight="5610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="175050" yWindow="0" windowWidth="17790" windowHeight="5610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="499">
   <si>
     <t>Accept</t>
   </si>
@@ -2457,7 +2457,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2485,17 +2485,13 @@
       <c r="A3" s="78" t="s">
         <v>249</v>
       </c>
-      <c r="B3" s="57" t="s">
-        <v>47</v>
-      </c>
+      <c r="B3" s="57"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="B4" s="57" t="s">
-        <v>47</v>
-      </c>
+      <c r="B4" s="57"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="78" t="s">

</xml_diff>

<commit_message>
Initial menu items count.
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WS\CBISmokeTests\src\com\generic\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whamad\git\CBISmoke\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30B6F14-8362-46F1-B263-316A10E09BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0644D18B-820F-4D69-8283-3EE0C12A9B6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -1616,15 +1616,15 @@
 getRandomProduct</t>
   </si>
   <si>
-    <t xml:space="preserve">Logo validation  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Site logo validation: 
 - Navigate to Homepage
 - Get the header logo and make sure it is exist
 - do a search on test
 - Click logo
 - validate if you are on home page or not. </t>
+  </si>
+  <si>
+    <t>Logo validation, menu</t>
   </si>
 </sst>
 </file>
@@ -5919,7 +5919,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5951,10 +5951,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="87" t="s">
+        <v>487</v>
+      </c>
+      <c r="D2" s="91" t="s">
         <v>488</v>
-      </c>
-      <c r="D2" s="91" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">

</xml_diff>

<commit_message>
SMK-4: Navigation menu existance and open / close.
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WS\CBISmokeTests\src\com\generic\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whamad\git\CBISmoke\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30B6F14-8362-46F1-B263-316A10E09BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4B566E-668D-43E4-B9CA-82BCDEEEC450}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7965" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -1616,15 +1616,15 @@
 getRandomProduct</t>
   </si>
   <si>
-    <t xml:space="preserve">Logo validation  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Site logo validation: 
 - Navigate to Homepage
 - Get the header logo and make sure it is exist
 - do a search on test
 - Click logo
 - validate if you are on home page or not. </t>
+  </si>
+  <si>
+    <t>Logo validation  , menu</t>
   </si>
 </sst>
 </file>
@@ -5919,7 +5919,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5951,10 +5951,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="87" t="s">
+        <v>487</v>
+      </c>
+      <c r="D2" s="91" t="s">
         <v>488</v>
-      </c>
-      <c r="D2" s="91" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">

</xml_diff>

<commit_message>
Mini Cart Validation and PDP add to cart function
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WS\CBISmokeTests\src\com\generic\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imad-\git\CBISmoke\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30B6F14-8362-46F1-B263-316A10E09BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A045A0EE-A0BE-456D-AA0B-523F11764C3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="494">
   <si>
     <t>Browser</t>
   </si>
@@ -251,21 +251,7 @@
     <t>HPV-02</t>
   </si>
   <si>
-    <t>check footer guest</t>
-  </si>
-  <si>
-    <t>verify
-footer</t>
-  </si>
-  <si>
     <t>HPV-03</t>
-  </si>
-  <si>
-    <t>check body guest</t>
-  </si>
-  <si>
-    <t>verify
-body</t>
   </si>
   <si>
     <t>product</t>
@@ -1626,12 +1612,48 @@
 - Click logo
 - validate if you are on home page or not. </t>
   </si>
+  <si>
+    <t>shop menu validation</t>
+  </si>
+  <si>
+    <t>My account menu validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Account </t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>search validation</t>
+  </si>
+  <si>
+    <t>Mini cart validation</t>
+  </si>
+  <si>
+    <t>HPV-04</t>
+  </si>
+  <si>
+    <t>HPV-05</t>
+  </si>
+  <si>
+    <t>Mini cart validation:
+- Navigate to the Homepage
+- Click on Mini cart
+- Verify the text for empty cart is displayed.
+- Click close and verify that modal is closed. 
+- Add products to cart 
+- Click on Mini cart
+- Verify the products data is displayed.
+- Verify checkout button is displayed
+- Click close and verify that modal is closed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1668,6 +1690,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2495,124 +2523,124 @@
         <v>22</v>
       </c>
       <c r="E1" s="55" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G1" s="55" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="43" customFormat="1">
       <c r="A2" s="56" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="F2" s="59" t="s">
         <v>220</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="57" t="s">
+      <c r="G2" s="47" t="s">
         <v>221</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>222</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>223</v>
-      </c>
-      <c r="F2" s="59" t="s">
-        <v>224</v>
-      </c>
-      <c r="G2" s="47" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="56" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="57" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="G3" s="47" t="s">
         <v>221</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>222</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>227</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>224</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="56" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D4" s="58" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F4" s="59" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="105">
       <c r="A5" s="56" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E5" s="58" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F5" s="58"/>
       <c r="G5" s="49" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="56" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D6" s="58" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E6" s="58" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F6" s="58"/>
       <c r="G6" s="47" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2660,39 +2688,39 @@
         <v>21</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>29</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="60">
       <c r="A2" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="53" t="s">
         <v>244</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>246</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="F2" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="53" t="s">
-        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2739,141 +2767,141 @@
         <v>29</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="26" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>251</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="47" t="s">
-        <v>254</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>255</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="26" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="17" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="50" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="17" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="17" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2925,19 +2953,19 @@
     </row>
     <row r="2" spans="1:6" ht="30">
       <c r="A2" s="29" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F2" s="46"/>
     </row>
@@ -2987,230 +3015,230 @@
         <v>29</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1">
       <c r="A2" s="38" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="39" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
       <c r="A3" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="H3" s="42" t="s">
         <v>285</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>286</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>287</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="H3" s="42" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" s="38" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>287</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>288</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="H4" s="42" t="s">
         <v>290</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>291</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>292</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="G4" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="H4" s="42" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60">
       <c r="A5" s="38" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H5" s="42" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="38" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F6" s="38"/>
       <c r="G6" s="38" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H6" s="42" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7" s="38" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F7" s="38">
         <v>123</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H7" s="42" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="38" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G8" s="38"/>
       <c r="H8" s="42" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
       <c r="A9" s="38" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G9" s="38">
         <v>123</v>
       </c>
       <c r="H9" s="42" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30">
       <c r="A10" s="38" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F10" s="38">
         <v>123</v>
@@ -3219,31 +3247,31 @@
         <v>123</v>
       </c>
       <c r="H10" s="42" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30">
       <c r="A11" s="38" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="39" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="H11" s="42" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -3287,7 +3315,7 @@
         <v>23</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>24</v>
@@ -3307,19 +3335,19 @@
     </row>
     <row r="2" spans="1:9" s="24" customFormat="1">
       <c r="A2" s="26" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F2" s="30" t="s">
         <v>40</v>
@@ -3336,19 +3364,19 @@
     </row>
     <row r="3" spans="1:9" s="24" customFormat="1">
       <c r="A3" s="26" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>40</v>
@@ -3365,19 +3393,19 @@
     </row>
     <row r="4" spans="1:9" s="24" customFormat="1">
       <c r="A4" s="26" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>40</v>
@@ -3394,19 +3422,19 @@
     </row>
     <row r="5" spans="1:9" s="24" customFormat="1">
       <c r="A5" s="26" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>40</v>
@@ -3423,19 +3451,19 @@
     </row>
     <row r="6" spans="1:9" s="24" customFormat="1">
       <c r="A6" s="26" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>40</v>
@@ -3452,19 +3480,19 @@
     </row>
     <row r="7" spans="1:9" s="24" customFormat="1">
       <c r="A7" s="26" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>40</v>
@@ -3481,19 +3509,19 @@
     </row>
     <row r="8" spans="1:9" s="24" customFormat="1">
       <c r="A8" s="26" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F8" s="30" t="s">
         <v>40</v>
@@ -3510,19 +3538,19 @@
     </row>
     <row r="9" spans="1:9" s="24" customFormat="1">
       <c r="A9" s="26" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>40</v>
@@ -3539,19 +3567,19 @@
     </row>
     <row r="10" spans="1:9" s="24" customFormat="1">
       <c r="A10" s="26" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F10" s="30" t="s">
         <v>40</v>
@@ -3568,19 +3596,19 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="26" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>40</v>
@@ -3592,24 +3620,24 @@
         <v>36</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="26" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F12" s="30" t="s">
         <v>40</v>
@@ -3621,24 +3649,24 @@
         <v>36</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="26" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>40</v>
@@ -3650,24 +3678,24 @@
         <v>36</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="26" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F14" s="30" t="s">
         <v>40</v>
@@ -3679,24 +3707,24 @@
         <v>36</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="26" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F15" s="30" t="s">
         <v>40</v>
@@ -3708,24 +3736,24 @@
         <v>36</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="26" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>40</v>
@@ -3737,24 +3765,24 @@
         <v>36</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="26" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F17" s="30" t="s">
         <v>40</v>
@@ -3766,24 +3794,24 @@
         <v>36</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="26" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F18" s="30" t="s">
         <v>40</v>
@@ -3795,24 +3823,24 @@
         <v>36</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="26" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F19" s="30" t="s">
         <v>40</v>
@@ -3824,24 +3852,24 @@
         <v>36</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="26" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F20" s="30" t="s">
         <v>40</v>
@@ -3853,24 +3881,24 @@
         <v>36</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="26" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>40</v>
@@ -3882,24 +3910,24 @@
         <v>36</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="26" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F22" s="30" t="s">
         <v>40</v>
@@ -3911,24 +3939,24 @@
         <v>36</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="26" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F23" s="30" t="s">
         <v>40</v>
@@ -3940,24 +3968,24 @@
         <v>36</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="26" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F24" s="30" t="s">
         <v>40</v>
@@ -3969,24 +3997,24 @@
         <v>36</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="26" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>40</v>
@@ -3998,24 +4026,24 @@
         <v>36</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="26" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F26" s="30" t="s">
         <v>40</v>
@@ -4027,24 +4055,24 @@
         <v>36</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="26" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B27" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>40</v>
@@ -4056,24 +4084,24 @@
         <v>36</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="26" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F28" s="30" t="s">
         <v>40</v>
@@ -4085,24 +4113,24 @@
         <v>36</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="26" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F29" s="30" t="s">
         <v>40</v>
@@ -4114,24 +4142,24 @@
         <v>36</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="26" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F30" s="30" t="s">
         <v>40</v>
@@ -4143,24 +4171,24 @@
         <v>36</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="26" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F31" s="30" t="s">
         <v>40</v>
@@ -4172,24 +4200,24 @@
         <v>36</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="26" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F32" s="30" t="s">
         <v>40</v>
@@ -4201,24 +4229,24 @@
         <v>36</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="26" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F33" s="30" t="s">
         <v>40</v>
@@ -4230,7 +4258,7 @@
         <v>36</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -4462,25 +4490,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="F1" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>366</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>368</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>369</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4488,22 +4516,22 @@
         <v>64</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="G2" s="21" t="s">
         <v>371</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>372</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>373</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>374</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4511,22 +4539,22 @@
         <v>41</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C3" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="G3" s="21" t="s">
         <v>372</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>373</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>374</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4534,22 +4562,22 @@
         <v>46</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D4" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>374</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4557,22 +4585,22 @@
         <v>50</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E5" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>374</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4580,22 +4608,22 @@
         <v>54</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4603,22 +4631,22 @@
         <v>57</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4626,22 +4654,22 @@
         <v>59</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4649,22 +4677,22 @@
         <v>61</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4672,551 +4700,551 @@
         <v>37</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="13" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="13" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="13" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="13" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="13" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="13" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="13" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="13" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="13" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="13" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="13" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="13" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="13" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="13" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="13" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="13" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="13" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -5284,40 +5312,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="8" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>410</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>412</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>414</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="60">
@@ -5325,16 +5353,16 @@
         <v>33</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -5342,93 +5370,93 @@
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="16" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="180">
       <c r="A3" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>420</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>422</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>423</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>419</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>425</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>426</v>
-      </c>
       <c r="H3" s="14" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="14" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="60">
       <c r="A4" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="J4" s="17"/>
       <c r="K4" s="14" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="210">
       <c r="A5" s="10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -5436,10 +5464,10 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -5476,89 +5504,89 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30">
       <c r="A1" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>441</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="I2" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -5566,57 +5594,57 @@
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -5648,22 +5676,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -5671,19 +5699,19 @@
         <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>467</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5691,79 +5719,79 @@
         <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5771,19 +5799,19 @@
         <v>35</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -5916,10 +5944,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5947,14 +5975,12 @@
       <c r="A2" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="90" t="s">
-        <v>7</v>
-      </c>
+      <c r="B2" s="90"/>
       <c r="C2" s="87" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D2" s="91" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">
@@ -5963,25 +5989,52 @@
       </c>
       <c r="B3" s="90"/>
       <c r="C3" s="88" t="s">
-        <v>67</v>
+        <v>485</v>
       </c>
       <c r="D3" s="91" t="s">
-        <v>68</v>
+        <v>485</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30">
       <c r="A4" s="89" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" s="90"/>
       <c r="C4" s="88" t="s">
-        <v>70</v>
+        <v>487</v>
       </c>
       <c r="D4" s="91" t="s">
-        <v>71</v>
+        <v>486</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="89" t="s">
+        <v>491</v>
+      </c>
+      <c r="B5" s="90"/>
+      <c r="C5" s="88" t="s">
+        <v>488</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="150">
+      <c r="A6" s="89" t="s">
+        <v>492</v>
+      </c>
+      <c r="B6" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="87" t="s">
+        <v>493</v>
+      </c>
+      <c r="D6" s="91" t="s">
+        <v>490</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6792,25 +6845,25 @@
         <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G1" s="60" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30">
       <c r="A2" s="29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="73" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D2" s="74" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E2" s="75" t="s">
         <v>33</v>
@@ -6820,14 +6873,14 @@
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="A3" s="29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="73" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D3" s="74" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E3" s="75" t="s">
         <v>33</v>
@@ -6837,152 +6890,152 @@
     </row>
     <row r="4" spans="1:7" ht="30">
       <c r="A4" s="29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="73" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D4" s="74" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E4" s="75" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F4" s="76"/>
       <c r="G4" s="77"/>
     </row>
     <row r="5" spans="1:7" ht="30">
       <c r="A5" s="29" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="73" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="74" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="74" t="s">
-        <v>85</v>
-      </c>
       <c r="E5" s="75" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F5" s="76"/>
       <c r="G5" s="77"/>
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6" s="29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="73" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D6" s="74" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E6" s="75" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F6" s="76"/>
       <c r="G6" s="77"/>
     </row>
     <row r="7" spans="1:7" ht="30">
       <c r="A7" s="29" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="73" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D7" s="74" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E7" s="75" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F7" s="76"/>
       <c r="G7" s="77"/>
     </row>
     <row r="8" spans="1:7" ht="30">
       <c r="A8" s="29" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="73" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D8" s="74" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E8" s="75" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F8" s="76"/>
       <c r="G8" s="77"/>
     </row>
     <row r="9" spans="1:7" ht="30">
       <c r="A9" s="29" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B9" s="29"/>
       <c r="C9" s="73" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D9" s="74" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E9" s="75" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F9" s="76"/>
       <c r="G9" s="77"/>
     </row>
     <row r="10" spans="1:7" ht="30">
       <c r="A10" s="29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="73" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D10" s="74" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E10" s="75" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F10" s="76"/>
       <c r="G10" s="77"/>
     </row>
     <row r="11" spans="1:7" ht="165">
       <c r="A11" s="29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D11" s="74" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E11" s="75" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F11" s="76"/>
       <c r="G11" s="77"/>
     </row>
     <row r="12" spans="1:7" ht="30">
       <c r="A12" s="29" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B12" s="29"/>
       <c r="C12" s="73" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D12" s="74" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E12" s="75" t="s">
         <v>33</v>
@@ -6992,14 +7045,14 @@
     </row>
     <row r="13" spans="1:7" ht="30">
       <c r="A13" s="29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="73" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D13" s="74" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E13" s="75" t="s">
         <v>33</v>
@@ -7009,14 +7062,14 @@
     </row>
     <row r="14" spans="1:7" ht="30">
       <c r="A14" s="29" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B14" s="29"/>
       <c r="C14" s="73" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D14" s="74" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E14" s="75" t="s">
         <v>33</v>
@@ -7026,14 +7079,14 @@
     </row>
     <row r="15" spans="1:7" ht="30">
       <c r="A15" s="29" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B15" s="29"/>
       <c r="C15" s="73" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D15" s="74" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E15" s="75" t="s">
         <v>33</v>
@@ -7043,14 +7096,14 @@
     </row>
     <row r="16" spans="1:7" ht="120">
       <c r="A16" s="29" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="73" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D16" s="74" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E16" s="75" t="s">
         <v>33</v>
@@ -7060,14 +7113,14 @@
     </row>
     <row r="17" spans="1:7" ht="30">
       <c r="A17" s="29" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="73" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D17" s="74" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E17" s="75" t="s">
         <v>33</v>
@@ -7079,14 +7132,14 @@
     </row>
     <row r="18" spans="1:7" ht="30">
       <c r="A18" s="29" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B18" s="29"/>
       <c r="C18" s="73" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D18" s="74" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E18" s="75" t="s">
         <v>33</v>
@@ -7098,14 +7151,14 @@
     </row>
     <row r="19" spans="1:7" ht="30">
       <c r="A19" s="29" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B19" s="29"/>
       <c r="C19" s="73" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D19" s="74" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E19" s="75" t="s">
         <v>33</v>
@@ -7117,14 +7170,14 @@
     </row>
     <row r="20" spans="1:7" ht="30">
       <c r="A20" s="29" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="73" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D20" s="74" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E20" s="75" t="s">
         <v>33</v>
@@ -7136,14 +7189,14 @@
     </row>
     <row r="21" spans="1:7" ht="30">
       <c r="A21" s="29" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B21" s="29"/>
       <c r="C21" s="73" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D21" s="74" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E21" s="75" t="s">
         <v>33</v>
@@ -7155,14 +7208,14 @@
     </row>
     <row r="22" spans="1:7" ht="30">
       <c r="A22" s="29" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B22" s="29"/>
       <c r="C22" s="73" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D22" s="74" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E22" s="75" t="s">
         <v>33</v>
@@ -7174,14 +7227,14 @@
     </row>
     <row r="23" spans="1:7" ht="30">
       <c r="A23" s="29" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B23" s="29"/>
       <c r="C23" s="73" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D23" s="74" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E23" s="75" t="s">
         <v>33</v>
@@ -7193,14 +7246,14 @@
     </row>
     <row r="24" spans="1:7" ht="120">
       <c r="A24" s="29" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B24" s="29"/>
       <c r="C24" s="73" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D24" s="74" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E24" s="75" t="s">
         <v>33</v>
@@ -7262,480 +7315,480 @@
         <v>29</v>
       </c>
       <c r="G1" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="67" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="67" t="s">
         <v>140</v>
-      </c>
-      <c r="H1" s="67" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="67" t="s">
-        <v>142</v>
-      </c>
-      <c r="J1" s="67" t="s">
-        <v>143</v>
-      </c>
-      <c r="K1" s="67" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30">
       <c r="A2" s="68" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B2" s="56"/>
       <c r="C2" s="69" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D2" s="70" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F2" s="69"/>
       <c r="G2" s="56"/>
       <c r="H2" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I2" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J2" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K2" s="56"/>
     </row>
     <row r="3" spans="1:11" ht="30">
       <c r="A3" s="68" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="69" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D3" s="70" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F3" s="69"/>
       <c r="G3" s="56"/>
       <c r="H3" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I3" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J3" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="45">
       <c r="A4" s="68" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B4" s="56"/>
       <c r="C4" s="69" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D4" s="70" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E4" s="56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F4" s="69"/>
       <c r="G4" s="56"/>
       <c r="H4" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I4" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J4" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K4" s="56"/>
     </row>
     <row r="5" spans="1:11" ht="45">
       <c r="A5" s="68" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B5" s="56"/>
       <c r="C5" s="69" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D5" s="70" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F5" s="69"/>
       <c r="G5" s="56"/>
       <c r="H5" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I5" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J5" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K5" s="56"/>
     </row>
     <row r="6" spans="1:11" ht="30">
       <c r="A6" s="68" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B6" s="56"/>
       <c r="C6" s="26" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="56"/>
       <c r="H6" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I6" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J6" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:11" ht="60">
       <c r="A7" s="68" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="27" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E7" s="68" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F7" s="68"/>
       <c r="G7" s="27" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H7" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I7" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J7" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="45">
       <c r="A8" s="68" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B8" s="71"/>
       <c r="C8" s="68" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E8" s="68" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F8" s="68"/>
       <c r="G8" s="68" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H8" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I8" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J8" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K8" s="68" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30">
       <c r="A9" s="68" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B9" s="56"/>
       <c r="C9" s="69" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D9" s="70" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G9" s="56"/>
       <c r="H9" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I9" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J9" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K9" s="56"/>
     </row>
     <row r="10" spans="1:11" ht="30">
       <c r="A10" s="68" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B10" s="56"/>
       <c r="C10" s="69" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D10" s="70" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E10" s="68" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G10" s="56"/>
       <c r="H10" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I10" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J10" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K10" s="56"/>
     </row>
     <row r="11" spans="1:11" ht="45">
       <c r="A11" s="68" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B11" s="56"/>
       <c r="C11" s="69" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D11" s="70" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E11" s="68" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G11" s="56"/>
       <c r="H11" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I11" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J11" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K11" s="56"/>
     </row>
     <row r="12" spans="1:11" ht="45">
       <c r="A12" s="68" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B12" s="56"/>
       <c r="C12" s="69" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D12" s="70" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E12" s="68" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G12" s="56"/>
       <c r="H12" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I12" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J12" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K12" s="56"/>
     </row>
     <row r="13" spans="1:11" ht="30">
       <c r="A13" s="68" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B13" s="56"/>
       <c r="C13" s="26" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E13" s="68" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G13" s="56"/>
       <c r="H13" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I13" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J13" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K13" s="56"/>
     </row>
     <row r="14" spans="1:11" ht="60">
       <c r="A14" s="68" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B14" s="71"/>
       <c r="C14" s="27" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E14" s="68" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F14" s="68"/>
       <c r="G14" s="27" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H14" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I14" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J14" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="45">
       <c r="A15" s="68" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B15" s="71"/>
       <c r="C15" s="68" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E15" s="68" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F15" s="68"/>
       <c r="G15" s="68" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H15" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I15" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J15" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K15" s="68" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="90">
       <c r="A16" s="68" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B16" s="56" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="69" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D16" s="70" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E16" s="68" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F16" s="69"/>
       <c r="G16" s="56"/>
       <c r="H16" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I16" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J16" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K16" s="56"/>
     </row>
     <row r="17" spans="1:11" ht="90">
       <c r="A17" s="68" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B17" s="56"/>
       <c r="C17" s="69" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D17" s="70" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E17" s="68" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F17" s="69" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G17" s="56"/>
       <c r="H17" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I17" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J17" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K17" s="56"/>
     </row>
@@ -7787,70 +7840,70 @@
         <v>29</v>
       </c>
       <c r="G1" s="67" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30">
       <c r="A2" s="68" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B2" s="56" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="69" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D2" s="70" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F2" s="69"/>
       <c r="G2" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="A3" s="68" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B3" s="56" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="69" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D3" s="70" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F3" s="69"/>
       <c r="G3" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45">
       <c r="A4" s="68" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B4" s="56" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D4" s="70" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E4" s="56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F4" s="69"/>
       <c r="G4" s="56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -7891,10 +7944,10 @@
         <v>21</v>
       </c>
       <c r="D1" s="60" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>29</v>
@@ -7902,122 +7955,122 @@
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1">
       <c r="A2" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2" s="63" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>200</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="61" t="s">
-        <v>201</v>
-      </c>
-      <c r="D2" s="62" t="s">
-        <v>202</v>
-      </c>
-      <c r="E2" s="63" t="s">
-        <v>203</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="29" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="61" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D3" s="63" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E3" s="63" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="29" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D4" s="63" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E4" s="63" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" s="29" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E5" s="63" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="29" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E6" s="63" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30">
       <c r="A7" s="29" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E7" s="63" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SMK-16: Positive form filling.
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whamad\git\CBISmoke\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4B566E-668D-43E4-B9CA-82BCDEEEC450}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDE280D-A4DB-4B3C-98F1-28336F4506C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7965" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16284" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -1624,7 +1624,7 @@
 - validate if you are on home page or not. </t>
   </si>
   <si>
-    <t>Logo validation  , menu</t>
+    <t>Logo validation, menu, SignIn validation</t>
   </si>
 </sst>
 </file>
@@ -5474,7 +5474,7 @@
     <col min="9" max="9" width="12.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>440</v>
       </c>
@@ -5919,7 +5919,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
PDP validation Updates on HomePage validation
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imad-\git\CBISmoke\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14E9101-271E-4F30-8EEC-7FDBEED7AE4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B7C188-2EE9-4862-B9E7-64B80105E32B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -257,9 +257,6 @@
     <t>PDP-01</t>
   </si>
   <si>
-    <t>Guest, verify the PDP basics id</t>
-  </si>
-  <si>
     <t>P2</t>
   </si>
   <si>
@@ -1410,7 +1407,10 @@
 - Click close and verify that modal is closed</t>
   </si>
   <si>
-    <t>Verify PDP elements</t>
+    <t>Verify the PDP basics</t>
+  </si>
+  <si>
+    <t>Validate PDP active elements</t>
   </si>
 </sst>
 </file>
@@ -2278,124 +2278,124 @@
         <v>22</v>
       </c>
       <c r="E1" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="G1" s="55" t="s">
         <v>150</v>
-      </c>
-      <c r="G1" s="55" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="43" customFormat="1">
       <c r="A2" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="57" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="57" t="s">
+      <c r="D2" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="E2" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="F2" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="G2" s="47" t="s">
         <v>156</v>
-      </c>
-      <c r="G2" s="47" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="57" t="s">
-        <v>153</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>154</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>159</v>
-      </c>
       <c r="F3" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="G3" s="47" t="s">
         <v>156</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="57" t="s">
         <v>160</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="57" t="s">
+      <c r="D4" s="58" t="s">
         <v>161</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="E4" s="58" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" s="47" t="s">
         <v>162</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>156</v>
-      </c>
-      <c r="G4" s="47" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="105">
       <c r="A5" s="56" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="49" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="49" t="s">
+      <c r="D5" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="E5" s="58" t="s">
         <v>166</v>
-      </c>
-      <c r="E5" s="58" t="s">
-        <v>167</v>
       </c>
       <c r="F5" s="58"/>
       <c r="G5" s="49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="57" t="s">
         <v>169</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="57" t="s">
+      <c r="D6" s="58" t="s">
         <v>170</v>
       </c>
-      <c r="D6" s="58" t="s">
-        <v>171</v>
-      </c>
       <c r="E6" s="58" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F6" s="58"/>
       <c r="G6" s="47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2443,39 +2443,39 @@
         <v>21</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>29</v>
       </c>
       <c r="F1" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>174</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="60">
       <c r="A2" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="E2" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="53" t="s">
         <v>179</v>
-      </c>
-      <c r="F2" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="53" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2522,141 +2522,141 @@
         <v>29</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="47" t="s">
+      <c r="D2" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="E2" s="13" t="s">
         <v>183</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>184</v>
       </c>
       <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="47" t="s">
+      <c r="D3" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="E3" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="47" t="s">
         <v>190</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="47" t="s">
+      <c r="D4" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="E4" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="47" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="47" t="s">
+      <c r="D5" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="E5" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="49" t="s">
-        <v>199</v>
-      </c>
       <c r="D6" s="48" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E8" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2708,19 +2708,19 @@
     </row>
     <row r="2" spans="1:6" ht="30">
       <c r="A2" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="45" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="45" t="s">
+      <c r="D2" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="E2" s="46" t="s">
         <v>208</v>
-      </c>
-      <c r="E2" s="46" t="s">
-        <v>209</v>
       </c>
       <c r="F2" s="46"/>
     </row>
@@ -2770,230 +2770,230 @@
         <v>29</v>
       </c>
       <c r="F1" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="G1" s="36" t="s">
-        <v>211</v>
-      </c>
       <c r="H1" s="37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1">
       <c r="A2" s="38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" s="40" t="s">
         <v>213</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="E2" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="F2" s="38" t="s">
-        <v>216</v>
-      </c>
       <c r="G2" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
       <c r="A3" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="39" t="s">
+      <c r="D3" s="40" t="s">
         <v>218</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="E3" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="H3" s="42" t="s">
         <v>220</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="H3" s="42" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="39" t="s">
+      <c r="D4" s="40" t="s">
         <v>223</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="E4" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="H4" s="42" t="s">
         <v>225</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="G4" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="H4" s="42" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60">
       <c r="A5" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>227</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="39" t="s">
+      <c r="D5" s="40" t="s">
         <v>228</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="E5" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="H5" s="42" t="s">
         <v>229</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="G5" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="H5" s="42" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="39" t="s">
+      <c r="D6" s="40" t="s">
         <v>232</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>233</v>
-      </c>
       <c r="E6" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F6" s="38"/>
       <c r="G6" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H6" s="42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="39" t="s">
         <v>235</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="39" t="s">
+      <c r="D7" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="D7" s="40" t="s">
-        <v>237</v>
-      </c>
       <c r="E7" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F7" s="38">
         <v>123</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H7" s="42" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="39" t="s">
         <v>239</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>240</v>
-      </c>
       <c r="D8" s="40" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G8" s="38"/>
       <c r="H8" s="42" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
       <c r="A9" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="39" t="s">
         <v>242</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="39" t="s">
+      <c r="D9" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="D9" s="40" t="s">
-        <v>244</v>
-      </c>
       <c r="E9" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G9" s="38">
         <v>123</v>
       </c>
       <c r="H9" s="42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30">
       <c r="A10" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>247</v>
-      </c>
       <c r="D10" s="40" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F10" s="38">
         <v>123</v>
@@ -3002,31 +3002,31 @@
         <v>123</v>
       </c>
       <c r="H10" s="42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30">
       <c r="A11" s="38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="F11" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="D11" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="F11" s="38" t="s">
+      <c r="G11" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="H11" s="42" t="s">
         <v>251</v>
-      </c>
-      <c r="H11" s="42" t="s">
-        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -3070,7 +3070,7 @@
         <v>23</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>24</v>
@@ -3090,19 +3090,19 @@
     </row>
     <row r="2" spans="1:9" s="24" customFormat="1">
       <c r="A2" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="29" t="s">
+      <c r="E2" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F2" s="30" t="s">
         <v>40</v>
@@ -3119,19 +3119,19 @@
     </row>
     <row r="3" spans="1:9" s="24" customFormat="1">
       <c r="A3" s="26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>40</v>
@@ -3148,19 +3148,19 @@
     </row>
     <row r="4" spans="1:9" s="24" customFormat="1">
       <c r="A4" s="26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>40</v>
@@ -3177,19 +3177,19 @@
     </row>
     <row r="5" spans="1:9" s="24" customFormat="1">
       <c r="A5" s="26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>40</v>
@@ -3206,19 +3206,19 @@
     </row>
     <row r="6" spans="1:9" s="24" customFormat="1">
       <c r="A6" s="26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>40</v>
@@ -3235,19 +3235,19 @@
     </row>
     <row r="7" spans="1:9" s="24" customFormat="1">
       <c r="A7" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>40</v>
@@ -3264,19 +3264,19 @@
     </row>
     <row r="8" spans="1:9" s="24" customFormat="1">
       <c r="A8" s="26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E8" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F8" s="30" t="s">
         <v>40</v>
@@ -3293,19 +3293,19 @@
     </row>
     <row r="9" spans="1:9" s="24" customFormat="1">
       <c r="A9" s="26" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>40</v>
@@ -3322,19 +3322,19 @@
     </row>
     <row r="10" spans="1:9" s="24" customFormat="1">
       <c r="A10" s="26" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F10" s="30" t="s">
         <v>40</v>
@@ -3351,19 +3351,19 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E11" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>40</v>
@@ -3375,24 +3375,24 @@
         <v>36</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F12" s="30" t="s">
         <v>40</v>
@@ -3404,24 +3404,24 @@
         <v>36</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E13" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>40</v>
@@ -3433,24 +3433,24 @@
         <v>36</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F14" s="30" t="s">
         <v>40</v>
@@ -3462,24 +3462,24 @@
         <v>36</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E15" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F15" s="30" t="s">
         <v>40</v>
@@ -3491,24 +3491,24 @@
         <v>36</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E16" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>40</v>
@@ -3520,24 +3520,24 @@
         <v>36</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F17" s="30" t="s">
         <v>40</v>
@@ -3549,24 +3549,24 @@
         <v>36</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F18" s="30" t="s">
         <v>40</v>
@@ -3578,24 +3578,24 @@
         <v>36</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F19" s="30" t="s">
         <v>40</v>
@@ -3607,24 +3607,24 @@
         <v>36</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F20" s="30" t="s">
         <v>40</v>
@@ -3636,24 +3636,24 @@
         <v>36</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E21" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>40</v>
@@ -3665,24 +3665,24 @@
         <v>36</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D22" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E22" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F22" s="30" t="s">
         <v>40</v>
@@ -3694,24 +3694,24 @@
         <v>36</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E23" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F23" s="30" t="s">
         <v>40</v>
@@ -3723,24 +3723,24 @@
         <v>36</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E24" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F24" s="30" t="s">
         <v>40</v>
@@ -3752,24 +3752,24 @@
         <v>36</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E25" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>40</v>
@@ -3781,24 +3781,24 @@
         <v>36</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D26" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E26" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F26" s="30" t="s">
         <v>40</v>
@@ -3810,24 +3810,24 @@
         <v>36</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B27" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E27" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>40</v>
@@ -3839,24 +3839,24 @@
         <v>36</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D28" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E28" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F28" s="30" t="s">
         <v>40</v>
@@ -3868,24 +3868,24 @@
         <v>36</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="26" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E29" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F29" s="30" t="s">
         <v>40</v>
@@ -3897,24 +3897,24 @@
         <v>36</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E30" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F30" s="30" t="s">
         <v>40</v>
@@ -3926,24 +3926,24 @@
         <v>36</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E31" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F31" s="30" t="s">
         <v>40</v>
@@ -3955,24 +3955,24 @@
         <v>36</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E32" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F32" s="30" t="s">
         <v>40</v>
@@ -3984,24 +3984,24 @@
         <v>36</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D33" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E33" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="E33" s="29" t="s">
-        <v>256</v>
       </c>
       <c r="F33" s="30" t="s">
         <v>40</v>
@@ -4013,7 +4013,7 @@
         <v>36</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -4245,25 +4245,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>301</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4271,22 +4271,22 @@
         <v>64</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" s="21" t="s">
         <v>306</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4294,22 +4294,22 @@
         <v>41</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F3" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4317,22 +4317,22 @@
         <v>46</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="D4" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F4" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4340,22 +4340,22 @@
         <v>50</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F5" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4363,22 +4363,22 @@
         <v>54</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F6" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4386,22 +4386,22 @@
         <v>57</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="D7" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="E7" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F7" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4409,22 +4409,22 @@
         <v>59</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F8" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4432,22 +4432,22 @@
         <v>61</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="E9" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F9" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4455,551 +4455,551 @@
         <v>37</v>
       </c>
       <c r="B10" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="E10" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F10" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="D11" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="E11" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F11" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="D12" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="E12" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F12" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B13" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="D13" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="E13" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F13" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="D14" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="E14" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F14" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="D15" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="E15" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F15" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="D16" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="E16" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F16" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B17" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="D17" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="E17" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F17" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B18" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="D18" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="E18" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F18" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B19" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="D19" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="E19" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F19" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B20" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="D20" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="E20" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F20" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="D21" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="E21" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F21" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="D22" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="E22" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F22" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="D23" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F23" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="D24" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="E24" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F24" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B25" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="D25" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="E25" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F25" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B26" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="D26" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="E26" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F26" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B27" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="D27" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="E27" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F27" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B28" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C28" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="D28" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="E28" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F28" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B29" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="D29" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="E29" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E29" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F29" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B30" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="D30" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="E30" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E30" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F30" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B31" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="D31" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="E31" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E31" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F31" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B32" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="D32" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="E32" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E32" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F32" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B33" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="D33" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="E33" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>306</v>
-      </c>
       <c r="F33" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -5067,40 +5067,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>345</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>346</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="60">
@@ -5108,16 +5108,16 @@
         <v>33</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>350</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>351</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -5125,93 +5125,93 @@
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>352</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="180">
       <c r="A3" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>354</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="15" t="s">
         <v>355</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>356</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>358</v>
-      </c>
       <c r="H3" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="L3" s="10" t="s">
         <v>360</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="60">
       <c r="A4" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>362</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>364</v>
-      </c>
       <c r="E4" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J4" s="17"/>
       <c r="K4" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>366</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="210">
       <c r="A5" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>370</v>
-      </c>
       <c r="E5" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -5219,10 +5219,10 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -5259,89 +5259,89 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30">
       <c r="A1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>386</v>
-      </c>
       <c r="H3" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -5349,57 +5349,57 @@
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>306</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>390</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>393</v>
-      </c>
       <c r="H5" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -5431,22 +5431,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -5454,19 +5454,19 @@
         <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5474,79 +5474,79 @@
         <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>413</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5554,19 +5554,19 @@
         <v>35</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -5732,10 +5732,10 @@
       </c>
       <c r="B2" s="87"/>
       <c r="C2" s="84" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D2" s="88" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">
@@ -5744,10 +5744,10 @@
       </c>
       <c r="B3" s="87"/>
       <c r="C3" s="85" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D3" s="88" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30">
@@ -5756,36 +5756,36 @@
       </c>
       <c r="B4" s="87"/>
       <c r="C4" s="85" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D4" s="88" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="86" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B5" s="87"/>
       <c r="C5" s="85" t="s">
+        <v>422</v>
+      </c>
+      <c r="D5" s="88" t="s">
         <v>423</v>
-      </c>
-      <c r="D5" s="88" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="150">
       <c r="A6" s="86" t="s">
+        <v>426</v>
+      </c>
+      <c r="B6" s="87" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="84" t="s">
         <v>427</v>
       </c>
-      <c r="B6" s="87" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="84" t="s">
-        <v>428</v>
-      </c>
       <c r="D6" s="88" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -6572,7 +6572,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -6597,7 +6597,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" s="29" t="s">
         <v>68</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="73" t="s">
-        <v>69</v>
+        <v>428</v>
       </c>
       <c r="D2" s="74" t="s">
         <v>429</v>
@@ -6663,480 +6663,480 @@
         <v>29</v>
       </c>
       <c r="G1" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="I1" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="J1" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="K1" s="67" t="s">
         <v>75</v>
-      </c>
-      <c r="K1" s="67" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30">
       <c r="A2" s="68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="56"/>
       <c r="C2" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="E2" s="56" t="s">
         <v>79</v>
-      </c>
-      <c r="E2" s="56" t="s">
-        <v>80</v>
       </c>
       <c r="F2" s="69"/>
       <c r="G2" s="56"/>
       <c r="H2" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J2" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K2" s="56"/>
     </row>
     <row r="3" spans="1:11" ht="30">
       <c r="A3" s="68" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="70" t="s">
-        <v>85</v>
-      </c>
       <c r="E3" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="69"/>
       <c r="G3" s="56"/>
       <c r="H3" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J3" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="45">
       <c r="A4" s="68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="56"/>
       <c r="C4" s="69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" s="70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="69"/>
       <c r="G4" s="56"/>
       <c r="H4" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J4" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K4" s="56"/>
     </row>
     <row r="5" spans="1:11" ht="45">
       <c r="A5" s="68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="56"/>
       <c r="C5" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="70" t="s">
-        <v>90</v>
-      </c>
       <c r="E5" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" s="69"/>
       <c r="G5" s="56"/>
       <c r="H5" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J5" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K5" s="56"/>
     </row>
     <row r="6" spans="1:11" ht="30">
       <c r="A6" s="68" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="56"/>
       <c r="C6" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="E6" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="56"/>
       <c r="H6" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J6" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:11" ht="60">
       <c r="A7" s="68" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>96</v>
-      </c>
       <c r="E7" s="68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" s="68"/>
       <c r="G7" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="K7" s="27" t="s">
         <v>97</v>
-      </c>
-      <c r="H7" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="I7" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="J7" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="K7" s="27" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="45">
       <c r="A8" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="71"/>
       <c r="C8" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>101</v>
-      </c>
       <c r="E8" s="68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="68"/>
       <c r="G8" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="K8" s="68" t="s">
         <v>102</v>
-      </c>
-      <c r="H8" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="J8" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="K8" s="68" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30">
       <c r="A9" s="68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="56"/>
       <c r="C9" s="69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>105</v>
-      </c>
-      <c r="E9" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>106</v>
       </c>
       <c r="G9" s="56"/>
       <c r="H9" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J9" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K9" s="56"/>
     </row>
     <row r="10" spans="1:11" ht="30">
       <c r="A10" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="56"/>
       <c r="C10" s="69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>108</v>
-      </c>
-      <c r="E10" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>109</v>
       </c>
       <c r="G10" s="56"/>
       <c r="H10" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J10" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K10" s="56"/>
     </row>
     <row r="11" spans="1:11" ht="45">
       <c r="A11" s="68" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="56"/>
       <c r="C11" s="69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="70" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>111</v>
-      </c>
-      <c r="E11" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>112</v>
       </c>
       <c r="G11" s="56"/>
       <c r="H11" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J11" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K11" s="56"/>
     </row>
     <row r="12" spans="1:11" ht="45">
       <c r="A12" s="68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" s="56"/>
       <c r="C12" s="69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D12" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>114</v>
-      </c>
-      <c r="E12" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>115</v>
       </c>
       <c r="G12" s="56"/>
       <c r="H12" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J12" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K12" s="56"/>
     </row>
     <row r="13" spans="1:11" ht="30">
       <c r="A13" s="68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="56"/>
       <c r="C13" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="E13" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>118</v>
-      </c>
-      <c r="E13" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>119</v>
       </c>
       <c r="G13" s="56"/>
       <c r="H13" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I13" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J13" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K13" s="56"/>
     </row>
     <row r="14" spans="1:11" ht="60">
       <c r="A14" s="68" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" s="71"/>
       <c r="C14" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>96</v>
-      </c>
       <c r="E14" s="68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" s="68"/>
       <c r="G14" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" s="27" t="s">
         <v>97</v>
-      </c>
-      <c r="H14" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="I14" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="J14" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="K14" s="27" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="45">
       <c r="A15" s="68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" s="71"/>
       <c r="C15" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="27" t="s">
-        <v>101</v>
-      </c>
       <c r="E15" s="68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" s="68"/>
       <c r="G15" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" s="68" t="s">
         <v>102</v>
-      </c>
-      <c r="H15" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="J15" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="K15" s="68" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="90">
       <c r="A16" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="69" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="70" t="s">
-        <v>123</v>
-      </c>
       <c r="E16" s="68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16" s="69"/>
       <c r="G16" s="56"/>
       <c r="H16" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J16" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K16" s="56"/>
     </row>
     <row r="17" spans="1:11" ht="90">
       <c r="A17" s="68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B17" s="56"/>
       <c r="C17" s="69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="69" t="s">
         <v>125</v>
-      </c>
-      <c r="E17" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="69" t="s">
-        <v>126</v>
       </c>
       <c r="G17" s="56"/>
       <c r="H17" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I17" s="56" t="s">
-        <v>82</v>
-      </c>
       <c r="J17" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K17" s="56"/>
     </row>
@@ -7188,70 +7188,70 @@
         <v>29</v>
       </c>
       <c r="G1" s="67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30">
       <c r="A2" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="69" t="s">
-        <v>78</v>
-      </c>
       <c r="D2" s="70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="69"/>
       <c r="G2" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="A3" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="69" t="s">
-        <v>84</v>
-      </c>
       <c r="D3" s="70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="69"/>
       <c r="G3" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45">
       <c r="A4" s="68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="56" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" s="70" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E4" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="69"/>
       <c r="G4" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -7292,10 +7292,10 @@
         <v>21</v>
       </c>
       <c r="D1" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>130</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>131</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>29</v>
@@ -7303,122 +7303,122 @@
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1">
       <c r="A2" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="61" t="s">
+      <c r="D2" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="E2" s="63" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="F2" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="61" t="s">
+      <c r="D3" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="63" t="s">
-        <v>139</v>
-      </c>
       <c r="E3" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="61" t="s">
+      <c r="D4" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="63" t="s">
-        <v>142</v>
-      </c>
       <c r="E4" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" s="62" t="s">
-        <v>144</v>
-      </c>
       <c r="E5" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="61" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>146</v>
-      </c>
       <c r="E6" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30">
       <c r="A7" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="61" t="s">
-        <v>141</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>148</v>
-      </c>
       <c r="E7" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
My account menu existence and open / close* ( SMK-5)
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WS\CBISmokeTests\src\com\generic\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kawthar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30B6F14-8362-46F1-B263-316A10E09BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617E1CEA-9C4B-4BA1-91C2-23E3D0096DC4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="492">
   <si>
     <t>Browser</t>
   </si>
@@ -1625,6 +1625,26 @@
 - do a search on test
 - Click logo
 - validate if you are on home page or not. </t>
+  </si>
+  <si>
+    <t>My account menu existence and open / close*
+*_Desktop/ Tablet_*
+# Navigate to the Homepage
+# Click/Hover on my account menu.
+!My  account  acount  Menue.png|thumbnail!
+# Verify that all my account links are displayed. 
+# Click on any link and verify it is clickable.
+*_Mobile:_*
+# Navigate to the Homepage
+# Click on my account menu.
+# Verify that all my account links are displayed.
+# Close my account menu.</t>
+  </si>
+  <si>
+    <t>HPV-04</t>
+  </si>
+  <si>
+    <t>Account menu validation</t>
   </si>
 </sst>
 </file>
@@ -5916,10 +5936,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5979,6 +5999,20 @@
       </c>
       <c r="D4" s="91" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="195">
+      <c r="A5" s="89" t="s">
+        <v>490</v>
+      </c>
+      <c r="B5" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="87" t="s">
+        <v>489</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restore datasheet from base homepage
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kawthar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WS\CBISmokeTests\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617E1CEA-9C4B-4BA1-91C2-23E3D0096DC4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30B6F14-8362-46F1-B263-316A10E09BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="489">
   <si>
     <t>Browser</t>
   </si>
@@ -1625,26 +1625,6 @@
 - do a search on test
 - Click logo
 - validate if you are on home page or not. </t>
-  </si>
-  <si>
-    <t>My account menu existence and open / close*
-*_Desktop/ Tablet_*
-# Navigate to the Homepage
-# Click/Hover on my account menu.
-!My  account  acount  Menue.png|thumbnail!
-# Verify that all my account links are displayed. 
-# Click on any link and verify it is clickable.
-*_Mobile:_*
-# Navigate to the Homepage
-# Click on my account menu.
-# Verify that all my account links are displayed.
-# Close my account menu.</t>
-  </si>
-  <si>
-    <t>HPV-04</t>
-  </si>
-  <si>
-    <t>Account menu validation</t>
   </si>
 </sst>
 </file>
@@ -5936,10 +5916,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5999,20 +5979,6 @@
       </c>
       <c r="D4" s="91" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="195">
-      <c r="A5" s="89" t="s">
-        <v>490</v>
-      </c>
-      <c r="B5" s="90" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="87" t="s">
-        <v>489</v>
-      </c>
-      <c r="D5" s="91" t="s">
-        <v>491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Julia changes to datasheet
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WS\CBISmokeTests\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21431A6-78F7-4832-B703-8C0DD2B10E0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB1DE9F-D08B-4ADF-99E4-3031D4FFD08A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="426">
   <si>
     <t>Browser</t>
   </si>
@@ -1423,6 +1423,31 @@
   </si>
   <si>
     <t>menu</t>
+  </si>
+  <si>
+    <t>Global footer existence
+- Navigate to the Homepage
+-  Verify that "Connect" accordion is displayed and loaded correctly.
+- Verify that "SERVICE" accordion is displayed and loaded correctly.
+- Verify that "COMPANY" accordion is displayed and loaded correctly.
+- Verify that "RESOURCES" accordion is displayed and loaded correctly.
+- Verify that "CATALOG" accordion is displayed and loaded correctly.
+- Verify that "country selector" is displayed and loaded correctly.</t>
+  </si>
+  <si>
+    <t>Global footer validation</t>
+  </si>
+  <si>
+    <t>wish list guest</t>
+  </si>
+  <si>
+    <t>wish list guest validation</t>
+  </si>
+  <si>
+    <t>HPV-08</t>
+  </si>
+  <si>
+    <t>HPV-09</t>
   </si>
 </sst>
 </file>
@@ -2499,7 +2524,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -5707,10 +5732,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5824,6 +5849,34 @@
       </c>
       <c r="D8" s="88" t="s">
         <v>419</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="150">
+      <c r="A9" s="82" t="s">
+        <v>424</v>
+      </c>
+      <c r="B9" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="80" t="s">
+        <v>420</v>
+      </c>
+      <c r="D9" s="84" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30">
+      <c r="A10" s="82" t="s">
+        <v>425</v>
+      </c>
+      <c r="B10" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>422</v>
+      </c>
+      <c r="D10" s="84" t="s">
+        <v>423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>